<commit_message>
Bachelier option pricing formulas
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710CE1E5-D1B0-4548-8757-2528E4E10137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE3F9DD-7576-4D2D-B454-2ABAA56C8E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="135">
   <si>
     <t>x</t>
   </si>
@@ -556,6 +556,18 @@
   </si>
   <si>
     <t>Black-Scholes Option Greeks</t>
+  </si>
+  <si>
+    <t>Normal to LogNormal Volatility</t>
+  </si>
+  <si>
+    <t>Black Vol</t>
+  </si>
+  <si>
+    <t>Vol * Fwd</t>
+  </si>
+  <si>
+    <t>Black Price</t>
   </si>
 </sst>
 </file>
@@ -2353,37 +2365,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2392,6 +2374,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Bachelier!$Q$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vol * Fwd</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -2406,7 +2399,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Bachelier!$R$4:$R$14</c:f>
+              <c:f>Bachelier!$M$34:$M$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2448,42 +2441,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Bachelier!$X$4:$X$14</c:f>
+              <c:f>Bachelier!$Q$34:$Q$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.16337417753836542</c:v>
+                  <c:v>4.1925341293792382</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30263024449245113</c:v>
+                  <c:v>6.5160991000895505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49688621950264117</c:v>
+                  <c:v>8.3047670271975864</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7176912829080615</c:v>
+                  <c:v>9.7916114048857441</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90045118752382813</c:v>
+                  <c:v>11.077214089676684</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95835079448049465</c:v>
+                  <c:v>12.216431818444882</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.82036451881056327</c:v>
+                  <c:v>13.243191870494238</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47656379473671151</c:v>
+                  <c:v>14.180231197819593</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>15.043668504368728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.47656379473671151</c:v>
+                  <c:v>15.845418088831126</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.82036451881056327</c:v>
+                  <c:v>16.59457612628745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2491,7 +2484,124 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-26DF-4C0C-B93E-DD56E71C085B}"/>
+              <c16:uniqueId val="{00000000-B735-44C1-AE56-FCE92E6D296E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Bachelier!$O$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vol</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Bachelier!$M$34:$M$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Bachelier!$O$34:$O$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>14.999999999999959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.999999999999885</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.999999999981359</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.99999999780432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.999999999999131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.999999999983274</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.999999999983274</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.999999999999133</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B735-44C1-AE56-FCE92E6D296E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2503,11 +2613,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1734785392"/>
-        <c:axId val="1734776656"/>
+        <c:axId val="1968834384"/>
+        <c:axId val="1968840624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1734785392"/>
+        <c:axId val="1968834384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2564,12 +2674,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1734776656"/>
+        <c:crossAx val="1968840624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1734776656"/>
+        <c:axId val="1968840624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,7 +2736,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1734785392"/>
+        <c:crossAx val="1968834384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2638,6 +2748,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -9602,23 +9743,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>433387</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>623887</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948466DD-931D-4137-9E9C-EA52FE89627E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACB5B362-802C-4D9B-86A3-BD2CA7AA65EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10039,7 +10180,7 @@
   <dimension ref="B2:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10070,7 +10211,7 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8023.26859</v>
+        <v>1.3.8023.27332</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -10167,8 +10308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB465FF-8B5A-499F-AD9B-C82D6914A8E1}">
   <dimension ref="A1:AQ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12559,17 +12700,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1ECCF0-931A-41E3-AFEA-2FABAE8E4DC6}">
-  <dimension ref="A1:AQ43"/>
+  <dimension ref="A1:AQ44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
@@ -12709,8 +12850,8 @@
         <f t="shared" ref="I4:I20" si="0">G4-H4 +(F4-$C$4)*EXP(-$C$6*$C$8)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="11">
-        <v>1E-10</v>
+      <c r="L4" s="12">
+        <v>0</v>
       </c>
       <c r="M4">
         <f>_xll.acq_options_bachelier_price($C$4,$C$5,$C$6,$C$8,L4,TRUE)</f>
@@ -14667,7 +14808,15 @@
         <v>-1.7544178133706541</v>
       </c>
     </row>
-    <row r="32" spans="6:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="M32" s="44"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+      <c r="P32" s="44"/>
+      <c r="Q32" s="44"/>
       <c r="AB32" t="s">
         <v>111</v>
       </c>
@@ -14684,9 +14833,31 @@
         <v>8.5756290957306192E-11</v>
       </c>
     </row>
-    <row r="33" spans="18:43" x14ac:dyDescent="0.25">
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
+    <row r="33" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>96</v>
+      </c>
+      <c r="M33" t="s">
+        <v>109</v>
+      </c>
+      <c r="N33" t="s">
+        <v>99</v>
+      </c>
+      <c r="O33" t="s">
+        <v>96</v>
+      </c>
+      <c r="P33" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>133</v>
+      </c>
+      <c r="R33" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S33" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="T33" s="12"/>
       <c r="U33" s="11"/>
       <c r="W33" s="11"/>
@@ -14699,16 +14870,106 @@
       <c r="AD33" s="11"/>
       <c r="AE33" s="11"/>
     </row>
-    <row r="34" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L34" s="13">
+        <v>15</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+      <c r="N34">
+        <f>_xll.acq_options_bachelier_price(M34,$C$5,$C$6,$C$8,L34,$C$9)</f>
+        <v>2.0131592811431349E-3</v>
+      </c>
+      <c r="O34">
+        <f>_xll.acq_options_bachelier_vol(M34,$C$5,$C$6,$C$8,N34,$C$9)</f>
+        <v>14.999999999999959</v>
+      </c>
+      <c r="P34">
+        <f>_xll.acq_options_black_vol(M34,$C$5,$C$6,$C$8,N34,$C$9)</f>
+        <v>0.41925341293792379</v>
+      </c>
+      <c r="Q34">
+        <f>P34*M34</f>
+        <v>4.1925341293792382</v>
+      </c>
+      <c r="R34">
+        <f>_xll.acq_options_black_price(M34,$C$5,$C$6,$C$8,P34,$C$9)</f>
+        <v>2.0131592811394945E-3</v>
+      </c>
+      <c r="S34">
+        <f>R34-N34</f>
+        <v>-3.6403172143373297E-15</v>
+      </c>
       <c r="T34" s="12"/>
     </row>
-    <row r="35" spans="18:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L35" s="13">
+        <v>15</v>
+      </c>
+      <c r="M35">
+        <v>20</v>
+      </c>
+      <c r="N35">
+        <f>_xll.acq_options_bachelier_price(M35,$C$5,$C$6,$C$8,L35,$C$9)</f>
+        <v>9.4848058973276278E-3</v>
+      </c>
+      <c r="O35">
+        <f>_xll.acq_options_bachelier_vol(M35,$C$5,$C$6,$C$8,N35,$C$9)</f>
+        <v>14.999999999999984</v>
+      </c>
+      <c r="P35">
+        <f>_xll.acq_options_black_vol(M35,$C$5,$C$6,$C$8,N35,$C$9)</f>
+        <v>0.32580495500447754</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" ref="Q35:Q44" si="1">P35*M35</f>
+        <v>6.5160991000895505</v>
+      </c>
+      <c r="R35">
+        <f>_xll.acq_options_black_price(M35,$C$5,$C$6,$C$8,P35,$C$9)</f>
+        <v>9.4848058971470205E-3</v>
+      </c>
+      <c r="S35">
+        <f t="shared" ref="S35:S44" si="2">R35-N35</f>
+        <v>-1.8060726525437332E-13</v>
+      </c>
       <c r="T35" s="12"/>
       <c r="AB35" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L36" s="13">
+        <v>15</v>
+      </c>
+      <c r="M36">
+        <v>30</v>
+      </c>
+      <c r="N36">
+        <f>_xll.acq_options_bachelier_price(M36,$C$5,$C$6,$C$8,L36,$C$9)</f>
+        <v>3.8230266986719816E-2</v>
+      </c>
+      <c r="O36">
+        <f>_xll.acq_options_bachelier_vol(M36,$C$5,$C$6,$C$8,N36,$C$9)</f>
+        <v>14.999999999999885</v>
+      </c>
+      <c r="P36">
+        <f>_xll.acq_options_black_vol(M36,$C$5,$C$6,$C$8,N36,$C$9)</f>
+        <v>0.27682556757325288</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="1"/>
+        <v>8.3047670271975864</v>
+      </c>
+      <c r="R36">
+        <f>_xll.acq_options_black_price(M36,$C$5,$C$6,$C$8,P36,$C$9)</f>
+        <v>3.8230266986681312E-2</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="2"/>
+        <v>-3.850392227278121E-14</v>
+      </c>
       <c r="T36" s="12"/>
       <c r="AG36" t="s">
         <v>100</v>
@@ -14720,7 +14981,37 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L37" s="13">
+        <v>15</v>
+      </c>
+      <c r="M37">
+        <v>40</v>
+      </c>
+      <c r="N37">
+        <f>_xll.acq_options_bachelier_price(M37,$C$5,$C$6,$C$8,L37,$C$9)</f>
+        <v>0.13235361008593996</v>
+      </c>
+      <c r="O37">
+        <f>_xll.acq_options_bachelier_vol(M37,$C$5,$C$6,$C$8,N37,$C$9)</f>
+        <v>14.999999999999996</v>
+      </c>
+      <c r="P37">
+        <f>_xll.acq_options_black_vol(M37,$C$5,$C$6,$C$8,N37,$C$9)</f>
+        <v>0.2447902851221436</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="1"/>
+        <v>9.7916114048857441</v>
+      </c>
+      <c r="R37">
+        <f>_xll.acq_options_black_price(M37,$C$5,$C$6,$C$8,P37,$C$9)</f>
+        <v>0.13235361008600149</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="2"/>
+        <v>6.1534111139849301E-14</v>
+      </c>
       <c r="T37" s="12"/>
       <c r="AB37" s="29" t="s">
         <v>120</v>
@@ -14738,7 +15029,37 @@
         <v>20.0001</v>
       </c>
     </row>
-    <row r="38" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L38" s="13">
+        <v>15</v>
+      </c>
+      <c r="M38">
+        <v>50</v>
+      </c>
+      <c r="N38">
+        <f>_xll.acq_options_bachelier_price(M38,$C$5,$C$6,$C$8,L38,$C$9)</f>
+        <v>0.39549502137976517</v>
+      </c>
+      <c r="O38">
+        <f>_xll.acq_options_bachelier_vol(M38,$C$5,$C$6,$C$8,N38,$C$9)</f>
+        <v>14.999999999981359</v>
+      </c>
+      <c r="P38">
+        <f>_xll.acq_options_black_vol(M38,$C$5,$C$6,$C$8,N38,$C$9)</f>
+        <v>0.22154428179353367</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="1"/>
+        <v>11.077214089676684</v>
+      </c>
+      <c r="R38">
+        <f>_xll.acq_options_black_price(M38,$C$5,$C$6,$C$8,P38,$C$9)</f>
+        <v>0.39549502116753965</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="2"/>
+        <v>-2.1222551493949027E-10</v>
+      </c>
       <c r="T38" s="12"/>
       <c r="AB38" s="26">
         <f>AB39-AC42</f>
@@ -14793,7 +15114,37 @@
         <v>5.295150627150619E-3</v>
       </c>
     </row>
-    <row r="39" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L39" s="13">
+        <v>15</v>
+      </c>
+      <c r="M39">
+        <v>60</v>
+      </c>
+      <c r="N39">
+        <f>_xll.acq_options_bachelier_price(M39,$C$5,$C$6,$C$8,L39,$C$9)</f>
+        <v>1.0262457624668468</v>
+      </c>
+      <c r="O39">
+        <f>_xll.acq_options_bachelier_vol(M39,$C$5,$C$6,$C$8,N39,$C$9)</f>
+        <v>14.99999999780432</v>
+      </c>
+      <c r="P39">
+        <f>_xll.acq_options_black_vol(M39,$C$5,$C$6,$C$8,N39,$C$9)</f>
+        <v>0.20360719697408136</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="1"/>
+        <v>12.216431818444882</v>
+      </c>
+      <c r="R39">
+        <f>_xll.acq_options_black_price(M39,$C$5,$C$6,$C$8,P39,$C$9)</f>
+        <v>1.0262457624660521</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="2"/>
+        <v>-7.9469764102668705E-13</v>
+      </c>
       <c r="T39" s="12"/>
       <c r="AB39" s="27">
         <f>C4</f>
@@ -14848,7 +15199,37 @@
         <v>5.2951029712477032E-3</v>
       </c>
     </row>
-    <row r="40" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L40" s="13">
+        <v>15</v>
+      </c>
+      <c r="M40">
+        <v>70</v>
+      </c>
+      <c r="N40">
+        <f>_xll.acq_options_bachelier_price(M40,$C$5,$C$6,$C$8,L40,$C$9)</f>
+        <v>2.3296938786038028</v>
+      </c>
+      <c r="O40">
+        <f>_xll.acq_options_bachelier_vol(M40,$C$5,$C$6,$C$8,N40,$C$9)</f>
+        <v>14.999999999999131</v>
+      </c>
+      <c r="P40">
+        <f>_xll.acq_options_black_vol(M40,$C$5,$C$6,$C$8,N40,$C$9)</f>
+        <v>0.18918845529277484</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="1"/>
+        <v>13.243191870494238</v>
+      </c>
+      <c r="R40">
+        <f>_xll.acq_options_black_price(M40,$C$5,$C$6,$C$8,P40,$C$9)</f>
+        <v>2.3296938786038002</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="T40" s="12"/>
       <c r="AB40" s="28">
         <f>AB39+AC42</f>
@@ -14903,10 +15284,70 @@
         <v>5.2950553151912315E-3</v>
       </c>
     </row>
-    <row r="41" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L41" s="13">
+        <v>15</v>
+      </c>
+      <c r="M41">
+        <v>80</v>
+      </c>
+      <c r="N41">
+        <f>_xll.acq_options_bachelier_price(M41,$C$5,$C$6,$C$8,L41,$C$9)</f>
+        <v>4.6688933344611057</v>
+      </c>
+      <c r="O41">
+        <f>_xll.acq_options_bachelier_vol(M41,$C$5,$C$6,$C$8,N41,$C$9)</f>
+        <v>14.999999999983274</v>
+      </c>
+      <c r="P41">
+        <f>_xll.acq_options_black_vol(M41,$C$5,$C$6,$C$8,N41,$C$9)</f>
+        <v>0.17725288997274491</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="1"/>
+        <v>14.180231197819593</v>
+      </c>
+      <c r="R41">
+        <f>_xll.acq_options_black_price(M41,$C$5,$C$6,$C$8,P41,$C$9)</f>
+        <v>4.6688933344573389</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="2"/>
+        <v>-3.7667646779482311E-12</v>
+      </c>
       <c r="T41" s="12"/>
     </row>
-    <row r="42" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L42" s="13">
+        <v>15</v>
+      </c>
+      <c r="M42">
+        <v>90</v>
+      </c>
+      <c r="N42">
+        <f>_xll.acq_options_bachelier_price(M42,$C$5,$C$6,$C$8,L42,$C$9)</f>
+        <v>8.3499623830996867</v>
+      </c>
+      <c r="O42">
+        <f>_xll.acq_options_bachelier_vol(M42,$C$5,$C$6,$C$8,N42,$C$9)</f>
+        <v>14.999999999999998</v>
+      </c>
+      <c r="P42">
+        <f>_xll.acq_options_black_vol(M42,$C$5,$C$6,$C$8,N42,$C$9)</f>
+        <v>0.16715187227076364</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="1"/>
+        <v>15.043668504368728</v>
+      </c>
+      <c r="R42">
+        <f>_xll.acq_options_black_price(M42,$C$5,$C$6,$C$8,P42,$C$9)</f>
+        <v>8.349962383108144</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="2"/>
+        <v>8.4572349123845925E-12</v>
+      </c>
       <c r="T42" s="12"/>
       <c r="AB42" t="s">
         <v>110</v>
@@ -14923,7 +15364,37 @@
         <v>5.2951532740116106E-3</v>
       </c>
     </row>
-    <row r="43" spans="18:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L43" s="13">
+        <v>15</v>
+      </c>
+      <c r="M43">
+        <v>100</v>
+      </c>
+      <c r="N43">
+        <f>_xll.acq_options_bachelier_price(M43,$C$5,$C$6,$C$8,L43,$C$9)</f>
+        <v>13.493862360307061</v>
+      </c>
+      <c r="O43">
+        <f>_xll.acq_options_bachelier_vol(M43,$C$5,$C$6,$C$8,N43,$C$9)</f>
+        <v>14.999999999983274</v>
+      </c>
+      <c r="P43">
+        <f>_xll.acq_options_black_vol(M43,$C$5,$C$6,$C$8,N43,$C$9)</f>
+        <v>0.15845418088831126</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="1"/>
+        <v>15.845418088831126</v>
+      </c>
+      <c r="R43">
+        <f>_xll.acq_options_black_price(M43,$C$5,$C$6,$C$8,P43,$C$9)</f>
+        <v>13.49386236030082</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="2"/>
+        <v>-6.2403415768130799E-12</v>
+      </c>
       <c r="AB43" t="s">
         <v>111</v>
       </c>
@@ -14937,13 +15408,46 @@
       </c>
       <c r="AF43" s="11"/>
     </row>
+    <row r="44" spans="12:43" x14ac:dyDescent="0.25">
+      <c r="L44" s="13">
+        <v>15</v>
+      </c>
+      <c r="M44">
+        <v>110</v>
+      </c>
+      <c r="N44">
+        <f>_xll.acq_options_bachelier_price(M44,$C$5,$C$6,$C$8,L44,$C$9)</f>
+        <v>19.979631930295714</v>
+      </c>
+      <c r="O44">
+        <f>_xll.acq_options_bachelier_vol(M44,$C$5,$C$6,$C$8,N44,$C$9)</f>
+        <v>14.999999999999133</v>
+      </c>
+      <c r="P44">
+        <f>_xll.acq_options_black_vol(M44,$C$5,$C$6,$C$8,N44,$C$9)</f>
+        <v>0.15085978296624955</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="1"/>
+        <v>16.59457612628745</v>
+      </c>
+      <c r="R44">
+        <f>_xll.acq_options_black_price(M44,$C$5,$C$6,$C$8,P44,$C$9)</f>
+        <v>19.979631930295717</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="L32:Q32"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="L2:P2"/>
     <mergeCell ref="S2:Z2"/>
     <mergeCell ref="S17:Z17"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added Bjerksund-Stensland Analytical Approximation for American options
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -2,23 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE3F9DD-7576-4D2D-B454-2ABAA56C8E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276C920C-9404-46B8-8BC2-3A9B48BD19E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
     <sheet name="Black" sheetId="13" r:id="rId2"/>
     <sheet name="Bachelier" sheetId="15" r:id="rId3"/>
     <sheet name="BlackScholes" sheetId="14" r:id="rId4"/>
-    <sheet name="Description" sheetId="7" r:id="rId5"/>
-    <sheet name="Special" sheetId="9" r:id="rId6"/>
+    <sheet name="BjerksundStensland2002" sheetId="16" r:id="rId5"/>
+    <sheet name="Description" sheetId="7" r:id="rId6"/>
+    <sheet name="Special" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -162,8 +163,33 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>chirokov</author>
+  </authors>
+  <commentList>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{318E53DF-D189-4CA7-9B6F-B52507DAE4F6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Numerical Methods versus Bjerksund and Stensland
+Approximations for American Options Pricing
+Marasovic Branka, Aljinovic Zdravka, Poklepovic Tea</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="145">
   <si>
     <t>x</t>
   </si>
@@ -569,6 +595,36 @@
   <si>
     <t>Black Price</t>
   </si>
+  <si>
+    <t>Bjerksund Stensland (2002) Option Greeks</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Black-Scholes</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Bjerksund Stensland (2002)</t>
+  </si>
+  <si>
+    <t>Call Option</t>
+  </si>
+  <si>
+    <t>Put Option</t>
+  </si>
+  <si>
+    <t>https://downloads.dxfeed.com/specifications/dxLibOptions/Numerical-Methods-versus-Bjerksund-and-Stensland-Approximations-for-American-Options-Pricing-.pdf</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Spot Price</t>
+  </si>
 </sst>
 </file>
 
@@ -579,7 +635,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,8 +709,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,6 +756,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -906,7 +976,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -916,8 +986,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -964,20 +1035,25 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
     <cellStyle name="40% - Accent4" xfId="5" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="6" builtinId="47"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Heading 1" xfId="8" builtinId="16"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
@@ -10177,6 +10253,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10211,7 +10288,7 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8023.27332</v>
+        <v>1.3.8023.35113</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -10306,6 +10383,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB465FF-8B5A-499F-AD9B-C82D6914A8E1}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AQ43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10324,37 +10402,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="L2" s="44" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="L2" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="S2" s="44" t="s">
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="S2" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -11529,16 +11607,16 @@
         <f>_xll.acq_options_black_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>0.65000000000000013</v>
       </c>
-      <c r="S17" s="44" t="s">
+      <c r="S17" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="44"/>
-      <c r="U17" s="44"/>
-      <c r="V17" s="44"/>
-      <c r="W17" s="44"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="44"/>
-      <c r="Z17" s="44"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>0.2</v>
@@ -12700,9 +12778,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1ECCF0-931A-41E3-AFEA-2FABAE8E4DC6}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AQ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
@@ -12718,37 +12797,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="L2" s="44" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="L2" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="S2" s="44" t="s">
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="S2" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -13923,16 +14002,16 @@
         <f>_xll.acq_options_bachelier_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>25.999999999962554</v>
       </c>
-      <c r="S17" s="44" t="s">
+      <c r="S17" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="44"/>
-      <c r="U17" s="44"/>
-      <c r="V17" s="44"/>
-      <c r="W17" s="44"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="44"/>
-      <c r="Z17" s="44"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>20</v>
@@ -14809,14 +14888,14 @@
       </c>
     </row>
     <row r="32" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="44" t="s">
+      <c r="L32" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
       <c r="AB32" t="s">
         <v>111</v>
       </c>
@@ -15457,10 +15536,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC30C1E-5BFB-47EF-8AD5-509FD4075E48}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AS56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15475,37 +15555,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="L2" s="44" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="L2" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="S2" s="44" t="s">
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="S2" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
       <c r="AA2" s="38"/>
       <c r="AB2" s="38"/>
       <c r="AD2" s="3" t="s">
@@ -16782,16 +16862,16 @@
         <f>_xll.acq_options_blackscholes_vol($C$4,$C$5,$C$6,$C$8,$C$9,$N17,FALSE)</f>
         <v>0.65</v>
       </c>
-      <c r="S17" s="44" t="s">
+      <c r="S17" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="44"/>
-      <c r="U17" s="44"/>
-      <c r="V17" s="44"/>
-      <c r="W17" s="44"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="44"/>
-      <c r="Z17" s="44"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
       <c r="AA17" s="38"/>
       <c r="AB17" s="38"/>
       <c r="AD17" s="16">
@@ -18396,7 +18476,1977 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937DB880-8B2C-4D2D-B567-C1990F7A61F3}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:AE45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>140</v>
+      </c>
+      <c r="U2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="F3" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="J3" s="45"/>
+      <c r="M3" t="s">
+        <v>144</v>
+      </c>
+      <c r="V3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="5">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" t="s">
+        <v>138</v>
+      </c>
+      <c r="L4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M4" s="44">
+        <v>120</v>
+      </c>
+      <c r="N4" s="44">
+        <v>130</v>
+      </c>
+      <c r="O4" s="44">
+        <v>140</v>
+      </c>
+      <c r="P4" s="44">
+        <v>150</v>
+      </c>
+      <c r="Q4" s="44">
+        <v>160</v>
+      </c>
+      <c r="R4" s="44">
+        <v>170</v>
+      </c>
+      <c r="S4" s="44">
+        <v>180</v>
+      </c>
+      <c r="U4" t="s">
+        <v>136</v>
+      </c>
+      <c r="V4" s="44">
+        <v>120</v>
+      </c>
+      <c r="W4" s="44">
+        <v>130</v>
+      </c>
+      <c r="X4" s="44">
+        <v>140</v>
+      </c>
+      <c r="Y4" s="44">
+        <v>150</v>
+      </c>
+      <c r="Z4" s="44">
+        <v>160</v>
+      </c>
+      <c r="AA4" s="44">
+        <v>170</v>
+      </c>
+      <c r="AB4" s="44">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="5">
+        <v>150</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>60.249558470704109</v>
+      </c>
+      <c r="H5">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.45451366506677E-8</v>
+      </c>
+      <c r="I5">
+        <f>_xll.acq_options_blackscholes_price($C$4,F5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>60.249558470704109</v>
+      </c>
+      <c r="J5">
+        <f>_xll.acq_options_blackscholes_price($C$4,G5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.2409702289365026</v>
+      </c>
+      <c r="L5" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="M5">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.5406465471966558E-5</v>
+      </c>
+      <c r="N5">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.2933090223175903E-2</v>
+      </c>
+      <c r="O5">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.42214400501387139</v>
+      </c>
+      <c r="P5">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.334777836621214</v>
+      </c>
+      <c r="Q5">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>10.501286446631354</v>
+      </c>
+      <c r="R5">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>19.978981172055768</v>
+      </c>
+      <c r="S5">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>29.911482759239618</v>
+      </c>
+      <c r="U5" s="48">
+        <v>0.05</v>
+      </c>
+      <c r="V5">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W5">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="X5">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>10.18504362777812</v>
+      </c>
+      <c r="Y5">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.1384221077732235</v>
+      </c>
+      <c r="Z5">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.47775635971180463</v>
+      </c>
+      <c r="AA5">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.3349932689986872E-2</v>
+      </c>
+      <c r="AB5">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.1017056366426914E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F6,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>51.643238988719183</v>
+      </c>
+      <c r="H6">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F6,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.7144366461252503E-4</v>
+      </c>
+      <c r="I6">
+        <f>_xll.acq_options_blackscholes_price($C$4,F6,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>51.643238988719183</v>
+      </c>
+      <c r="J6">
+        <f>_xll.acq_options_blackscholes_price($C$4,G6,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.4604738210067554</v>
+      </c>
+      <c r="L6" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="M6">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>7.4321492242979126E-3</v>
+      </c>
+      <c r="N6">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.15262645017283294</v>
+      </c>
+      <c r="O6">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.2014947001305352</v>
+      </c>
+      <c r="P6">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.7013488821066858</v>
+      </c>
+      <c r="Q6">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>11.361232793456026</v>
+      </c>
+      <c r="R6">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>20.183594612760373</v>
+      </c>
+      <c r="S6">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>29.866937861547115</v>
+      </c>
+      <c r="U6" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="V6">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W6">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="X6">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>10.70274525100454</v>
+      </c>
+      <c r="Y6">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.323515151201903</v>
+      </c>
+      <c r="Z6">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.2488238283683302</v>
+      </c>
+      <c r="AA6">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.25445924170767853</v>
+      </c>
+      <c r="AB6">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.7185007899296352E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F7,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>43.070218293843979</v>
+      </c>
+      <c r="H7">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F7,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.1270787915449887E-2</v>
+      </c>
+      <c r="I7">
+        <f>_xll.acq_options_blackscholes_price($C$4,F7,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>43.070218293843979</v>
+      </c>
+      <c r="J7">
+        <f>_xll.acq_options_blackscholes_price($C$4,G7,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.49501536694438641</v>
+      </c>
+      <c r="L7" s="48">
+        <v>0.15</v>
+      </c>
+      <c r="M7">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.6461255493347009E-2</v>
+      </c>
+      <c r="N7">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.41252916144221174</v>
+      </c>
+      <c r="O7">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.9436117065435283</v>
+      </c>
+      <c r="P7">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.7399577137358477</v>
+      </c>
+      <c r="Q7">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>12.155858521118432</v>
+      </c>
+      <c r="R7">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>20.52879418638193</v>
+      </c>
+      <c r="S7">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>29.91318851001617</v>
+      </c>
+      <c r="U7" s="48">
+        <v>0.15</v>
+      </c>
+      <c r="V7">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W7">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.001920467055228</v>
+      </c>
+      <c r="X7">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>11.215430755407048</v>
+      </c>
+      <c r="Y7">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.190490800613432</v>
+      </c>
+      <c r="Z7">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.9396936783394665</v>
+      </c>
+      <c r="AA7">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.58423039563368206</v>
+      </c>
+      <c r="AB7">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.14353303380678994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F8,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>34.732350696547442</v>
+      </c>
+      <c r="H8">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F8,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.12687762656902635</v>
+      </c>
+      <c r="I8">
+        <f>_xll.acq_options_blackscholes_price($C$4,F8,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>34.732350696547442</v>
+      </c>
+      <c r="J8">
+        <f>_xll.acq_options_blackscholes_price($C$4,G8,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.11085764156847244</v>
+      </c>
+      <c r="L8" s="48">
+        <v>0.2</v>
+      </c>
+      <c r="M8">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.12708917162981281</v>
+      </c>
+      <c r="N8">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.73204173962328056</v>
+      </c>
+      <c r="O8">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.6237251947986522</v>
+      </c>
+      <c r="P8">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.6072182042030931</v>
+      </c>
+      <c r="Q8">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>12.873137023332717</v>
+      </c>
+      <c r="R8">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>20.924799488846745</v>
+      </c>
+      <c r="S8">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>30.033950291703007</v>
+      </c>
+      <c r="U8" s="48">
+        <v>0.2</v>
+      </c>
+      <c r="V8">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W8">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.059879979875106</v>
+      </c>
+      <c r="X8">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>11.685170289085562</v>
+      </c>
+      <c r="Y8">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.8941074536139695</v>
+      </c>
+      <c r="Z8">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.5490123498013304</v>
+      </c>
+      <c r="AA8">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.94675254931996733</v>
+      </c>
+      <c r="AB8">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.30487700103364546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0.06</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F9,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>27.039778414947577</v>
+      </c>
+      <c r="H9">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F9,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.61844884365571318</v>
+      </c>
+      <c r="I9">
+        <f>_xll.acq_options_blackscholes_price($C$4,F9,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>27.039778414947577</v>
+      </c>
+      <c r="J9">
+        <f>_xll.acq_options_blackscholes_price($C$4,G9,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.426895703799709E-2</v>
+      </c>
+      <c r="L9" s="48">
+        <v>0.25</v>
+      </c>
+      <c r="M9">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.24444161162469946</v>
+      </c>
+      <c r="N9">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.0777160954364895</v>
+      </c>
+      <c r="O9">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.248672450495846</v>
+      </c>
+      <c r="P9">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>7.364007980336666</v>
+      </c>
+      <c r="Q9">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>13.525614789490845</v>
+      </c>
+      <c r="R9">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>21.334437719804967</v>
+      </c>
+      <c r="S9">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>30.203730848908037</v>
+      </c>
+      <c r="U9" s="48">
+        <v>0.25</v>
+      </c>
+      <c r="V9">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W9">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.161734159445849</v>
+      </c>
+      <c r="X9">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>12.113197097513428</v>
+      </c>
+      <c r="Y9">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.4941271274534387</v>
+      </c>
+      <c r="Z9">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.0929303826990946</v>
+      </c>
+      <c r="AA9">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.3124840209453339</v>
+      </c>
+      <c r="AB9">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.50014792053050883</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F10,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>20.390726908197692</v>
+      </c>
+      <c r="H10">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F10,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.8903923326725192</v>
+      </c>
+      <c r="I10">
+        <f>_xll.acq_options_blackscholes_price($C$4,F10,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>20.390726908197692</v>
+      </c>
+      <c r="J10">
+        <f>_xll.acq_options_blackscholes_price($C$4,G10,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.3215811534007841E-4</v>
+      </c>
+      <c r="L10" s="48">
+        <v>0.3</v>
+      </c>
+      <c r="M10">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.39027254010901835</v>
+      </c>
+      <c r="N10">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.4328005583922518</v>
+      </c>
+      <c r="O10">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.8271849497956225</v>
+      </c>
+      <c r="P10">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>8.0416556749709116</v>
+      </c>
+      <c r="Q10">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>14.124975956034859</v>
+      </c>
+      <c r="R10">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>21.742022411399475</v>
+      </c>
+      <c r="S10">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>30.403895162587332</v>
+      </c>
+      <c r="U10" s="48">
+        <v>0.3</v>
+      </c>
+      <c r="V10">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W10">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.28856722306762</v>
+      </c>
+      <c r="X10">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>12.50527118864953</v>
+      </c>
+      <c r="Y10">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.0210995775381946</v>
+      </c>
+      <c r="Z10">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.5847032433122621</v>
+      </c>
+      <c r="AA10">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.6699745140907396</v>
+      </c>
+      <c r="AB10">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.7146162868865531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>70</v>
+      </c>
+      <c r="G11">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F11,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>14.980604982041015</v>
+      </c>
+      <c r="H11">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F11,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.3382949849802444</v>
+      </c>
+      <c r="I11">
+        <f>_xll.acq_options_blackscholes_price($C$4,F11,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>14.980604982041015</v>
+      </c>
+      <c r="J11">
+        <f>_xll.acq_options_blackscholes_price($C$4,G11,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.8027241433398957E-5</v>
+      </c>
+      <c r="L11" s="48">
+        <v>0.35</v>
+      </c>
+      <c r="M11">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.55711743962789662</v>
+      </c>
+      <c r="N11">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.7886799574834953</v>
+      </c>
+      <c r="O11">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.3665619494254173</v>
+      </c>
+      <c r="P11">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>8.6588352118634049</v>
+      </c>
+      <c r="Q11">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>14.68024803329898</v>
+      </c>
+      <c r="R11">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>22.140673845586747</v>
+      </c>
+      <c r="S11">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>30.622208044236658</v>
+      </c>
+      <c r="U11" s="48">
+        <v>0.35</v>
+      </c>
+      <c r="V11">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W11">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.429110201976329</v>
+      </c>
+      <c r="X11">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>12.866860834687323</v>
+      </c>
+      <c r="Y11">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.4931101832985831</v>
+      </c>
+      <c r="Z11">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.0341331984300837</v>
+      </c>
+      <c r="AA11">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.0148616348597272</v>
+      </c>
+      <c r="AB11">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.93898654017260696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>80</v>
+      </c>
+      <c r="G12">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F12,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>10.788121014927199</v>
+      </c>
+      <c r="H12">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F12,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>8.2510544914383672</v>
+      </c>
+      <c r="I12">
+        <f>_xll.acq_options_blackscholes_price($C$4,F12,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>10.788121014927199</v>
+      </c>
+      <c r="J12">
+        <f>_xll.acq_options_blackscholes_price($C$4,G12,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.6218005932214387E-7</v>
+      </c>
+      <c r="L12" s="48">
+        <v>0.4</v>
+      </c>
+      <c r="M12">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.73908665875073609</v>
+      </c>
+      <c r="N12">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.1408011079752605</v>
+      </c>
+      <c r="O12">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.8725625175067293</v>
+      </c>
+      <c r="P12">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>9.227755099494388</v>
+      </c>
+      <c r="Q12">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>15.19829496627456</v>
+      </c>
+      <c r="R12">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>22.527416601592876</v>
+      </c>
+      <c r="S12">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>30.850737745484096</v>
+      </c>
+      <c r="U12" s="48">
+        <v>0.4</v>
+      </c>
+      <c r="V12">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W12">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.576702408336132</v>
+      </c>
+      <c r="X12">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>13.202481650454104</v>
+      </c>
+      <c r="Y12">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.9219003176608709</v>
+      </c>
+      <c r="Z12">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.448487889031</v>
+      </c>
+      <c r="AA12">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.3457563802716948</v>
+      </c>
+      <c r="AB12">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.1674803035433001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>90</v>
+      </c>
+      <c r="G13">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F13,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>7.6566957498111279</v>
+      </c>
+      <c r="H13">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F13,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>13.793321561722518</v>
+      </c>
+      <c r="I13">
+        <f>_xll.acq_options_blackscholes_price($C$4,F13,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>7.6566957498111279</v>
+      </c>
+      <c r="J13">
+        <f>_xll.acq_options_blackscholes_price($C$4,G13,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.9304414708222245E-9</v>
+      </c>
+      <c r="L13" s="48">
+        <v>0.45</v>
+      </c>
+      <c r="M13">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.93172725196149564</v>
+      </c>
+      <c r="N13">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.4867387486766575</v>
+      </c>
+      <c r="O13">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.3497205066058342</v>
+      </c>
+      <c r="P13">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>9.7569243809158763</v>
+      </c>
+      <c r="Q13">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>15.684404035736932</v>
+      </c>
+      <c r="R13">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>22.901118497951956</v>
+      </c>
+      <c r="S13">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>31.084295825844606</v>
+      </c>
+      <c r="U13" s="48">
+        <v>0.45</v>
+      </c>
+      <c r="V13">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W13">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.727323879111289</v>
+      </c>
+      <c r="X13">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>13.51576476330748</v>
+      </c>
+      <c r="Y13">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>8.3155956253103511</v>
+      </c>
+      <c r="Z13">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.8332655650513772</v>
+      </c>
+      <c r="AA13">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.662572789779432</v>
+      </c>
+      <c r="AB13">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.3964938482637308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F14,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.3796450816355517</v>
+      </c>
+      <c r="H14">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F14,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.034358320176022</v>
+      </c>
+      <c r="I14">
+        <f>_xll.acq_options_blackscholes_price($C$4,F14,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.3796450816355517</v>
+      </c>
+      <c r="J14">
+        <f>_xll.acq_options_blackscholes_price($C$4,G14,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.167517628471426E-12</v>
+      </c>
+      <c r="L14" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="M14">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.1317126138357825</v>
+      </c>
+      <c r="N14">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.825231535228955</v>
+      </c>
+      <c r="O14">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.801645731668323</v>
+      </c>
+      <c r="P14">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>10.252559729951784</v>
+      </c>
+      <c r="Q14">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>16.142724570029145</v>
+      </c>
+      <c r="R14">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>23.261552607007062</v>
+      </c>
+      <c r="S14">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>31.319444688823182</v>
+      </c>
+      <c r="U14" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="V14">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W14">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.878498091942536</v>
+      </c>
+      <c r="X14">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>13.809632330257585</v>
+      </c>
+      <c r="Y14">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>8.6800903822513931</v>
+      </c>
+      <c r="Z14">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.1927188835421703</v>
+      </c>
+      <c r="AA14">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.9657980624896823</v>
+      </c>
+      <c r="AB14">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.6237713217188059</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B15" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15">
+        <v>110</v>
+      </c>
+      <c r="G15">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F15,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.7550156571442077</v>
+      </c>
+      <c r="H15">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F15,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="I15">
+        <f>_xll.acq_options_blackscholes_price($C$4,F15,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.7550156571442077</v>
+      </c>
+      <c r="J15">
+        <f>_xll.acq_options_blackscholes_price($C$4,G15,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.6428793012235105E-15</v>
+      </c>
+      <c r="L15" s="48">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M15">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.3365585025591749</v>
+      </c>
+      <c r="N15">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.1556763506308201</v>
+      </c>
+      <c r="O15">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.2312540008503348</v>
+      </c>
+      <c r="P15">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>10.719370459089447</v>
+      </c>
+      <c r="Q15">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>16.576573753268661</v>
+      </c>
+      <c r="R15">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>23.608942745230109</v>
+      </c>
+      <c r="S15">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>31.553881861379864</v>
+      </c>
+      <c r="U15" s="48">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V15">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="W15">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.028678254900704</v>
+      </c>
+      <c r="X15">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>14.086457106078548</v>
+      </c>
+      <c r="Y15">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.0198177682868135</v>
+      </c>
+      <c r="Z15">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.5302052099230963</v>
+      </c>
+      <c r="AA15">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.2561561952630882</v>
+      </c>
+      <c r="AB15">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.8479046798663319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>120</v>
+      </c>
+      <c r="G16">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F16,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.6109483404114453</v>
+      </c>
+      <c r="H16">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F16,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="I16">
+        <f>_xll.acq_options_blackscholes_price($C$4,F16,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.6109483404114453</v>
+      </c>
+      <c r="J16">
+        <f>_xll.acq_options_blackscholes_price($C$4,G16,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.3059135679790043E-18</v>
+      </c>
+      <c r="L16" s="48">
+        <v>0.6</v>
+      </c>
+      <c r="M16">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.5444021816862641</v>
+      </c>
+      <c r="N16">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.4778509106740358</v>
+      </c>
+      <c r="O16">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.6409346906283346</v>
+      </c>
+      <c r="P16">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>11.161027963773662</v>
+      </c>
+      <c r="Q16">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>16.988648850197563</v>
+      </c>
+      <c r="R16">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>23.943732677531585</v>
+      </c>
+      <c r="S16">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>31.786054869626298</v>
+      </c>
+      <c r="U16" s="48">
+        <v>0.6</v>
+      </c>
+      <c r="V16">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.005345917754727</v>
+      </c>
+      <c r="W16">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.176894025870496</v>
+      </c>
+      <c r="X16">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>14.348187494698188</v>
+      </c>
+      <c r="Y16">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.3382092346537036</v>
+      </c>
+      <c r="Z16">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.8484237377127499</v>
+      </c>
+      <c r="AA16">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.5344479649784546</v>
+      </c>
+      <c r="AB16">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.068028069267541</v>
+      </c>
+    </row>
+    <row r="17" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>130</v>
+      </c>
+      <c r="G17">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F17,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.8122480682922486</v>
+      </c>
+      <c r="H17">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F17,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="I17">
+        <f>_xll.acq_options_blackscholes_price($C$4,F17,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.8122480682922486</v>
+      </c>
+      <c r="J17">
+        <f>_xll.acq_options_blackscholes_price($C$4,G17,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.9625621136394617E-22</v>
+      </c>
+      <c r="L17" s="48">
+        <v>0.65</v>
+      </c>
+      <c r="M17">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.7538393451341321</v>
+      </c>
+      <c r="N17">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.7917558451558833</v>
+      </c>
+      <c r="O17">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>7.0326722168859277</v>
+      </c>
+      <c r="P17">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>11.580462132074587</v>
+      </c>
+      <c r="Q17">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>17.381176441458152</v>
+      </c>
+      <c r="R17">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>24.266465058303936</v>
+      </c>
+      <c r="S17">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>32.014915973629982</v>
+      </c>
+      <c r="U17" s="48">
+        <v>0.65</v>
+      </c>
+      <c r="V17">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.019387489338804</v>
+      </c>
+      <c r="W17">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.322541467052218</v>
+      </c>
+      <c r="X17">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>14.596441833137632</v>
+      </c>
+      <c r="Y17">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.637983728017673</v>
+      </c>
+      <c r="Z17">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.1495793862091972</v>
+      </c>
+      <c r="AA17">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.8014742129426224</v>
+      </c>
+      <c r="AB17">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.283627586778664</v>
+      </c>
+    </row>
+    <row r="18" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>140</v>
+      </c>
+      <c r="G18">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F18,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.2576425804726288</v>
+      </c>
+      <c r="H18">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F18,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="I18">
+        <f>_xll.acq_options_blackscholes_price($C$4,F18,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.2576425804726288</v>
+      </c>
+      <c r="J18">
+        <f>_xll.acq_options_blackscholes_price($C$4,G18,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.2715942320358724E-26</v>
+      </c>
+      <c r="L18" s="48">
+        <v>0.7</v>
+      </c>
+      <c r="M18">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.96380565221979</v>
+      </c>
+      <c r="N18">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.0975220615232182</v>
+      </c>
+      <c r="O18">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>7.40813485023385</v>
+      </c>
+      <c r="P18">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>11.980056871550772</v>
+      </c>
+      <c r="Q18">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>17.756019281551474</v>
+      </c>
+      <c r="R18">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>24.577716756978504</v>
+      </c>
+      <c r="S18">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>32.239762763653374</v>
+      </c>
+      <c r="U18" s="48">
+        <v>0.7</v>
+      </c>
+      <c r="V18">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.040155624016606</v>
+      </c>
+      <c r="W18">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.465254318063465</v>
+      </c>
+      <c r="X18">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>14.832578998839985</v>
+      </c>
+      <c r="Y18">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.9213379184106572</v>
+      </c>
+      <c r="Z18">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.435498641492515</v>
+      </c>
+      <c r="AA18">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.0580000145426993</v>
+      </c>
+      <c r="AB18">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.4944205008523568</v>
+      </c>
+    </row>
+    <row r="19" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>150</v>
+      </c>
+      <c r="G19">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F19,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.87364917342515458</v>
+      </c>
+      <c r="H19">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F19,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="I19">
+        <f>_xll.acq_options_blackscholes_price($C$4,F19,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.87364917342515458</v>
+      </c>
+      <c r="J19">
+        <f>_xll.acq_options_blackscholes_price($C$4,G19,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.6669095805321848E-31</v>
+      </c>
+      <c r="L19" s="48">
+        <v>0.75</v>
+      </c>
+      <c r="M19">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.1734908239105728</v>
+      </c>
+      <c r="N19">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.3953551181175712</v>
+      </c>
+      <c r="O19">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>7.7687405195595787</v>
+      </c>
+      <c r="P19">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>12.361783822894068</v>
+      </c>
+      <c r="Q19">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>18.114754266184605</v>
+      </c>
+      <c r="R19">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>24.878064222330167</v>
+      </c>
+      <c r="S19">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>32.460132474437401</v>
+      </c>
+      <c r="U19" s="48">
+        <v>0.75</v>
+      </c>
+      <c r="V19">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.066381381137603</v>
+      </c>
+      <c r="W19">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.604822951440077</v>
+      </c>
+      <c r="X19">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>15.057751545192005</v>
+      </c>
+      <c r="Y19">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>10.190075896726043</v>
+      </c>
+      <c r="Z19">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.7077131968609081</v>
+      </c>
+      <c r="AA19">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.3047394093293008</v>
+      </c>
+      <c r="AB19">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.7002771269771699</v>
+      </c>
+    </row>
+    <row r="20" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>160</v>
+      </c>
+      <c r="G20">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F20,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.60806327909027225</v>
+      </c>
+      <c r="H20">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F20,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="I20">
+        <f>_xll.acq_options_blackscholes_price($C$4,F20,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.60806327909027225</v>
+      </c>
+      <c r="J20">
+        <f>_xll.acq_options_blackscholes_price($C$4,G20,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.868419745828726E-36</v>
+      </c>
+      <c r="L20" s="48">
+        <v>0.8</v>
+      </c>
+      <c r="M20">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.3822760589289196</v>
+      </c>
+      <c r="N20">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.6855012429099574</v>
+      </c>
+      <c r="O20">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>8.1157062758994982</v>
+      </c>
+      <c r="P20">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>12.727296608648729</v>
+      </c>
+      <c r="Q20">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>18.458730355326026</v>
+      </c>
+      <c r="R20">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.168065289543748</v>
+      </c>
+      <c r="S20">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>32.675730604857705</v>
+      </c>
+      <c r="U20" s="48">
+        <v>0.8</v>
+      </c>
+      <c r="V20">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.097033642388915</v>
+      </c>
+      <c r="W20">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.741142139247827</v>
+      </c>
+      <c r="X20">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>15.2729460671897</v>
+      </c>
+      <c r="Y20">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>10.445700309453485</v>
+      </c>
+      <c r="Z20">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.9675215419987353</v>
+      </c>
+      <c r="AA20">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.5423505649096114</v>
+      </c>
+      <c r="AB20">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.901169441243951</v>
+      </c>
+      <c r="AD20">
+        <v>3.4746592085343946</v>
+      </c>
+      <c r="AE20">
+        <f>AD20-AB23</f>
+        <v>-6.7057470687359455E-14</v>
+      </c>
+    </row>
+    <row r="21" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>170</v>
+      </c>
+      <c r="G21">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F21,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.4243122048375545</v>
+      </c>
+      <c r="H21">
+        <f>_xll.acq_options_bjerksund_price_approx($C$4,F21,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="I21">
+        <f>_xll.acq_options_blackscholes_price($C$4,F21,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.4243122048375545</v>
+      </c>
+      <c r="J21">
+        <f>_xll.acq_options_blackscholes_price($C$4,G21,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.0810353477718544E-41</v>
+      </c>
+      <c r="L21" s="48">
+        <v>0.85</v>
+      </c>
+      <c r="M21">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.5896880914419889</v>
+      </c>
+      <c r="N21">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.9682263472148094</v>
+      </c>
+      <c r="O21">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>8.4500860099740365</v>
+      </c>
+      <c r="P21">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>13.077998996876133</v>
+      </c>
+      <c r="Q21">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>18.789112332169893</v>
+      </c>
+      <c r="R21">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.448250155289202</v>
+      </c>
+      <c r="S21">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>32.886381891485414</v>
+      </c>
+      <c r="U21" s="48">
+        <v>0.85</v>
+      </c>
+      <c r="V21">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.131271677953357</v>
+      </c>
+      <c r="W21">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>21.874176704910447</v>
+      </c>
+      <c r="X21">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>15.479014206765569</v>
+      </c>
+      <c r="Y21">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>10.689478061153395</v>
+      </c>
+      <c r="Z21">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.2160351309845367</v>
+      </c>
+      <c r="AA21">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.7714361792330635</v>
+      </c>
+      <c r="AB21">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.0971367888594727</v>
+      </c>
+    </row>
+    <row r="22" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="L22" s="48">
+        <v>0.9</v>
+      </c>
+      <c r="M22">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.7953651665542871</v>
+      </c>
+      <c r="N22">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.2438030119484296</v>
+      </c>
+      <c r="O22">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>8.7727996072321659</v>
+      </c>
+      <c r="P22">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>13.415095305183144</v>
+      </c>
+      <c r="Q22">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>19.106914373391973</v>
+      </c>
+      <c r="R22">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.719117512390625</v>
+      </c>
+      <c r="S22">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>33.091996127090255</v>
+      </c>
+      <c r="U22" s="48">
+        <v>0.9</v>
+      </c>
+      <c r="V22">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.168407147610274</v>
+      </c>
+      <c r="W22">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>22.003938547541125</v>
+      </c>
+      <c r="X22">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>15.676696740899636</v>
+      </c>
+      <c r="Y22">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>10.922488741216739</v>
+      </c>
+      <c r="Z22">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.4542135528883051</v>
+      </c>
+      <c r="AA22">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.992546402492394</v>
+      </c>
+      <c r="AB22">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.2882627227475894</v>
+      </c>
+    </row>
+    <row r="23" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="L23" s="48">
+        <v>0.95</v>
+      </c>
+      <c r="M23">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.9990316100764289</v>
+      </c>
+      <c r="N23">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.5125024519297554</v>
+      </c>
+      <c r="O23">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>9.0846557728416073</v>
+      </c>
+      <c r="P23">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>13.739628399632494</v>
+      </c>
+      <c r="Q23">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>19.413026166473443</v>
+      </c>
+      <c r="R23">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.981133583523786</v>
+      </c>
+      <c r="S23">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>33.292544011466831</v>
+      </c>
+      <c r="U23" s="48">
+        <v>0.95</v>
+      </c>
+      <c r="V23">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.207874016497883</v>
+      </c>
+      <c r="W23">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>22.130471052706028</v>
+      </c>
+      <c r="X23">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>15.866642505105219</v>
+      </c>
+      <c r="Y23">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>11.14566101178896</v>
+      </c>
+      <c r="Z23">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.6828917175824216</v>
+      </c>
+      <c r="AA23">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.2061828422575331</v>
+      </c>
+      <c r="AB23">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.4746592085344616</v>
+      </c>
+      <c r="AD23">
+        <v>3.4746600000000001</v>
+      </c>
+      <c r="AE23">
+        <f>AB23-AD23</f>
+        <v>-7.9146553844111622E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="L24" s="48">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <f>_xll.acq_options_bjerksund_price_approx(M$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.2004786488600772</v>
+      </c>
+      <c r="N24">
+        <f>_xll.acq_options_bjerksund_price_approx(N$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.7745896314136331</v>
+      </c>
+      <c r="O24">
+        <f>_xll.acq_options_bjerksund_price_approx(O$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>9.3863701128630979</v>
+      </c>
+      <c r="P24">
+        <f>_xll.acq_options_bjerksund_price_approx(P$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>14.052508832531942</v>
+      </c>
+      <c r="Q24">
+        <f>_xll.acq_options_bjerksund_price_approx(Q$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>19.708233489832239</v>
+      </c>
+      <c r="R24">
+        <f>_xll.acq_options_bjerksund_price_approx(R$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>26.234732756665451</v>
+      </c>
+      <c r="S24">
+        <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>33.488039891384361</v>
+      </c>
+      <c r="U24" s="48">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <f>_xll.acq_options_bjerksund_price_approx(V$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>30.249204819926547</v>
+      </c>
+      <c r="W24">
+        <f>_xll.acq_options_bjerksund_price_approx(W$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>22.253838391226381</v>
+      </c>
+      <c r="X24">
+        <f>_xll.acq_options_bjerksund_price_approx(X$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>16.049423418172978</v>
+      </c>
+      <c r="Y24">
+        <f>_xll.acq_options_bjerksund_price_approx(Y$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>11.359800416866619</v>
+      </c>
+      <c r="Z24">
+        <f>_xll.acq_options_bjerksund_price_approx(Z$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.902801148209889</v>
+      </c>
+      <c r="AA24">
+        <f>_xll.acq_options_bjerksund_price_approx(AA$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.412802895372181</v>
+      </c>
+      <c r="AB24">
+        <f>_xll.acq_options_bjerksund_price_approx(AB$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.6564557766512564</v>
+      </c>
+    </row>
+    <row r="26" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="V26" s="49"/>
+      <c r="W26" s="49"/>
+      <c r="X26" s="49"/>
+      <c r="Y26" s="49"/>
+    </row>
+    <row r="27" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="V27" s="49"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="49"/>
+      <c r="Z27" s="49"/>
+    </row>
+    <row r="28" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="V28" s="49"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
+      <c r="Y28" s="49"/>
+      <c r="Z28" s="49"/>
+    </row>
+    <row r="29" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="V29" s="49"/>
+      <c r="W29" s="49"/>
+      <c r="X29" s="49"/>
+      <c r="Y29" s="49"/>
+      <c r="Z29" s="49"/>
+    </row>
+    <row r="30" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="V30" s="49"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="49"/>
+      <c r="Y30" s="49"/>
+      <c r="Z30" s="49"/>
+      <c r="AA30" s="49"/>
+    </row>
+    <row r="31" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="V31" s="49"/>
+      <c r="W31" s="49"/>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="49"/>
+      <c r="Z31" s="49"/>
+      <c r="AA31" s="49"/>
+    </row>
+    <row r="32" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="V32" s="49"/>
+      <c r="W32" s="49"/>
+      <c r="X32" s="49"/>
+      <c r="Y32" s="49"/>
+      <c r="Z32" s="49"/>
+      <c r="AA32" s="49"/>
+    </row>
+    <row r="33" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V33" s="49"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="49"/>
+      <c r="Z33" s="49"/>
+      <c r="AA33" s="49"/>
+      <c r="AB33" s="49"/>
+    </row>
+    <row r="34" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="49"/>
+      <c r="Z34" s="49"/>
+      <c r="AA34" s="49"/>
+      <c r="AB34" s="49"/>
+    </row>
+    <row r="35" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V35" s="49"/>
+      <c r="W35" s="49"/>
+      <c r="X35" s="49"/>
+      <c r="Y35" s="49"/>
+      <c r="Z35" s="49"/>
+      <c r="AA35" s="49"/>
+      <c r="AB35" s="49"/>
+    </row>
+    <row r="36" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V36" s="49"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="49"/>
+      <c r="Y36" s="49"/>
+      <c r="Z36" s="49"/>
+      <c r="AA36" s="49"/>
+      <c r="AB36" s="49"/>
+    </row>
+    <row r="37" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="49"/>
+      <c r="Z37" s="49"/>
+      <c r="AA37" s="49"/>
+      <c r="AB37" s="49"/>
+    </row>
+    <row r="38" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V38" s="49"/>
+      <c r="W38" s="49"/>
+      <c r="X38" s="49"/>
+      <c r="Y38" s="49"/>
+      <c r="Z38" s="49"/>
+      <c r="AA38" s="49"/>
+      <c r="AB38" s="49"/>
+    </row>
+    <row r="39" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="49"/>
+      <c r="Z39" s="49"/>
+      <c r="AA39" s="49"/>
+      <c r="AB39" s="49"/>
+    </row>
+    <row r="40" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49"/>
+      <c r="Y40" s="49"/>
+      <c r="Z40" s="49"/>
+      <c r="AA40" s="49"/>
+      <c r="AB40" s="49"/>
+    </row>
+    <row r="41" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="49"/>
+      <c r="Y41" s="49"/>
+      <c r="Z41" s="49"/>
+      <c r="AA41" s="49"/>
+      <c r="AB41" s="49"/>
+    </row>
+    <row r="42" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="49"/>
+      <c r="Z42" s="49"/>
+      <c r="AA42" s="49"/>
+      <c r="AB42" s="49"/>
+    </row>
+    <row r="43" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49"/>
+      <c r="Y43" s="49"/>
+      <c r="Z43" s="49"/>
+      <c r="AA43" s="49"/>
+      <c r="AB43" s="49"/>
+    </row>
+    <row r="44" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V44" s="49"/>
+      <c r="W44" s="49"/>
+      <c r="X44" s="49"/>
+      <c r="Y44" s="49"/>
+      <c r="Z44" s="49"/>
+      <c r="AA44" s="49"/>
+      <c r="AB44" s="49"/>
+    </row>
+    <row r="45" spans="22:28" x14ac:dyDescent="0.25">
+      <c r="V45" s="49"/>
+      <c r="W45" s="49"/>
+      <c r="X45" s="49"/>
+      <c r="Y45" s="49"/>
+      <c r="Z45" s="49"/>
+      <c r="AA45" s="49"/>
+      <c r="AB45" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{69E1F7C3-E9DE-4863-9FC4-322489C91572}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18766,9 +20816,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet7">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B1:K202"/>

</xml_diff>

<commit_message>
added greeks for Bjerksund-Stensland approximation for american options
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276C920C-9404-46B8-8BC2-3A9B48BD19E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31BF5AE-1871-4388-8DBB-0FAA2192299F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="150">
   <si>
     <t>x</t>
   </si>
@@ -625,6 +625,21 @@
   <si>
     <t>Spot Price</t>
   </si>
+  <si>
+    <t>Call Greeks: Bjerksund Stensland Numerical Greeks</t>
+  </si>
+  <si>
+    <t>Call Greeks: Black-Scholes Analyical Greeks</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Put Greeks: Black-Scholes Analyical Greeks</t>
+  </si>
+  <si>
+    <t>Put Greeks: Bjerksund Stensland Numerical Greeks</t>
+  </si>
 </sst>
 </file>
 
@@ -1036,15 +1051,15 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
@@ -10288,7 +10303,7 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8023.35113</v>
+        <v>1.3.8023.37862</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -10402,37 +10417,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="L2" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="S2" s="45" t="s">
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="S2" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -11607,16 +11622,16 @@
         <f>_xll.acq_options_black_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>0.65000000000000013</v>
       </c>
-      <c r="S17" s="45" t="s">
+      <c r="S17" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="45"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>0.2</v>
@@ -12797,37 +12812,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="L2" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="S2" s="45" t="s">
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="S2" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -14002,16 +14017,16 @@
         <f>_xll.acq_options_bachelier_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>25.999999999962554</v>
       </c>
-      <c r="S17" s="45" t="s">
+      <c r="S17" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="45"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>20</v>
@@ -14888,14 +14903,14 @@
       </c>
     </row>
     <row r="32" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="45" t="s">
+      <c r="L32" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="48"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
       <c r="AB32" t="s">
         <v>111</v>
       </c>
@@ -15540,7 +15555,7 @@
   <dimension ref="A1:AS56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15555,37 +15570,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="L2" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="S2" s="45" t="s">
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="S2" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
       <c r="AA2" s="38"/>
       <c r="AB2" s="38"/>
       <c r="AD2" s="3" t="s">
@@ -16862,16 +16877,16 @@
         <f>_xll.acq_options_blackscholes_vol($C$4,$C$5,$C$6,$C$8,$C$9,$N17,FALSE)</f>
         <v>0.65</v>
       </c>
-      <c r="S17" s="45" t="s">
+      <c r="S17" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="45"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
       <c r="AA17" s="38"/>
       <c r="AB17" s="38"/>
       <c r="AD17" s="16">
@@ -18478,14 +18493,15 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937DB880-8B2C-4D2D-B567-C1990F7A61F3}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:AE45"/>
+  <dimension ref="A1:AI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
@@ -18493,15 +18509,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -18516,15 +18532,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45" t="s">
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="45"/>
+      <c r="J3" s="48"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -18629,7 +18645,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.2409702289365026</v>
       </c>
-      <c r="L5" s="48">
+      <c r="L5" s="46">
         <v>0.05</v>
       </c>
       <c r="M5">
@@ -18660,7 +18676,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
         <v>29.911482759239618</v>
       </c>
-      <c r="U5" s="48">
+      <c r="U5" s="46">
         <v>0.05</v>
       </c>
       <c r="V5">
@@ -18718,7 +18734,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G6,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.4604738210067554</v>
       </c>
-      <c r="L6" s="48">
+      <c r="L6" s="46">
         <v>0.1</v>
       </c>
       <c r="M6">
@@ -18749,7 +18765,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>29.866937861547115</v>
       </c>
-      <c r="U6" s="48">
+      <c r="U6" s="46">
         <v>0.1</v>
       </c>
       <c r="V6">
@@ -18807,7 +18823,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G7,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.49501536694438641</v>
       </c>
-      <c r="L7" s="48">
+      <c r="L7" s="46">
         <v>0.15</v>
       </c>
       <c r="M7">
@@ -18838,7 +18854,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
         <v>29.91318851001617</v>
       </c>
-      <c r="U7" s="48">
+      <c r="U7" s="46">
         <v>0.15</v>
       </c>
       <c r="V7">
@@ -18896,7 +18912,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G8,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.11085764156847244</v>
       </c>
-      <c r="L8" s="48">
+      <c r="L8" s="46">
         <v>0.2</v>
       </c>
       <c r="M8">
@@ -18927,7 +18943,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.033950291703007</v>
       </c>
-      <c r="U8" s="48">
+      <c r="U8" s="46">
         <v>0.2</v>
       </c>
       <c r="V8">
@@ -18985,7 +19001,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G9,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.426895703799709E-2</v>
       </c>
-      <c r="L9" s="48">
+      <c r="L9" s="46">
         <v>0.25</v>
       </c>
       <c r="M9">
@@ -19016,7 +19032,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.203730848908037</v>
       </c>
-      <c r="U9" s="48">
+      <c r="U9" s="46">
         <v>0.25</v>
       </c>
       <c r="V9">
@@ -19074,7 +19090,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G10,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>9.3215811534007841E-4</v>
       </c>
-      <c r="L10" s="48">
+      <c r="L10" s="46">
         <v>0.3</v>
       </c>
       <c r="M10">
@@ -19105,7 +19121,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.403895162587332</v>
       </c>
-      <c r="U10" s="48">
+      <c r="U10" s="46">
         <v>0.3</v>
       </c>
       <c r="V10">
@@ -19157,7 +19173,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G11,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>2.8027241433398957E-5</v>
       </c>
-      <c r="L11" s="48">
+      <c r="L11" s="46">
         <v>0.35</v>
       </c>
       <c r="M11">
@@ -19188,7 +19204,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.622208044236658</v>
       </c>
-      <c r="U11" s="48">
+      <c r="U11" s="46">
         <v>0.35</v>
       </c>
       <c r="V11">
@@ -19240,7 +19256,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G12,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.6218005932214387E-7</v>
       </c>
-      <c r="L12" s="48">
+      <c r="L12" s="46">
         <v>0.4</v>
       </c>
       <c r="M12">
@@ -19271,7 +19287,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.850737745484096</v>
       </c>
-      <c r="U12" s="48">
+      <c r="U12" s="46">
         <v>0.4</v>
       </c>
       <c r="V12">
@@ -19323,7 +19339,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G13,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.9304414708222245E-9</v>
       </c>
-      <c r="L13" s="48">
+      <c r="L13" s="46">
         <v>0.45</v>
       </c>
       <c r="M13">
@@ -19354,7 +19370,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.084295825844606</v>
       </c>
-      <c r="U13" s="48">
+      <c r="U13" s="46">
         <v>0.45</v>
       </c>
       <c r="V13">
@@ -19409,7 +19425,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G14,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>4.167517628471426E-12</v>
       </c>
-      <c r="L14" s="48">
+      <c r="L14" s="46">
         <v>0.5</v>
       </c>
       <c r="M14">
@@ -19440,7 +19456,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.319444688823182</v>
       </c>
-      <c r="U14" s="48">
+      <c r="U14" s="46">
         <v>0.5</v>
       </c>
       <c r="V14">
@@ -19473,7 +19489,7 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="45" t="s">
         <v>142</v>
       </c>
       <c r="F15">
@@ -19495,7 +19511,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G15,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.6428793012235105E-15</v>
       </c>
-      <c r="L15" s="48">
+      <c r="L15" s="46">
         <v>0.55000000000000004</v>
       </c>
       <c r="M15">
@@ -19526,7 +19542,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.553881861379864</v>
       </c>
-      <c r="U15" s="48">
+      <c r="U15" s="46">
         <v>0.55000000000000004</v>
       </c>
       <c r="V15">
@@ -19578,7 +19594,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G16,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.3059135679790043E-18</v>
       </c>
-      <c r="L16" s="48">
+      <c r="L16" s="46">
         <v>0.6</v>
       </c>
       <c r="M16">
@@ -19609,7 +19625,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.786054869626298</v>
       </c>
-      <c r="U16" s="48">
+      <c r="U16" s="46">
         <v>0.6</v>
       </c>
       <c r="V16">
@@ -19641,7 +19657,7 @@
         <v>2.068028069267541</v>
       </c>
     </row>
-    <row r="17" spans="6:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:35" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>130</v>
       </c>
@@ -19661,7 +19677,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G17,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.9625621136394617E-22</v>
       </c>
-      <c r="L17" s="48">
+      <c r="L17" s="46">
         <v>0.65</v>
       </c>
       <c r="M17">
@@ -19692,7 +19708,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.014915973629982</v>
       </c>
-      <c r="U17" s="48">
+      <c r="U17" s="46">
         <v>0.65</v>
       </c>
       <c r="V17">
@@ -19724,7 +19740,7 @@
         <v>2.283627586778664</v>
       </c>
     </row>
-    <row r="18" spans="6:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:35" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>140</v>
       </c>
@@ -19744,7 +19760,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G18,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.2715942320358724E-26</v>
       </c>
-      <c r="L18" s="48">
+      <c r="L18" s="46">
         <v>0.7</v>
       </c>
       <c r="M18">
@@ -19775,7 +19791,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.239762763653374</v>
       </c>
-      <c r="U18" s="48">
+      <c r="U18" s="46">
         <v>0.7</v>
       </c>
       <c r="V18">
@@ -19807,7 +19823,7 @@
         <v>2.4944205008523568</v>
       </c>
     </row>
-    <row r="19" spans="6:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:35" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>150</v>
       </c>
@@ -19827,7 +19843,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G19,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.6669095805321848E-31</v>
       </c>
-      <c r="L19" s="48">
+      <c r="L19" s="46">
         <v>0.75</v>
       </c>
       <c r="M19">
@@ -19858,7 +19874,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.460132474437401</v>
       </c>
-      <c r="U19" s="48">
+      <c r="U19" s="46">
         <v>0.75</v>
       </c>
       <c r="V19">
@@ -19890,7 +19906,7 @@
         <v>2.7002771269771699</v>
       </c>
     </row>
-    <row r="20" spans="6:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:35" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>160</v>
       </c>
@@ -19910,7 +19926,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G20,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>4.868419745828726E-36</v>
       </c>
-      <c r="L20" s="48">
+      <c r="L20" s="46">
         <v>0.8</v>
       </c>
       <c r="M20">
@@ -19941,7 +19957,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.675730604857705</v>
       </c>
-      <c r="U20" s="48">
+      <c r="U20" s="46">
         <v>0.8</v>
       </c>
       <c r="V20">
@@ -19980,7 +19996,7 @@
         <v>-6.7057470687359455E-14</v>
       </c>
     </row>
-    <row r="21" spans="6:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:35" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>170</v>
       </c>
@@ -20000,7 +20016,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G21,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.0810353477718544E-41</v>
       </c>
-      <c r="L21" s="48">
+      <c r="L21" s="46">
         <v>0.85</v>
       </c>
       <c r="M21">
@@ -20031,7 +20047,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.886381891485414</v>
       </c>
-      <c r="U21" s="48">
+      <c r="U21" s="46">
         <v>0.85</v>
       </c>
       <c r="V21">
@@ -20063,8 +20079,8 @@
         <v>3.0971367888594727</v>
       </c>
     </row>
-    <row r="22" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="L22" s="48">
+    <row r="22" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="L22" s="46">
         <v>0.9</v>
       </c>
       <c r="M22">
@@ -20095,7 +20111,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
         <v>33.091996127090255</v>
       </c>
-      <c r="U22" s="48">
+      <c r="U22" s="46">
         <v>0.9</v>
       </c>
       <c r="V22">
@@ -20127,8 +20143,8 @@
         <v>3.2882627227475894</v>
       </c>
     </row>
-    <row r="23" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="L23" s="48">
+    <row r="23" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="L23" s="46">
         <v>0.95</v>
       </c>
       <c r="M23">
@@ -20159,7 +20175,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
         <v>33.292544011466831</v>
       </c>
-      <c r="U23" s="48">
+      <c r="U23" s="46">
         <v>0.95</v>
       </c>
       <c r="V23">
@@ -20198,8 +20214,8 @@
         <v>-7.9146553844111622E-7</v>
       </c>
     </row>
-    <row r="24" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="L24" s="48">
+    <row r="24" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="L24" s="46">
         <v>1</v>
       </c>
       <c r="M24">
@@ -20230,7 +20246,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
         <v>33.488039891384361</v>
       </c>
-      <c r="U24" s="48">
+      <c r="U24" s="46">
         <v>1</v>
       </c>
       <c r="V24">
@@ -20262,179 +20278,2157 @@
         <v>3.6564557766512564</v>
       </c>
     </row>
-    <row r="26" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="V26" s="49"/>
-      <c r="W26" s="49"/>
-      <c r="X26" s="49"/>
-      <c r="Y26" s="49"/>
-    </row>
-    <row r="27" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="V27" s="49"/>
-      <c r="W27" s="49"/>
-      <c r="X27" s="49"/>
-      <c r="Y27" s="49"/>
-      <c r="Z27" s="49"/>
-    </row>
-    <row r="28" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="V28" s="49"/>
-      <c r="W28" s="49"/>
-      <c r="X28" s="49"/>
-      <c r="Y28" s="49"/>
-      <c r="Z28" s="49"/>
-    </row>
-    <row r="29" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="V29" s="49"/>
-      <c r="W29" s="49"/>
-      <c r="X29" s="49"/>
-      <c r="Y29" s="49"/>
-      <c r="Z29" s="49"/>
-    </row>
-    <row r="30" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="V30" s="49"/>
-      <c r="W30" s="49"/>
-      <c r="X30" s="49"/>
-      <c r="Y30" s="49"/>
-      <c r="Z30" s="49"/>
-      <c r="AA30" s="49"/>
-    </row>
-    <row r="31" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="V31" s="49"/>
-      <c r="W31" s="49"/>
-      <c r="X31" s="49"/>
-      <c r="Y31" s="49"/>
-      <c r="Z31" s="49"/>
-      <c r="AA31" s="49"/>
-    </row>
-    <row r="32" spans="6:31" x14ac:dyDescent="0.25">
-      <c r="V32" s="49"/>
-      <c r="W32" s="49"/>
-      <c r="X32" s="49"/>
-      <c r="Y32" s="49"/>
-      <c r="Z32" s="49"/>
-      <c r="AA32" s="49"/>
-    </row>
-    <row r="33" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V33" s="49"/>
-      <c r="W33" s="49"/>
-      <c r="X33" s="49"/>
-      <c r="Y33" s="49"/>
-      <c r="Z33" s="49"/>
-      <c r="AA33" s="49"/>
-      <c r="AB33" s="49"/>
-    </row>
-    <row r="34" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V34" s="49"/>
-      <c r="W34" s="49"/>
-      <c r="X34" s="49"/>
-      <c r="Y34" s="49"/>
-      <c r="Z34" s="49"/>
-      <c r="AA34" s="49"/>
-      <c r="AB34" s="49"/>
-    </row>
-    <row r="35" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V35" s="49"/>
-      <c r="W35" s="49"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="49"/>
-      <c r="Z35" s="49"/>
-      <c r="AA35" s="49"/>
-      <c r="AB35" s="49"/>
-    </row>
-    <row r="36" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V36" s="49"/>
-      <c r="W36" s="49"/>
-      <c r="X36" s="49"/>
-      <c r="Y36" s="49"/>
-      <c r="Z36" s="49"/>
-      <c r="AA36" s="49"/>
-      <c r="AB36" s="49"/>
-    </row>
-    <row r="37" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V37" s="49"/>
-      <c r="W37" s="49"/>
-      <c r="X37" s="49"/>
-      <c r="Y37" s="49"/>
-      <c r="Z37" s="49"/>
-      <c r="AA37" s="49"/>
-      <c r="AB37" s="49"/>
-    </row>
-    <row r="38" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V38" s="49"/>
-      <c r="W38" s="49"/>
-      <c r="X38" s="49"/>
-      <c r="Y38" s="49"/>
-      <c r="Z38" s="49"/>
-      <c r="AA38" s="49"/>
-      <c r="AB38" s="49"/>
-    </row>
-    <row r="39" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V39" s="49"/>
-      <c r="W39" s="49"/>
-      <c r="X39" s="49"/>
-      <c r="Y39" s="49"/>
-      <c r="Z39" s="49"/>
-      <c r="AA39" s="49"/>
-      <c r="AB39" s="49"/>
-    </row>
-    <row r="40" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V40" s="49"/>
-      <c r="W40" s="49"/>
-      <c r="X40" s="49"/>
-      <c r="Y40" s="49"/>
-      <c r="Z40" s="49"/>
-      <c r="AA40" s="49"/>
-      <c r="AB40" s="49"/>
-    </row>
-    <row r="41" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V41" s="49"/>
-      <c r="W41" s="49"/>
-      <c r="X41" s="49"/>
-      <c r="Y41" s="49"/>
-      <c r="Z41" s="49"/>
-      <c r="AA41" s="49"/>
-      <c r="AB41" s="49"/>
-    </row>
-    <row r="42" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V42" s="49"/>
-      <c r="W42" s="49"/>
-      <c r="X42" s="49"/>
-      <c r="Y42" s="49"/>
-      <c r="Z42" s="49"/>
-      <c r="AA42" s="49"/>
-      <c r="AB42" s="49"/>
-    </row>
-    <row r="43" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V43" s="49"/>
-      <c r="W43" s="49"/>
-      <c r="X43" s="49"/>
-      <c r="Y43" s="49"/>
-      <c r="Z43" s="49"/>
-      <c r="AA43" s="49"/>
-      <c r="AB43" s="49"/>
-    </row>
-    <row r="44" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V44" s="49"/>
-      <c r="W44" s="49"/>
-      <c r="X44" s="49"/>
-      <c r="Y44" s="49"/>
-      <c r="Z44" s="49"/>
-      <c r="AA44" s="49"/>
-      <c r="AB44" s="49"/>
-    </row>
-    <row r="45" spans="22:28" x14ac:dyDescent="0.25">
-      <c r="V45" s="49"/>
-      <c r="W45" s="49"/>
-      <c r="X45" s="49"/>
-      <c r="Y45" s="49"/>
-      <c r="Z45" s="49"/>
-      <c r="AA45" s="49"/>
-      <c r="AB45" s="49"/>
+    <row r="26" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+    </row>
+    <row r="27" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="V27" s="47"/>
+      <c r="W27" s="47"/>
+      <c r="X27" s="47"/>
+      <c r="Y27" s="47"/>
+      <c r="Z27" s="47"/>
+    </row>
+    <row r="28" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="V28" s="47"/>
+      <c r="W28" s="47"/>
+      <c r="X28" s="47"/>
+      <c r="Y28" s="47"/>
+      <c r="Z28" s="47"/>
+    </row>
+    <row r="29" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="V29" s="47"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="47"/>
+      <c r="Y29" s="47"/>
+      <c r="Z29" s="47"/>
+    </row>
+    <row r="30" spans="6:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="S30" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="T30" s="48"/>
+      <c r="U30" s="48"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="48"/>
+      <c r="X30" s="48"/>
+      <c r="Y30" s="48"/>
+      <c r="Z30" s="48"/>
+      <c r="AC30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" t="s">
+        <v>100</v>
+      </c>
+      <c r="I31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J31" t="s">
+        <v>102</v>
+      </c>
+      <c r="K31" t="s">
+        <v>103</v>
+      </c>
+      <c r="L31" t="s">
+        <v>104</v>
+      </c>
+      <c r="M31" t="s">
+        <v>105</v>
+      </c>
+      <c r="N31" t="s">
+        <v>106</v>
+      </c>
+      <c r="R31" t="s">
+        <v>125</v>
+      </c>
+      <c r="S31" t="s">
+        <v>99</v>
+      </c>
+      <c r="T31" t="s">
+        <v>100</v>
+      </c>
+      <c r="U31" t="s">
+        <v>101</v>
+      </c>
+      <c r="V31" t="s">
+        <v>102</v>
+      </c>
+      <c r="W31" t="s">
+        <v>103</v>
+      </c>
+      <c r="X31" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F32" s="13">
+        <v>100</v>
+      </c>
+      <c r="G32">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.2636854255143088</v>
+      </c>
+      <c r="H32">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.17541526927900009</v>
+      </c>
+      <c r="I32">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.1639582327188691E-3</v>
+      </c>
+      <c r="J32">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>38.532113576183825</v>
+      </c>
+      <c r="K32">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>156.14909596450843</v>
+      </c>
+      <c r="L32">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.1925599174844592</v>
+      </c>
+      <c r="M32">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>35.656088692297416</v>
+      </c>
+      <c r="N32">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-1.7307953841516621</v>
+      </c>
+      <c r="R32" s="13">
+        <v>100</v>
+      </c>
+      <c r="S32">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>46.29908424676718</v>
+      </c>
+      <c r="T32">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.17541526934222221</v>
+      </c>
+      <c r="U32">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.1651385288094013E-3</v>
+      </c>
+      <c r="V32">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>38.532115805058758</v>
+      </c>
+      <c r="W32">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>156.14908813078776</v>
+      </c>
+      <c r="X32">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.1925600030594994</v>
+      </c>
+      <c r="Y32">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>35.694603771769785</v>
+      </c>
+      <c r="Z32">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-1.7307846647220793</v>
+      </c>
+      <c r="AB32">
+        <f>G32-S32</f>
+        <v>-43.035398821252869</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" ref="AC32:AI42" si="0">H32-T32</f>
+        <v>-6.3222121982065005E-11</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="0"/>
+        <v>-1.1802960905322318E-6</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="0"/>
+        <v>-2.2288749335075408E-6</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="0"/>
+        <v>7.8337206730338949E-6</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="0"/>
+        <v>-8.5575040165153382E-8</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="0"/>
+        <v>-3.8515079472368541E-2</v>
+      </c>
+      <c r="AI32">
+        <f t="shared" si="0"/>
+        <v>-1.071942958286165E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F33" s="13">
+        <v>110</v>
+      </c>
+      <c r="G33">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.3357296360768061</v>
+      </c>
+      <c r="H33">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.23979644236504782</v>
+      </c>
+      <c r="I33">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.6478378357714973E-3</v>
+      </c>
+      <c r="J33">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>50.269871257656568</v>
+      </c>
+      <c r="K33">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>115.94092050870586</v>
+      </c>
+      <c r="L33">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.1356379836513497</v>
+      </c>
+      <c r="M33">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>52.554444882328966</v>
+      </c>
+      <c r="N33">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.1933746518243424</v>
+      </c>
+      <c r="R33" s="13">
+        <v>110</v>
+      </c>
+      <c r="S33">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.3357296360768061</v>
+      </c>
+      <c r="T33">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.23979644241728901</v>
+      </c>
+      <c r="U33">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.6472559788822673E-3</v>
+      </c>
+      <c r="V33">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>50.269873340297138</v>
+      </c>
+      <c r="W33">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>115.94090950324943</v>
+      </c>
+      <c r="X33">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>1.1356382729549774</v>
+      </c>
+      <c r="Y33">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>52.604697574562458</v>
+      </c>
+      <c r="Z33">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.1933498888502481</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" ref="AB33:AB42" si="1">G33-S33</f>
+        <v>0</v>
+      </c>
+      <c r="AC33">
+        <f t="shared" ref="AC33:AC42" si="2">H33-T33</f>
+        <v>-5.2241183601253738E-11</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" ref="AD33:AD42" si="3">I33-U33</f>
+        <v>5.8185688923007711E-7</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" ref="AE33:AE42" si="4">J33-V33</f>
+        <v>-2.0826405702223383E-6</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" ref="AF33:AF42" si="5">K33-W33</f>
+        <v>1.1005456428847538E-5</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" ref="AG33:AG42" si="6">L33-X33</f>
+        <v>-2.8930362772072726E-7</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" ref="AH33:AH42" si="7">M33-Y33</f>
+        <v>-5.0252692233492269E-2</v>
+      </c>
+      <c r="AI33">
+        <f t="shared" si="0"/>
+        <v>-2.4762974094372225E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F34" s="13">
+        <v>120</v>
+      </c>
+      <c r="G34">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>8.0694676224533275</v>
+      </c>
+      <c r="H34">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.30715015673976609</v>
+      </c>
+      <c r="I34">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.7668537440113141E-3</v>
+      </c>
+      <c r="J34">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>60.910241782383736</v>
+      </c>
+      <c r="K34">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>68.125187979717339</v>
+      </c>
+      <c r="L34">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.97868468884598769</v>
+      </c>
+      <c r="M34">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>71.910482979671286</v>
+      </c>
+      <c r="N34">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.5613828668369365</v>
+      </c>
+      <c r="R34" s="13">
+        <v>120</v>
+      </c>
+      <c r="S34">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>8.0694676224533275</v>
+      </c>
+      <c r="T34">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.30715015675424467</v>
+      </c>
+      <c r="U34">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.7678048079652378E-3</v>
+      </c>
+      <c r="V34">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>60.91024327168715</v>
+      </c>
+      <c r="W34">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>68.125179693630088</v>
+      </c>
+      <c r="X34">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.97868484003505463</v>
+      </c>
+      <c r="Y34">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>71.971377970140097</v>
+      </c>
+      <c r="Z34">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.5613441062371574</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="2"/>
+        <v>-1.447858499759036E-11</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="3"/>
+        <v>-9.5106395392365733E-7</v>
+      </c>
+      <c r="AE34">
+        <f t="shared" si="4"/>
+        <v>-1.4893034148144579E-6</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="5"/>
+        <v>8.2860872510082118E-6</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="6"/>
+        <v>-1.5118906693256662E-7</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="7"/>
+        <v>-6.0894990468810306E-2</v>
+      </c>
+      <c r="AI34">
+        <f t="shared" si="0"/>
+        <v>-3.8760599779141813E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F35" s="13">
+        <v>130</v>
+      </c>
+      <c r="G35">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>11.477513762412599</v>
+      </c>
+      <c r="H35">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.37416443724680448</v>
+      </c>
+      <c r="I35">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.5938365878537297E-3</v>
+      </c>
+      <c r="J35">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>69.632493502681427</v>
+      </c>
+      <c r="K35">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.623580057754225</v>
+      </c>
+      <c r="L35">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.75837629509578619</v>
+      </c>
+      <c r="M35">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>92.840036806656201</v>
+      </c>
+      <c r="N35">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.7930243266638399</v>
+      </c>
+      <c r="R35" s="13">
+        <v>130</v>
+      </c>
+      <c r="S35">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>11.477513762412599</v>
+      </c>
+      <c r="T35">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.3741644372389949</v>
+      </c>
+      <c r="U35">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.5924254948707267E-3</v>
+      </c>
+      <c r="V35">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>69.632494289572065</v>
+      </c>
+      <c r="W35">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.62357394681667</v>
+      </c>
+      <c r="X35">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.75837574370535099</v>
+      </c>
+      <c r="Y35">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>92.909657696641844</v>
+      </c>
+      <c r="Z35">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.7929738887338473</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC35">
+        <f t="shared" si="2"/>
+        <v>7.8095863109695074E-12</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="3"/>
+        <v>1.411092983003015E-6</v>
+      </c>
+      <c r="AE35">
+        <f t="shared" si="4"/>
+        <v>-7.8689063798265124E-7</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="5"/>
+        <v>6.1109375550927325E-6</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="6"/>
+        <v>5.5139043519947251E-7</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="7"/>
+        <v>-6.9620889985642975E-2</v>
+      </c>
+      <c r="AI35">
+        <f t="shared" si="0"/>
+        <v>-5.0437929992597219E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F36" s="13">
+        <v>140</v>
+      </c>
+      <c r="G36">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>15.543021627094788</v>
+      </c>
+      <c r="H36">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.43828610799323542</v>
+      </c>
+      <c r="I36">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.2030380831856746E-3</v>
+      </c>
+      <c r="J36">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>75.988528294290191</v>
+      </c>
+      <c r="K36">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.6135147379591217</v>
+      </c>
+      <c r="L36">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.51105253362493386</v>
+      </c>
+      <c r="M36">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>114.46660199482039</v>
+      </c>
+      <c r="N36">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.8669034510642177</v>
+      </c>
+      <c r="R36" s="13">
+        <v>140</v>
+      </c>
+      <c r="S36">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>15.543021627094788</v>
+      </c>
+      <c r="T36">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.43828610798973633</v>
+      </c>
+      <c r="U36">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>6.2031451884485686E-3</v>
+      </c>
+      <c r="V36">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>75.988528558494963</v>
+      </c>
+      <c r="W36">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.6135177115936088</v>
+      </c>
+      <c r="X36">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.51105236932348352</v>
+      </c>
+      <c r="Y36">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>114.54258372867073</v>
+      </c>
+      <c r="Z36">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.8668451302990605</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="2"/>
+        <v>3.4990899067111059E-12</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="3"/>
+        <v>-1.071052628939459E-7</v>
+      </c>
+      <c r="AE36">
+        <f t="shared" si="4"/>
+        <v>-2.6420477183819457E-7</v>
+      </c>
+      <c r="AF36">
+        <f t="shared" si="5"/>
+        <v>2.9736344870912035E-6</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="6"/>
+        <v>1.6430145033385912E-7</v>
+      </c>
+      <c r="AH36">
+        <f t="shared" si="7"/>
+        <v>-7.5981733850341016E-2</v>
+      </c>
+      <c r="AI36">
+        <f t="shared" si="0"/>
+        <v>-5.8320765157215959E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F37" s="13">
+        <v>150</v>
+      </c>
+      <c r="G37">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>20.227726902988501</v>
+      </c>
+      <c r="H37">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.49777974464149111</v>
+      </c>
+      <c r="I37">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.680789172402001E-3</v>
+      </c>
+      <c r="J37">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>79.862856978154454</v>
+      </c>
+      <c r="K37">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-12.478572131158217</v>
+      </c>
+      <c r="L37">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.26620927684462004</v>
+      </c>
+      <c r="M37">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>136.01822552182341</v>
+      </c>
+      <c r="N37">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.7795410490227823</v>
+      </c>
+      <c r="R37" s="13">
+        <v>150</v>
+      </c>
+      <c r="S37">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>20.227726902988501</v>
+      </c>
+      <c r="T37">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.49777974455582391</v>
+      </c>
+      <c r="U37">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.6791365019068672E-3</v>
+      </c>
+      <c r="V37">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>79.86285705806533</v>
+      </c>
+      <c r="W37">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-12.478571415322708</v>
+      </c>
+      <c r="X37">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.26620952352688443</v>
+      </c>
+      <c r="Y37">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>136.09808695096271</v>
+      </c>
+      <c r="Z37">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.7794792387239546</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="2"/>
+        <v>8.5667195559580023E-11</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="3"/>
+        <v>1.652670495133797E-6</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="4"/>
+        <v>-7.9910876138455933E-8</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="5"/>
+        <v>-7.1583550820264463E-7</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="6"/>
+        <v>-2.4668226439317209E-7</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="7"/>
+        <v>-7.9861429139299389E-2</v>
+      </c>
+      <c r="AI37">
+        <f t="shared" si="0"/>
+        <v>-6.1810298827680299E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F38" s="13">
+        <v>160</v>
+      </c>
+      <c r="G38">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.479783849233741</v>
+      </c>
+      <c r="H38">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.55164313309319368</v>
+      </c>
+      <c r="I38">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.0874859880423173E-3</v>
+      </c>
+      <c r="J38">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>81.389919636736337</v>
+      </c>
+      <c r="K38">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-4.0385963018252369</v>
+      </c>
+      <c r="L38">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.4231462936750177E-2</v>
+      </c>
+      <c r="M38">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>156.87639973791079</v>
+      </c>
+      <c r="N38">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.5407699952495477</v>
+      </c>
+      <c r="R38" s="13">
+        <v>160</v>
+      </c>
+      <c r="S38">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>25.479783849233741</v>
+      </c>
+      <c r="T38">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.55164313309694135</v>
+      </c>
+      <c r="U38">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>5.0868699934212263E-3</v>
+      </c>
+      <c r="V38">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>81.389919894739634</v>
+      </c>
+      <c r="W38">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-4.0385962960226589</v>
+      </c>
+      <c r="X38">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.4232097050586193E-2</v>
+      </c>
+      <c r="Y38">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>156.9577936156922</v>
+      </c>
+      <c r="Z38">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.5407089637829561</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="2"/>
+        <v>-3.7476688419246784E-12</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="3"/>
+        <v>6.1599462109103442E-7</v>
+      </c>
+      <c r="AE38">
+        <f t="shared" si="4"/>
+        <v>-2.5800329694902757E-7</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="5"/>
+        <v>-5.8025779736681216E-9</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="6"/>
+        <v>-6.3411383601635896E-7</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="7"/>
+        <v>-8.1393877781408719E-2</v>
+      </c>
+      <c r="AI38">
+        <f t="shared" si="0"/>
+        <v>-6.103146659164338E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F39" s="13">
+        <v>170</v>
+      </c>
+      <c r="G39">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>31.240386486968163</v>
+      </c>
+      <c r="H39">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.5994597565006643</v>
+      </c>
+      <c r="I39">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.4735770643455908E-3</v>
+      </c>
+      <c r="J39">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>80.863442736083286</v>
+      </c>
+      <c r="K39">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>19.79495323212177</v>
+      </c>
+      <c r="L39">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.14319709862320451</v>
+      </c>
+      <c r="M39">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>176.5885578844717</v>
+      </c>
+      <c r="N39">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.1688055781510229</v>
+      </c>
+      <c r="R39" s="13">
+        <v>170</v>
+      </c>
+      <c r="S39">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>31.240386486968163</v>
+      </c>
+      <c r="T39">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.59945975645114769</v>
+      </c>
+      <c r="U39">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>4.4768688421219201E-3</v>
+      </c>
+      <c r="V39">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>80.863443460827213</v>
+      </c>
+      <c r="W39">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>19.794950167327933</v>
+      </c>
+      <c r="X39">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.14319684567580498</v>
+      </c>
+      <c r="Y39">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>176.66943027431739</v>
+      </c>
+      <c r="Z39">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-2.1687489838232725</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="2"/>
+        <v>4.9516613032096757E-11</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="3"/>
+        <v>-3.2917777763293368E-6</v>
+      </c>
+      <c r="AE39">
+        <f t="shared" si="4"/>
+        <v>-7.2474392709409585E-7</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="5"/>
+        <v>3.0647938373817851E-6</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="6"/>
+        <v>-2.5294739952608225E-7</v>
+      </c>
+      <c r="AH39">
+        <f t="shared" si="7"/>
+        <v>-8.087238984569467E-2</v>
+      </c>
+      <c r="AI39">
+        <f t="shared" si="0"/>
+        <v>-5.6594327750403295E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F40" s="13">
+        <v>180</v>
+      </c>
+      <c r="G40">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>37.448826769677652</v>
+      </c>
+      <c r="H40">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.64124009220734024</v>
+      </c>
+      <c r="I40">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.8838265936647076E-3</v>
+      </c>
+      <c r="J40">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>78.657261950931598</v>
+      </c>
+      <c r="K40">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>54.645056479785126</v>
+      </c>
+      <c r="L40">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.29140636570446077</v>
+      </c>
+      <c r="M40">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>194.85730404177559</v>
+      </c>
+      <c r="N40">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-1.6859829145232652</v>
+      </c>
+      <c r="R40" s="13">
+        <v>180</v>
+      </c>
+      <c r="S40">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>37.448826769677652</v>
+      </c>
+      <c r="T40">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.64124009219541911</v>
+      </c>
+      <c r="U40">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.8843092991744498E-3</v>
+      </c>
+      <c r="V40">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>78.657263308282623</v>
+      </c>
+      <c r="W40">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>54.645044691036254</v>
+      </c>
+      <c r="X40">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.29140679123763585</v>
+      </c>
+      <c r="Y40">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>194.93597456374454</v>
+      </c>
+      <c r="Z40">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-1.6859335592334741</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="2"/>
+        <v>1.1921130749215081E-11</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="3"/>
+        <v>-4.8270550974220672E-7</v>
+      </c>
+      <c r="AE40">
+        <f t="shared" si="4"/>
+        <v>-1.3573510244668796E-6</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="5"/>
+        <v>1.1788748871310872E-5</v>
+      </c>
+      <c r="AG40">
+        <f t="shared" si="6"/>
+        <v>4.2553317508575716E-7</v>
+      </c>
+      <c r="AH40">
+        <f t="shared" si="7"/>
+        <v>-7.8670521968945195E-2</v>
+      </c>
+      <c r="AI40">
+        <f t="shared" si="0"/>
+        <v>-4.9355289791108703E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F41" s="13">
+        <v>190</v>
+      </c>
+      <c r="G41">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>44.046032792087559</v>
+      </c>
+      <c r="H41">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.6772793124554255</v>
+      </c>
+      <c r="I41">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.3352876016579103E-3</v>
+      </c>
+      <c r="J41">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>75.165349350507185</v>
+      </c>
+      <c r="K41">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>95.780904985076631</v>
+      </c>
+      <c r="L41">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.4007052467613903</v>
+      </c>
+      <c r="M41">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>211.51740933184726</v>
+      </c>
+      <c r="N41">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-1.1155458332723356</v>
+      </c>
+      <c r="R41" s="13">
+        <v>190</v>
+      </c>
+      <c r="S41">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>44.046032792087559</v>
+      </c>
+      <c r="T41">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.6772793124339278</v>
+      </c>
+      <c r="U41">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>3.3314283158335785E-3</v>
+      </c>
+      <c r="V41">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>75.165351375995115</v>
+      </c>
+      <c r="W41">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>95.780888595578617</v>
+      </c>
+      <c r="X41">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.40070576802662339</v>
+      </c>
+      <c r="Y41">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>211.59259142589679</v>
+      </c>
+      <c r="Z41">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-1.1155056012745028</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC41">
+        <f t="shared" si="2"/>
+        <v>2.1497692515026756E-11</v>
+      </c>
+      <c r="AD41">
+        <f t="shared" si="3"/>
+        <v>3.8592858243318047E-6</v>
+      </c>
+      <c r="AE41">
+        <f t="shared" si="4"/>
+        <v>-2.0254879302683548E-6</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="5"/>
+        <v>1.6389498014746096E-5</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" si="6"/>
+        <v>5.21265233088819E-7</v>
+      </c>
+      <c r="AH41">
+        <f t="shared" si="7"/>
+        <v>-7.5182094049523585E-2</v>
+      </c>
+      <c r="AI41">
+        <f t="shared" si="0"/>
+        <v>-4.0231997832762545E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F42" s="13">
+        <v>200</v>
+      </c>
+      <c r="G42">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>50.976817270494237</v>
+      </c>
+      <c r="H42">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.70804251137701613</v>
+      </c>
+      <c r="I42">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.8308022592682391E-3</v>
+      </c>
+      <c r="J42">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>70.761619529172719</v>
+      </c>
+      <c r="K42">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>138.86481298186482</v>
+      </c>
+      <c r="L42">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.47451536033804587</v>
+      </c>
+      <c r="M42">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>226.50843155716416</v>
+      </c>
+      <c r="N42">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.47950214678849079</v>
+      </c>
+      <c r="R42" s="13">
+        <v>200</v>
+      </c>
+      <c r="S42">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>50.976817270494237</v>
+      </c>
+      <c r="T42">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>0.70804251141064367</v>
+      </c>
+      <c r="U42">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>2.8304648858819411E-3</v>
+      </c>
+      <c r="V42">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>70.761622147048541</v>
+      </c>
+      <c r="W42">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>138.86479773727993</v>
+      </c>
+      <c r="X42">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.47451514813038681</v>
+      </c>
+      <c r="Y42">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>226.57921252908628</v>
+      </c>
+      <c r="Z42">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
+        <v>-0.4794720711227729</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC42">
+        <f t="shared" si="2"/>
+        <v>-3.3627545192871366E-11</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="3"/>
+        <v>3.3737338629800245E-7</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" si="4"/>
+        <v>-2.6178758218975418E-6</v>
+      </c>
+      <c r="AF42">
+        <f t="shared" si="5"/>
+        <v>1.5244584886886514E-5</v>
+      </c>
+      <c r="AG42">
+        <f t="shared" si="6"/>
+        <v>-2.1220765905605177E-7</v>
+      </c>
+      <c r="AH42">
+        <f t="shared" si="7"/>
+        <v>-7.0780971922118852E-2</v>
+      </c>
+      <c r="AI42">
+        <f t="shared" si="0"/>
+        <v>-3.0075665717888E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="V43" s="47"/>
+      <c r="W43" s="47"/>
+      <c r="X43" s="47"/>
+      <c r="Y43" s="47"/>
+      <c r="Z43" s="47"/>
+      <c r="AA43" s="47"/>
+      <c r="AB43" s="47"/>
+    </row>
+    <row r="44" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="V44" s="47"/>
+      <c r="W44" s="47"/>
+      <c r="X44" s="47"/>
+      <c r="Y44" s="47"/>
+      <c r="Z44" s="47"/>
+      <c r="AA44" s="47"/>
+      <c r="AB44" s="47"/>
+    </row>
+    <row r="45" spans="6:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="S45" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="T45" s="48"/>
+      <c r="U45" s="48"/>
+      <c r="V45" s="48"/>
+      <c r="W45" s="48"/>
+      <c r="X45" s="48"/>
+      <c r="Y45" s="48"/>
+      <c r="Z45" s="48"/>
+      <c r="AA45" s="47"/>
+      <c r="AB45" s="47"/>
+    </row>
+    <row r="46" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>125</v>
+      </c>
+      <c r="G46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H46" t="s">
+        <v>100</v>
+      </c>
+      <c r="I46" t="s">
+        <v>101</v>
+      </c>
+      <c r="J46" t="s">
+        <v>102</v>
+      </c>
+      <c r="K46" t="s">
+        <v>103</v>
+      </c>
+      <c r="L46" t="s">
+        <v>104</v>
+      </c>
+      <c r="M46" t="s">
+        <v>105</v>
+      </c>
+      <c r="N46" t="s">
+        <v>106</v>
+      </c>
+      <c r="R46" t="s">
+        <v>125</v>
+      </c>
+      <c r="S46" t="s">
+        <v>99</v>
+      </c>
+      <c r="T46" t="s">
+        <v>100</v>
+      </c>
+      <c r="U46" t="s">
+        <v>101</v>
+      </c>
+      <c r="V46" t="s">
+        <v>102</v>
+      </c>
+      <c r="W46" t="s">
+        <v>103</v>
+      </c>
+      <c r="X46" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F47" s="13">
+        <v>100</v>
+      </c>
+      <c r="G47">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="H47">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.0000000000331966</v>
+      </c>
+      <c r="I47">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="R47" s="13">
+        <v>100</v>
+      </c>
+      <c r="S47">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>46.29908424676718</v>
+      </c>
+      <c r="T47">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.68529270708283563</v>
+      </c>
+      <c r="U47">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.1651385288094013E-3</v>
+      </c>
+      <c r="V47">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>38.532115805058758</v>
+      </c>
+      <c r="W47">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>156.14908813078776</v>
+      </c>
+      <c r="X47">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.1925600030594994</v>
+      </c>
+      <c r="Y47">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-287.0708873876269</v>
+      </c>
+      <c r="Z47">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F47,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.8513392645530935</v>
+      </c>
+    </row>
+    <row r="48" spans="6:35" x14ac:dyDescent="0.25">
+      <c r="F48" s="13">
+        <v>110</v>
+      </c>
+      <c r="G48">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>40.017066978067525</v>
+      </c>
+      <c r="H48">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.9524609334121692</v>
+      </c>
+      <c r="I48">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.3065638288244372E-2</v>
+      </c>
+      <c r="J48">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.1505904793730632</v>
+      </c>
+      <c r="K48">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>913.85448826031279</v>
+      </c>
+      <c r="L48">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.6372848672149303</v>
+      </c>
+      <c r="M48">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-3.7298693757392698</v>
+      </c>
+      <c r="N48">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.11531254486385478</v>
+      </c>
+      <c r="R48" s="13">
+        <v>110</v>
+      </c>
+      <c r="S48">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>39.764048693079118</v>
+      </c>
+      <c r="T48">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.62091153400776877</v>
+      </c>
+      <c r="U48">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.6472559788822673E-3</v>
+      </c>
+      <c r="V48">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>50.269873340297138</v>
+      </c>
+      <c r="W48">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>115.94090950324943</v>
+      </c>
+      <c r="X48">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.1356382729549774</v>
+      </c>
+      <c r="Y48">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-270.16079358483421</v>
+      </c>
+      <c r="Z48">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F48,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.12765074543010924</v>
+      </c>
+    </row>
+    <row r="49" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F49" s="13">
+        <v>120</v>
+      </c>
+      <c r="G49">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>31.551537480264027</v>
+      </c>
+      <c r="H49">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.74929179008975666</v>
+      </c>
+      <c r="I49">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.7862333834273159E-2</v>
+      </c>
+      <c r="J49">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>45.692384103355778</v>
+      </c>
+      <c r="K49">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>411.82160614994245</v>
+      </c>
+      <c r="L49">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.7926628121122121</v>
+      </c>
+      <c r="M49">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-13.778562590474053</v>
+      </c>
+      <c r="N49">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.75186854111564116</v>
+      </c>
+      <c r="R49" s="13">
+        <v>120</v>
+      </c>
+      <c r="S49">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>33.890706915205044</v>
+      </c>
+      <c r="T49">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.55355781967081308</v>
+      </c>
+      <c r="U49">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.7678048079652378E-3</v>
+      </c>
+      <c r="V49">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>60.91024327168715</v>
+      </c>
+      <c r="W49">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>68.125179693630088</v>
+      </c>
+      <c r="X49">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.97868484003505463</v>
+      </c>
+      <c r="Y49">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-250.79411318925656</v>
+      </c>
+      <c r="Z49">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F49,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.012069748672054</v>
+      </c>
+    </row>
+    <row r="50" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F50" s="13">
+        <v>130</v>
+      </c>
+      <c r="G50">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>24.882702630293402</v>
+      </c>
+      <c r="H50">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.59088314507960149</v>
+      </c>
+      <c r="I50">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.4009060578246135E-2</v>
+      </c>
+      <c r="J50">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>66.9671715357441</v>
+      </c>
+      <c r="K50">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>158.0445029958355</v>
+      </c>
+      <c r="L50">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.5418802234989926</v>
+      </c>
+      <c r="M50">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-17.565620957640249</v>
+      </c>
+      <c r="N50">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.2608148363568716</v>
+      </c>
+      <c r="R50" s="13">
+        <v>130</v>
+      </c>
+      <c r="S50">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>28.691673290913748</v>
+      </c>
+      <c r="T50">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.48654353918606291</v>
+      </c>
+      <c r="U50">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.5924254948707267E-3</v>
+      </c>
+      <c r="V50">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>69.632494289572065</v>
+      </c>
+      <c r="W50">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>25.62357394681667</v>
+      </c>
+      <c r="X50">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.75837574370535099</v>
+      </c>
+      <c r="Y50">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-229.85583346275484</v>
+      </c>
+      <c r="Z50">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F50,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.7601243170237777</v>
+      </c>
+    </row>
+    <row r="51" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F51" s="13">
+        <v>140</v>
+      </c>
+      <c r="G51">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>19.621669271250902</v>
+      </c>
+      <c r="H51">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.46624407396222978</v>
+      </c>
+      <c r="I51">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>1.1033307600882836E-2</v>
+      </c>
+      <c r="J51">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>77.851720028343195</v>
+      </c>
+      <c r="K51">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>52.171603215356299</v>
+      </c>
+      <c r="L51">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.68997323410258105</v>
+      </c>
+      <c r="M51">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-18.074536261352137</v>
+      </c>
+      <c r="N51">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.6248623295211928</v>
+      </c>
+      <c r="R51" s="13">
+        <v>140</v>
+      </c>
+      <c r="S51">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>24.150101391345359</v>
+      </c>
+      <c r="T51">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.42242186843532148</v>
+      </c>
+      <c r="U51">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.2031451884485686E-3</v>
+      </c>
+      <c r="V51">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>75.988528558494963</v>
+      </c>
+      <c r="W51">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-2.6135177115936088</v>
+      </c>
+      <c r="X51">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.51105236932348352</v>
+      </c>
+      <c r="Y51">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-208.22290743072591</v>
+      </c>
+      <c r="Z51">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F51,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-2.3504203444440268</v>
+      </c>
+    </row>
+    <row r="52" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F52" s="13">
+        <v>150</v>
+      </c>
+      <c r="G52">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>15.470727171446882</v>
+      </c>
+      <c r="H52">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.3677971641025124</v>
+      </c>
+      <c r="I52">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>8.7339913079631515E-3</v>
+      </c>
+      <c r="J52">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>81.694007672874605</v>
+      </c>
+      <c r="K52">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>32.489069212715549</v>
+      </c>
+      <c r="L52">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.11754330841995397</v>
+      </c>
+      <c r="M52">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-16.959207043711899</v>
+      </c>
+      <c r="N52">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.851405528725536</v>
+      </c>
+      <c r="R52" s="13">
+        <v>150</v>
+      </c>
+      <c r="S52">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>20.227726902988501</v>
+      </c>
+      <c r="T52">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.3629282318692339</v>
+      </c>
+      <c r="U52">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.6791365019068672E-3</v>
+      </c>
+      <c r="V52">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>79.86285705806533</v>
+      </c>
+      <c r="W52">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-12.478571415322708</v>
+      </c>
+      <c r="X52">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>0.26620952352688443</v>
+      </c>
+      <c r="Y52">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-186.66740420843396</v>
+      </c>
+      <c r="Z52">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F52,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-2.7794792387239551</v>
+      </c>
+    </row>
+    <row r="53" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F53" s="13">
+        <v>160</v>
+      </c>
+      <c r="G53">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>12.197163796635536</v>
+      </c>
+      <c r="H53">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.28996089064037278</v>
+      </c>
+      <c r="I53">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>6.9050543061166536E-3</v>
+      </c>
+      <c r="J53">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>80.866097236773655</v>
+      </c>
+      <c r="K53">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>59.706425759031845</v>
+      </c>
+      <c r="L53">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.25508093415282929</v>
+      </c>
+      <c r="M53">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-15.134372397156426</v>
+      </c>
+      <c r="N53">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.9602662409567984</v>
+      </c>
+      <c r="R53" s="13">
+        <v>160</v>
+      </c>
+      <c r="S53">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>16.872704084983141</v>
+      </c>
+      <c r="T53">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.30906484332811646</v>
+      </c>
+      <c r="U53">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.0868699934212263E-3</v>
+      </c>
+      <c r="V53">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>81.389919894739634</v>
+      </c>
+      <c r="W53">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-4.0385962960226589</v>
+      </c>
+      <c r="X53">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.4232097050586193E-2</v>
+      </c>
+      <c r="Y53">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-165.80769754370445</v>
+      </c>
+      <c r="Z53">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F53,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-3.0571337496379924</v>
+      </c>
+    </row>
+    <row r="54" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F54" s="13">
+        <v>170</v>
+      </c>
+      <c r="G54">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.6171978371390026</v>
+      </c>
+      <c r="H54">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.22844808022171037</v>
+      </c>
+      <c r="I54">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.4527049542230088E-3</v>
+      </c>
+      <c r="J54">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>77.068352341464632</v>
+      </c>
+      <c r="K54">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>108.64413013678131</v>
+      </c>
+      <c r="L54">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.48441464173265558</v>
+      </c>
+      <c r="M54">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-13.097309789600331</v>
+      </c>
+      <c r="N54">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.9757614813897817</v>
+      </c>
+      <c r="R54" s="13">
+        <v>170</v>
+      </c>
+      <c r="S54">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>14.026226958466978</v>
+      </c>
+      <c r="T54">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.26124821997391018</v>
+      </c>
+      <c r="U54">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.4768688421219201E-3</v>
+      </c>
+      <c r="V54">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>80.863443460827213</v>
+      </c>
+      <c r="W54">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>19.794950167327933</v>
+      </c>
+      <c r="X54">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.14319684567580498</v>
+      </c>
+      <c r="Y54">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-146.09606088507928</v>
+      </c>
+      <c r="Z54">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F54,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-3.2015985555333408</v>
+      </c>
+    </row>
+    <row r="55" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F55" s="13">
+        <v>180</v>
+      </c>
+      <c r="G55">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.5851013072030753</v>
+      </c>
+      <c r="H55">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.17988830094850528</v>
+      </c>
+      <c r="I55">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.3172576624783687E-3</v>
+      </c>
+      <c r="J55">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>71.516035002482482</v>
+      </c>
+      <c r="K55">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>163.50398652775766</v>
+      </c>
+      <c r="L55">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.61191869349386252</v>
+      </c>
+      <c r="M55">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-11.107712442992579</v>
+      </c>
+      <c r="N55">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.922011885540087</v>
+      </c>
+      <c r="R55" s="13">
+        <v>180</v>
+      </c>
+      <c r="S55">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>11.62758747692591</v>
+      </c>
+      <c r="T55">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.21946788422963862</v>
+      </c>
+      <c r="U55">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.8843092991744498E-3</v>
+      </c>
+      <c r="V55">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>78.657263308282623</v>
+      </c>
+      <c r="W55">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>54.645044691036254</v>
+      </c>
+      <c r="X55">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.29140679123763585</v>
+      </c>
+      <c r="Y55">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-127.82951659565217</v>
+      </c>
+      <c r="Z55">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F55,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-3.2352079167985752</v>
+      </c>
+    </row>
+    <row r="56" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F56" s="13">
+        <v>190</v>
+      </c>
+      <c r="G56">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>5.9852452016453697</v>
+      </c>
+      <c r="H56">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.14160239913962869</v>
+      </c>
+      <c r="I56">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.3821834222180769E-3</v>
+      </c>
+      <c r="J56">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>65.065637175372672</v>
+      </c>
+      <c r="K56">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>214.88167192273977</v>
+      </c>
+      <c r="L56">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.66844592083725729</v>
+      </c>
+      <c r="M56">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-9.2903124588872288</v>
+      </c>
+      <c r="N56">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.8204827898671283</v>
+      </c>
+      <c r="R56" s="13">
+        <v>190</v>
+      </c>
+      <c r="S56">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>9.6177137350852462</v>
+      </c>
+      <c r="T56">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.18342866399112998</v>
+      </c>
+      <c r="U56">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>3.3314283158335785E-3</v>
+      </c>
+      <c r="V56">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>75.165351375995115</v>
+      </c>
+      <c r="W56">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>95.780888595578617</v>
+      </c>
+      <c r="X56">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.40070576802662339</v>
+      </c>
+      <c r="Y56">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-111.17289973349986</v>
+      </c>
+      <c r="Z56">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F56,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-3.1812047446946408</v>
+      </c>
+    </row>
+    <row r="57" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F57" s="13">
+        <v>200</v>
+      </c>
+      <c r="G57">
+        <f>_xll.acq_options_bjerksund_greeks(G$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>4.7259808316812553</v>
+      </c>
+      <c r="H57">
+        <f>_xll.acq_options_bjerksund_greeks(H$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.11145255484734662</v>
+      </c>
+      <c r="I57">
+        <f>_xll.acq_options_bjerksund_greeks(I$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.6659563445718959E-3</v>
+      </c>
+      <c r="J57">
+        <f>_xll.acq_options_bjerksund_greeks(J$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>58.306669315164356</v>
+      </c>
+      <c r="K57">
+        <f>_xll.acq_options_bjerksund_greeks(K$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>257.72598917228606</v>
+      </c>
+      <c r="L57">
+        <f>_xll.acq_options_bjerksund_greeks(L$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.67690351102100976</v>
+      </c>
+      <c r="M57">
+        <f>_xll.acq_options_bjerksund_greeks(M$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-7.6942194169760114</v>
+      </c>
+      <c r="N57">
+        <f>_xll.acq_options_bjerksund_greeks(N$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-1.6889631692151852</v>
+      </c>
+      <c r="R57" s="13">
+        <v>200</v>
+      </c>
+      <c r="S57">
+        <f>_xll.acq_options_blackscholes_greeks(S$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>7.9414184492413362</v>
+      </c>
+      <c r="T57">
+        <f>_xll.acq_options_blackscholes_greeks(T$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.15266546501441408</v>
+      </c>
+      <c r="U57">
+        <f>_xll.acq_options_blackscholes_greeks(U$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>2.8304648858819411E-3</v>
+      </c>
+      <c r="V57">
+        <f>_xll.acq_options_blackscholes_greeks(V$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>70.761622147048541</v>
+      </c>
+      <c r="W57">
+        <f>_xll.acq_options_blackscholes_greeks(W$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>138.86479773727993</v>
+      </c>
+      <c r="X57">
+        <f>_xll.acq_options_blackscholes_greeks(X$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-0.47451514813038681</v>
+      </c>
+      <c r="Y57">
+        <f>_xll.acq_options_blackscholes_greeks(Y$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-96.186278630310397</v>
+      </c>
+      <c r="Z57">
+        <f>_xll.acq_options_blackscholes_greeks(Z$31,$F57,$C$5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
+        <v>-3.0615960003979468</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="G45:N45"/>
+    <mergeCell ref="S45:Z45"/>
+    <mergeCell ref="S30:Z30"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="G30:N30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" xr:uid="{69E1F7C3-E9DE-4863-9FC4-322489C91572}"/>

</xml_diff>

<commit_message>
commended out individual option greek functions
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31BF5AE-1871-4388-8DBB-0FAA2192299F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BFFC55-3F41-4F14-8DAC-A269988898E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="152">
   <si>
     <t>x</t>
   </si>
@@ -640,6 +640,12 @@
   <si>
     <t>Put Greeks: Bjerksund Stensland Numerical Greeks</t>
   </si>
+  <si>
+    <t>Next Business Day</t>
+  </si>
+  <si>
+    <t>Adjust to Business Day</t>
+  </si>
 </sst>
 </file>
 
@@ -733,7 +739,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +782,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1022,7 +1034,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="1" fillId="7" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1060,6 +1071,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
@@ -10303,7 +10315,7 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8023.37862</v>
+        <v>1.3.8024.36739</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -10379,12 +10391,18 @@
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="C20" s="4">
         <f>_xll.acq_nextbusinessday(C19)</f>
         <v>42186</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="C21" s="4">
         <f>_xll.acq_adjustbusinessday(C19,-1)</f>
         <v>42185</v>
@@ -10402,7 +10420,7 @@
   <dimension ref="A1:AQ43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="AH43" sqref="AH43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10417,37 +10435,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="L2" s="48" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="S2" s="48" t="s">
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="S2" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -10696,15 +10714,15 @@
         <v>89.999899999999997</v>
       </c>
       <c r="AC5" s="13">
-        <f>_xll.acq_options_black_price($AB5,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AC$3,$AB5,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>15.519036627414497</v>
       </c>
       <c r="AD5" s="13">
-        <f>_xll.acq_options_black_delta($AB5,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AD$3,$AB5,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>-0.50257071403175657</v>
       </c>
       <c r="AE5" s="13">
-        <f>_xll.acq_options_black_gamma($AB5,$C$5,$C$6,$C$8,$C$7)</f>
+        <f>_xll.acq_options_black_greeks(AE$3,$AB5,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>1.2182203831523738E-2</v>
       </c>
       <c r="AF5" s="11"/>
@@ -10799,16 +10817,16 @@
         <f>C4</f>
         <v>90</v>
       </c>
-      <c r="AC6" s="18">
-        <f>_xll.acq_options_black_price($AB6,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
+      <c r="AC6" s="13">
+        <f>_xll.acq_options_black_greeks(AC$3,$AB6,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>15.518986370404006</v>
       </c>
-      <c r="AD6" s="18">
-        <f>_xll.acq_options_black_delta($AB6,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
+      <c r="AD6" s="13">
+        <f>_xll.acq_options_black_greeks(AD$3,$AB6,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>-0.50256949581167554</v>
       </c>
-      <c r="AE6" s="18">
-        <f>_xll.acq_options_black_gamma($AB6,$C$5,$C$6,$C$8,$C$7)</f>
+      <c r="AE6" s="13">
+        <f>_xll.acq_options_black_greeks(AE$3,$AB6,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>1.2182197789293775E-2</v>
       </c>
       <c r="AF6" s="11"/>
@@ -10898,15 +10916,15 @@
         <v>90.000100000000003</v>
       </c>
       <c r="AC7" s="13">
-        <f>_xll.acq_options_black_price($AB7,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AC$3,$AB7,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>15.518936113515325</v>
       </c>
       <c r="AD7" s="13">
-        <f>_xll.acq_options_black_delta($AB7,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AD$3,$AB7,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>-0.50256827759219869</v>
       </c>
       <c r="AE7" s="13">
-        <f>_xll.acq_options_black_gamma($AB7,$C$5,$C$6,$C$8,$C$7)</f>
+        <f>_xll.acq_options_black_greeks(AE$3,$AB7,$C$5,$C$6,$C$8,$C$7,$C$9)</f>
         <v>1.2182191746923128E-2</v>
       </c>
       <c r="AH7" s="11"/>
@@ -11166,15 +11184,15 @@
       <c r="AB10" t="s">
         <v>111</v>
       </c>
-      <c r="AD10" s="36">
+      <c r="AD10" s="35">
         <f>AD6-AD9</f>
         <v>3.1002755918052571E-11</v>
       </c>
-      <c r="AE10" s="36">
+      <c r="AE10" s="35">
         <f>AE6-AE9</f>
         <v>1.186034878804948E-6</v>
       </c>
-      <c r="AF10" s="36">
+      <c r="AF10" s="35">
         <f>AE6-AF9</f>
         <v>2.7498316124141553E-13</v>
       </c>
@@ -11258,18 +11276,18 @@
       <c r="AI11" s="11"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="F12">
+      <c r="F12" s="49">
         <v>90</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="49">
         <f>_xll.acq_options_black_price($C$4,F12,$C$6,$C$8,$C$7,TRUE)</f>
         <v>9.9783611447713145</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="49">
         <f>_xll.acq_options_black_price($C$4,F12,$C$6,$C$8,$C$7,FALSE)</f>
         <v>9.9783611447713145</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -11573,17 +11591,17 @@
         <f>AB17-AC20</f>
         <v>0.19990000000000002</v>
       </c>
-      <c r="AC16">
-        <f>_xll.acq_options_black_price($C$4,$C$5,$C$6,$C$8,AB16,C9)</f>
+      <c r="AC16" s="13">
+        <f>_xll.acq_options_black_greeks(AC$14,$C$4,$C$5,$C$6,$C$8,$AB16)</f>
         <v>15.514052686458282</v>
       </c>
       <c r="AD16" s="13">
-        <f>_xll.acq_options_black_vega($C$4,$C$5,$C$6,$C$8,AB16)</f>
+        <f>_xll.acq_options_black_greeks(AD$14,$C$4,$C$5,$C$6,$C$8,$AB16)</f>
         <v>49.335777146424881</v>
       </c>
       <c r="AE16" s="13">
-        <f>_xll.acq_options_black_vomma($C$4,$C$5,$C$6,$C$8,AB16)</f>
-        <v>21.26065171426006</v>
+        <f>_xll.acq_options_black_greeks(AE$14,$C$4,$C$5,$C$6,$C$8,AC16)</f>
+        <v>-1.1070078009949605E-30</v>
       </c>
       <c r="AF16" s="11"/>
     </row>
@@ -11622,30 +11640,30 @@
         <f>_xll.acq_options_black_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>0.65000000000000013</v>
       </c>
-      <c r="S17" s="48" t="s">
+      <c r="S17" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="48"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
-      <c r="X17" s="48"/>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="48"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>0.2</v>
       </c>
-      <c r="AC17" s="19">
-        <f>_xll.acq_options_black_price($C$4,$C$5,$C$6,$C$8,AB17,C9)</f>
+      <c r="AC17" s="13">
+        <f>_xll.acq_options_black_greeks(AC$14,$C$4,$C$5,$C$6,$C$8,$AB17)</f>
         <v>15.518986370404006</v>
       </c>
-      <c r="AD17" s="18">
-        <f>_xll.acq_options_black_vega($C$4,$C$5,$C$6,$C$8,AB17)</f>
+      <c r="AD17" s="13">
+        <f>_xll.acq_options_black_greeks(AD$14,$C$4,$C$5,$C$6,$C$8,$AB17)</f>
         <v>49.3379010466398</v>
       </c>
-      <c r="AE17" s="18">
-        <f>_xll.acq_options_black_vomma($C$4,$C$5,$C$6,$C$8,AB17)</f>
+      <c r="AE17" s="13">
+        <f>_xll.acq_options_black_greeks(AE$14,$C$4,$C$5,$C$6,$C$8,$AB17)</f>
         <v>21.217365348719802</v>
       </c>
       <c r="AF17" s="11"/>
@@ -11716,16 +11734,16 @@
         <f>AB17+AC20</f>
         <v>0.2001</v>
       </c>
-      <c r="AC18">
-        <f>_xll.acq_options_black_price($C$4,$C$5,$C$6,$C$8,AB18,C9)</f>
+      <c r="AC18" s="13">
+        <f>_xll.acq_options_black_greeks(AC$14,$C$4,$C$5,$C$6,$C$8,$AB18)</f>
         <v>15.523920266523435</v>
       </c>
       <c r="AD18" s="13">
-        <f>_xll.acq_options_black_vega($C$4,$C$5,$C$6,$C$8,AB18)</f>
+        <f>_xll.acq_options_black_greeks(AD$14,$C$4,$C$5,$C$6,$C$8,$AB18)</f>
         <v>49.340020622044484</v>
       </c>
       <c r="AE18" s="13">
-        <f>_xll.acq_options_black_vomma($C$4,$C$5,$C$6,$C$8,AB18)</f>
+        <f>_xll.acq_options_black_greeks(AE$14,$C$4,$C$5,$C$6,$C$8,$AB18)</f>
         <v>21.174155479006156</v>
       </c>
       <c r="AH18" s="11"/>
@@ -11958,15 +11976,15 @@
       <c r="AB21" t="s">
         <v>111</v>
       </c>
-      <c r="AD21" s="36">
+      <c r="AD21" s="35">
         <f>AD17-AD20</f>
         <v>7.2086890412492721E-7</v>
       </c>
-      <c r="AE21" s="36">
+      <c r="AE21" s="35">
         <f>AE17-AE20</f>
         <v>-5.0896470042971487E-6</v>
       </c>
-      <c r="AF21" s="36">
+      <c r="AF21" s="35">
         <f>AE17-AF20</f>
         <v>-1.2749297695791029E-5</v>
       </c>
@@ -12334,12 +12352,12 @@
         <f>AB28-AC31</f>
         <v>4.99E-2</v>
       </c>
-      <c r="AC27">
-        <f>_xll.acq_options_black_price($C$4,$C$5,$C$6,AB27,$C$7,$C$20)</f>
+      <c r="AC27" s="13">
+        <f>_xll.acq_options_black_greeks(AC$25,$C$4,$C$5,$C$6,$AB27,$C$7,$C$9)</f>
         <v>15.522866602005347</v>
       </c>
       <c r="AD27" s="13">
-        <f>_xll.acq_options_black_rho($C$4,$C$5,$C$6,AB27,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AD$25,$C$4,$C$5,$C$6,$AB27,$C$7,$C$9)</f>
         <v>-38.80716650501337</v>
       </c>
       <c r="AE27" s="13"/>
@@ -12347,12 +12365,12 @@
         <f>AF28-AG31</f>
         <v>2.4998999999999998</v>
       </c>
-      <c r="AG27">
-        <f>_xll.acq_options_black_price($C$4,$C$5,AF27,$C$8,$C$7,$C$20)</f>
+      <c r="AG27" s="13">
+        <f>_xll.acq_options_black_greeks(AG$25,$C$4,$C$5,$AF27,$C$8,$C$7,$C$9)</f>
         <v>15.518866611135088</v>
       </c>
       <c r="AH27" s="13">
-        <f>_xll.acq_options_black_theta($C$4,$C$5,AF27,$C$8,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AH$25,$C$4,$C$5,$AF27,$C$8,$C$7,$C$9)</f>
         <v>-1.1976186555803805</v>
       </c>
     </row>
@@ -12396,12 +12414,12 @@
         <f>C8</f>
         <v>0.05</v>
       </c>
-      <c r="AC28" s="19">
-        <f>_xll.acq_options_black_price($C$4,$C$5,$C$6,AB28,$C$7,$C$20)</f>
+      <c r="AC28" s="13">
+        <f>_xll.acq_options_black_greeks(AC$25,$C$4,$C$5,$C$6,$AB28,$C$7,$C$9)</f>
         <v>15.518986370404006</v>
       </c>
-      <c r="AD28" s="18">
-        <f>_xll.acq_options_black_rho($C$4,$C$5,$C$6,AB28,$C$7,$C$9)</f>
+      <c r="AD28" s="13">
+        <f>_xll.acq_options_black_greeks(AD$25,$C$4,$C$5,$C$6,$AB28,$C$7,$C$9)</f>
         <v>-38.797465926010013</v>
       </c>
       <c r="AE28" s="13"/>
@@ -12409,12 +12427,12 @@
         <f>C6</f>
         <v>2.5</v>
       </c>
-      <c r="AG28">
-        <f>_xll.acq_options_black_price($C$4,$C$5,AF28,$C$8,$C$7,$C$20)</f>
+      <c r="AG28" s="13">
+        <f>_xll.acq_options_black_greeks(AG$25,$C$4,$C$5,$AF28,$C$8,$C$7,$C$9)</f>
         <v>15.518986370404006</v>
       </c>
       <c r="AH28" s="13">
-        <f>_xll.acq_options_black_theta($C$4,$C$5,AF28,$C$8,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AH$25,$C$4,$C$5,$AF28,$C$8,$C$7,$C$9)</f>
         <v>-1.1975667233453915</v>
       </c>
     </row>
@@ -12458,12 +12476,12 @@
         <f>AB28+AC31</f>
         <v>5.0100000000000006E-2</v>
       </c>
-      <c r="AC29">
-        <f>_xll.acq_options_black_price($C$4,$C$5,$C$6,AB29,$C$7,$C$20)</f>
+      <c r="AC29" s="13">
+        <f>_xll.acq_options_black_greeks(AC$25,$C$4,$C$5,$C$6,$AB29,$C$7,$C$9)</f>
         <v>15.515107108739317</v>
       </c>
       <c r="AD29" s="13">
-        <f>_xll.acq_options_black_rho($C$4,$C$5,$C$6,AB29,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AD$25,$C$4,$C$5,$C$6,$AB29,$C$7,$C$9)</f>
         <v>-38.787767771848287</v>
       </c>
       <c r="AE29" s="13"/>
@@ -12471,12 +12489,12 @@
         <f>AF28+AG31</f>
         <v>2.5001000000000002</v>
       </c>
-      <c r="AG29">
-        <f>_xll.acq_options_black_price($C$4,$C$5,AF29,$C$8,$C$7,$C$20)</f>
+      <c r="AG29" s="13">
+        <f>_xll.acq_options_black_greeks(AG$25,$C$4,$C$5,$AF29,$C$8,$C$7,$C$9)</f>
         <v>15.519106124479837</v>
       </c>
       <c r="AH29" s="13">
-        <f>_xll.acq_options_black_theta($C$4,$C$5,AF29,$C$8,$C$7,$C$9)</f>
+        <f>_xll.acq_options_black_greeks(AH$25,$C$4,$C$5,$AF29,$C$8,$C$7,$C$9)</f>
         <v>-1.197514793667896</v>
       </c>
     </row>
@@ -12511,7 +12529,7 @@
       <c r="AB32" t="s">
         <v>111</v>
       </c>
-      <c r="AD32" s="36">
+      <c r="AD32" s="35">
         <f>AD28-AD31</f>
         <v>4.0414267488131372E-7</v>
       </c>
@@ -12519,7 +12537,7 @@
       <c r="AF32" t="s">
         <v>111</v>
       </c>
-      <c r="AH32" s="36">
+      <c r="AH32" s="35">
         <f>AH28-AH31</f>
         <v>3.9501890647386517E-10</v>
       </c>
@@ -12562,184 +12580,184 @@
     </row>
     <row r="37" spans="18:43" x14ac:dyDescent="0.25">
       <c r="T37" s="12"/>
-      <c r="AB37" s="29" t="s">
+      <c r="AB37" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="AC37" s="30">
+      <c r="AC37" s="29">
         <f>AD37-AC42</f>
         <v>0.19990000000000002</v>
       </c>
-      <c r="AD37" s="31">
+      <c r="AD37" s="30">
         <f>C7</f>
         <v>0.2</v>
       </c>
-      <c r="AE37" s="32">
+      <c r="AE37" s="31">
         <f>AD37+AC42</f>
         <v>0.2001</v>
       </c>
     </row>
     <row r="38" spans="18:43" x14ac:dyDescent="0.25">
       <c r="T38" s="12"/>
-      <c r="AB38" s="26">
+      <c r="AB38" s="25">
         <f>AB39-AC42</f>
         <v>89.999899999999997</v>
       </c>
-      <c r="AC38" s="20">
+      <c r="AC38" s="19">
         <f>_xll.acq_options_black_price($AB38,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>15.514102951988354</v>
       </c>
-      <c r="AD38" s="21">
+      <c r="AD38" s="20">
         <f>_xll.acq_options_black_price($AB38,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>15.519036627414497</v>
       </c>
-      <c r="AE38" s="33">
+      <c r="AE38" s="32">
         <f>_xll.acq_options_black_price($AB38,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>15.523970515019768</v>
       </c>
       <c r="AG38">
-        <f>_xll.acq_options_black_delta($AB38,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
+        <f>_xll.acq_options_black_greeks($AG$36,$AB38,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>-0.50265591011290189</v>
       </c>
       <c r="AH38">
-        <f>_xll.acq_options_black_delta($AB38,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
+        <f>_xll.acq_options_black_greeks($AG$36,$AB38,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>-0.50257071403175657</v>
       </c>
       <c r="AI38">
-        <f>_xll.acq_options_black_delta($AB38,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
+        <f>_xll.acq_options_black_greeks($AG$36,$AB38,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>-0.50248557204699029</v>
       </c>
       <c r="AK38">
-        <f>_xll.acq_options_black_vega($AB38,$C$5,$C$6,$C$8,AC$37)</f>
+        <f>_xll.acq_options_black_greeks($AK$36,$AB38,$C$5,$C$6,$C$8,AC$37)</f>
         <v>49.335691923549369</v>
       </c>
-      <c r="AL38" s="19">
-        <f>_xll.acq_options_black_vega($AB38,$C$5,$C$6,$C$8,AD$37)</f>
+      <c r="AL38">
+        <f>_xll.acq_options_black_greeks($AK$36,$AB38,$C$5,$C$6,$C$8,AD$37)</f>
         <v>49.337815877897569</v>
       </c>
       <c r="AM38">
-        <f>_xll.acq_options_black_vega($AB38,$C$5,$C$6,$C$8,AE$37)</f>
+        <f>_xll.acq_options_black_greeks($AK$36,$AB38,$C$5,$C$6,$C$8,AE$37)</f>
         <v>49.339935507361311</v>
       </c>
       <c r="AO38">
-        <f>_xll.acq_options_black_vanna($AB38,$C$5,$C$6,$C$8,AC$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB38,$C$5,$C$6,$C$8,AC$37)</f>
         <v>0.8522315408095249</v>
       </c>
       <c r="AP38">
-        <f>_xll.acq_options_black_vanna($AB38,$C$5,$C$6,$C$8,AD$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB38,$C$5,$C$6,$C$8,AD$37)</f>
         <v>0.8516902058832212</v>
       </c>
       <c r="AQ38">
-        <f>_xll.acq_options_black_vanna($AB38,$C$5,$C$6,$C$8,AE$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB38,$C$5,$C$6,$C$8,AE$37)</f>
         <v>0.85114961300657732</v>
       </c>
     </row>
     <row r="39" spans="18:43" x14ac:dyDescent="0.25">
       <c r="T39" s="12"/>
-      <c r="AB39" s="27">
+      <c r="AB39" s="26">
         <f>C4</f>
         <v>90</v>
       </c>
-      <c r="AC39" s="34">
+      <c r="AC39" s="33">
         <f>_xll.acq_options_black_price($AB39,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>15.514052686458282</v>
       </c>
-      <c r="AD39" s="22">
+      <c r="AD39" s="21">
         <f>_xll.acq_options_black_price($AB39,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>15.518986370404006</v>
       </c>
-      <c r="AE39" s="23">
+      <c r="AE39" s="22">
         <f>_xll.acq_options_black_price($AB39,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>15.523920266523435</v>
       </c>
-      <c r="AG39" s="19">
-        <f>_xll.acq_options_black_delta($AB39,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
+      <c r="AG39">
+        <f>_xll.acq_options_black_greeks($AG$36,$AB39,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>-0.50265469133587493</v>
       </c>
-      <c r="AH39" s="19">
-        <f>_xll.acq_options_black_delta($AB39,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
+      <c r="AH39">
+        <f>_xll.acq_options_black_greeks($AG$36,$AB39,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>-0.50256949581167554</v>
       </c>
-      <c r="AI39" s="19">
-        <f>_xll.acq_options_black_delta($AB39,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
+      <c r="AI39">
+        <f>_xll.acq_options_black_greeks($AG$36,$AB39,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>-0.50248435438340511</v>
       </c>
       <c r="AK39">
-        <f>_xll.acq_options_black_vega($AB39,$C$5,$C$6,$C$8,AC$37)</f>
+        <f>_xll.acq_options_black_greeks($AK$36,$AB39,$C$5,$C$6,$C$8,AC$37)</f>
         <v>49.335777146424881</v>
       </c>
-      <c r="AL39" s="19">
-        <f>_xll.acq_options_black_vega($AB39,$C$5,$C$6,$C$8,AD$37)</f>
+      <c r="AL39">
+        <f>_xll.acq_options_black_greeks($AK$36,$AB39,$C$5,$C$6,$C$8,AD$37)</f>
         <v>49.3379010466398</v>
       </c>
       <c r="AM39">
-        <f>_xll.acq_options_black_vega($AB39,$C$5,$C$6,$C$8,AE$37)</f>
+        <f>_xll.acq_options_black_greeks($AK$36,$AB39,$C$5,$C$6,$C$8,AE$37)</f>
         <v>49.340020622044484</v>
       </c>
       <c r="AO39">
-        <f>_xll.acq_options_black_vanna($AB39,$C$5,$C$6,$C$8,AC$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB39,$C$5,$C$6,$C$8,AC$37)</f>
         <v>0.85222596910017023</v>
       </c>
-      <c r="AP39" s="19">
-        <f>_xll.acq_options_black_vanna($AB39,$C$5,$C$6,$C$8,AD$37)</f>
+      <c r="AP39">
+        <f>_xll.acq_options_black_greeks($AO$36,$AB39,$C$5,$C$6,$C$8,AD$37)</f>
         <v>0.85168463867564059</v>
       </c>
       <c r="AQ39">
-        <f>_xll.acq_options_black_vanna($AB39,$C$5,$C$6,$C$8,AE$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB39,$C$5,$C$6,$C$8,AE$37)</f>
         <v>0.85114405029591067</v>
       </c>
     </row>
     <row r="40" spans="18:43" x14ac:dyDescent="0.25">
       <c r="T40" s="12"/>
-      <c r="AB40" s="28">
+      <c r="AB40" s="27">
         <f>AB39+AC42</f>
         <v>90.000100000000003</v>
       </c>
-      <c r="AC40" s="35">
+      <c r="AC40" s="34">
         <f>_xll.acq_options_black_price($AB40,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>15.514002421050082</v>
       </c>
-      <c r="AD40" s="24">
+      <c r="AD40" s="23">
         <f>_xll.acq_options_black_price($AB40,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>15.518936113515325</v>
       </c>
-      <c r="AE40" s="25">
+      <c r="AE40" s="24">
         <f>_xll.acq_options_black_price($AB40,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>15.523870018148884</v>
       </c>
       <c r="AG40">
-        <f>_xll.acq_options_black_delta($AB40,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
+        <f>_xll.acq_options_black_greeks($AG$36,$AB40,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>-0.50265347255945125</v>
       </c>
       <c r="AH40">
-        <f>_xll.acq_options_black_delta($AB40,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
+        <f>_xll.acq_options_black_greeks($AG$36,$AB40,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>-0.50256827759219869</v>
       </c>
       <c r="AI40">
-        <f>_xll.acq_options_black_delta($AB40,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
+        <f>_xll.acq_options_black_greeks($AG$36,$AB40,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>-0.50248313672042533</v>
       </c>
       <c r="AK40">
-        <f>_xll.acq_options_black_vega($AB40,$C$5,$C$6,$C$8,AC$37)</f>
+        <f>_xll.acq_options_black_greeks($AK$36,$AB40,$C$5,$C$6,$C$8,AC$37)</f>
         <v>49.3358623687432</v>
       </c>
-      <c r="AL40" s="19">
-        <f>_xll.acq_options_black_vega($AB40,$C$5,$C$6,$C$8,AD$37)</f>
+      <c r="AL40">
+        <f>_xll.acq_options_black_greeks($AK$36,$AB40,$C$5,$C$6,$C$8,AD$37)</f>
         <v>49.337986214825321</v>
       </c>
       <c r="AM40">
-        <f>_xll.acq_options_black_vega($AB40,$C$5,$C$6,$C$8,AE$37)</f>
+        <f>_xll.acq_options_black_greeks($AK$36,$AB40,$C$5,$C$6,$C$8,AE$37)</f>
         <v>49.340105736171374</v>
       </c>
       <c r="AO40">
-        <f>_xll.acq_options_black_vanna($AB40,$C$5,$C$6,$C$8,AC$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB40,$C$5,$C$6,$C$8,AC$37)</f>
         <v>0.85222039737928323</v>
       </c>
       <c r="AP40">
-        <f>_xll.acq_options_black_vanna($AB40,$C$5,$C$6,$C$8,AD$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB40,$C$5,$C$6,$C$8,AD$37)</f>
         <v>0.85167907145655986</v>
       </c>
       <c r="AQ40">
-        <f>_xll.acq_options_black_vanna($AB40,$C$5,$C$6,$C$8,AE$37)</f>
+        <f>_xll.acq_options_black_greeks($AO$36,$AB40,$C$5,$C$6,$C$8,AE$37)</f>
         <v>0.85113848757377619</v>
       </c>
     </row>
@@ -12767,11 +12785,11 @@
       <c r="AB43" t="s">
         <v>111</v>
       </c>
-      <c r="AD43" s="36">
+      <c r="AD43" s="35">
         <f>AP39-AD42</f>
         <v>-1.2367354518261209E-7</v>
       </c>
-      <c r="AE43" s="36">
+      <c r="AE43" s="35">
         <f>AP39-AE42</f>
         <v>-5.6816662485914549E-11</v>
       </c>
@@ -12796,8 +12814,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AQ44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView topLeftCell="P16" workbookViewId="0">
+      <selection activeCell="AJ34" sqref="AJ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12812,37 +12830,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="L2" s="48" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="S2" s="48" t="s">
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="S2" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -13561,15 +13579,15 @@
       <c r="AB10" t="s">
         <v>111</v>
       </c>
-      <c r="AD10" s="36">
+      <c r="AD10" s="35">
         <f>AD6-AD9</f>
         <v>-7.0438099797343057E-13</v>
       </c>
-      <c r="AE10" s="36">
+      <c r="AE10" s="35">
         <f>AE6-AE9</f>
         <v>2.2344919848454881E-8</v>
       </c>
-      <c r="AF10" s="36">
+      <c r="AF10" s="35">
         <f>AE6-AF9</f>
         <v>2.9370082754720528E-13</v>
       </c>
@@ -14017,16 +14035,16 @@
         <f>_xll.acq_options_bachelier_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>25.999999999962554</v>
       </c>
-      <c r="S17" s="48" t="s">
+      <c r="S17" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="48"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
-      <c r="X17" s="48"/>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="48"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>20</v>
@@ -14353,15 +14371,15 @@
       <c r="AB21" t="s">
         <v>111</v>
       </c>
-      <c r="AD21" s="36">
+      <c r="AD21" s="35">
         <f>AD17-AD20</f>
         <v>8.6886053907164751E-13</v>
       </c>
-      <c r="AE21" s="36">
+      <c r="AE21" s="35">
         <f>AE17-AE20</f>
         <v>1.8322181984152877E-7</v>
       </c>
-      <c r="AF21" s="36">
+      <c r="AF21" s="35">
         <f>AE17-AF20</f>
         <v>4.8752668568852187E-14</v>
       </c>
@@ -14903,18 +14921,18 @@
       </c>
     </row>
     <row r="32" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="48" t="s">
+      <c r="L32" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="48"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="48"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="47"/>
       <c r="AB32" t="s">
         <v>111</v>
       </c>
-      <c r="AD32" s="36">
+      <c r="AD32" s="35">
         <f>AD28-AD31</f>
         <v>4.7191761609610694E-10</v>
       </c>
@@ -14922,7 +14940,7 @@
       <c r="AF32" t="s">
         <v>111</v>
       </c>
-      <c r="AH32" s="36">
+      <c r="AH32" s="35">
         <f>AH28-AH31</f>
         <v>8.5756290957306192E-11</v>
       </c>
@@ -15107,18 +15125,18 @@
         <v>6.1534111139849301E-14</v>
       </c>
       <c r="T37" s="12"/>
-      <c r="AB37" s="29" t="s">
+      <c r="AB37" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="AC37" s="30">
+      <c r="AC37" s="29">
         <f>AD37-AC42</f>
         <v>19.9999</v>
       </c>
-      <c r="AD37" s="31">
+      <c r="AD37" s="30">
         <f>C7</f>
         <v>20</v>
       </c>
-      <c r="AE37" s="32">
+      <c r="AE37" s="31">
         <f>AD37+AC42</f>
         <v>20.0001</v>
       </c>
@@ -15155,19 +15173,19 @@
         <v>-2.1222551493949027E-10</v>
       </c>
       <c r="T38" s="12"/>
-      <c r="AB38" s="26">
+      <c r="AB38" s="25">
         <f>AB39-AC42</f>
         <v>79.999899999999997</v>
       </c>
-      <c r="AC38" s="20">
+      <c r="AC38" s="19">
         <f>_xll.acq_options_bachelier_price($AB38,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>7.2727838073410682</v>
       </c>
-      <c r="AD38" s="21">
+      <c r="AD38" s="20">
         <f>_xll.acq_options_bachelier_price($AB38,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>7.2728367588076281</v>
       </c>
-      <c r="AE38" s="33">
+      <c r="AE38" s="32">
         <f>_xll.acq_options_bachelier_price($AB38,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>7.272889710300662</v>
       </c>
@@ -15187,7 +15205,7 @@
         <f>_xll.acq_options_bachelier_greeks($AK$36,$AB38,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>0.52951453320291109</v>
       </c>
-      <c r="AL38" s="19">
+      <c r="AL38" s="18">
         <f>_xll.acq_options_bachelier_greeks($AK$36,$AB38,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>0.52951479796752488</v>
       </c>
@@ -15240,19 +15258,19 @@
         <v>-7.9469764102668705E-13</v>
       </c>
       <c r="T39" s="12"/>
-      <c r="AB39" s="27">
+      <c r="AB39" s="26">
         <f>C4</f>
         <v>80</v>
       </c>
-      <c r="AC39" s="34">
+      <c r="AC39" s="33">
         <f>_xll.acq_options_bachelier_price($AB39,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>7.2728169816013324</v>
       </c>
-      <c r="AD39" s="22">
+      <c r="AD39" s="21">
         <f>_xll.acq_options_bachelier_price($AB39,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>7.2728699331208437</v>
       </c>
-      <c r="AE39" s="23">
+      <c r="AE39" s="22">
         <f>_xll.acq_options_bachelier_price($AB39,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>7.272922884666829</v>
       </c>
@@ -15272,7 +15290,7 @@
         <f>_xll.acq_options_bachelier_greeks($AK$36,$AB39,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>0.52951506272565185</v>
       </c>
-      <c r="AL39" s="19">
+      <c r="AL39" s="18">
         <f>_xll.acq_options_bachelier_greeks($AK$36,$AB39,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>0.52951532748523511</v>
       </c>
@@ -15284,7 +15302,7 @@
         <f>_xll.acq_options_bachelier_greeks($AO$36,$AB39,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>5.2952035791599301E-3</v>
       </c>
-      <c r="AP39" s="19">
+      <c r="AP39" s="18">
         <f>_xll.acq_options_bachelier_greeks($AO$36,$AB39,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>5.2951532748523504E-3</v>
       </c>
@@ -15325,19 +15343,19 @@
         <v>0</v>
       </c>
       <c r="T40" s="12"/>
-      <c r="AB40" s="28">
+      <c r="AB40" s="27">
         <f>AB39+AC42</f>
         <v>80.000100000000003</v>
       </c>
-      <c r="AC40" s="35">
+      <c r="AC40" s="34">
         <f>_xll.acq_options_bachelier_price($AB40,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>7.2728501559674976</v>
       </c>
-      <c r="AD40" s="24">
+      <c r="AD40" s="23">
         <f>_xll.acq_options_bachelier_price($AB40,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>7.2729031075399622</v>
       </c>
-      <c r="AE40" s="25">
+      <c r="AE40" s="24">
         <f>_xll.acq_options_bachelier_price($AB40,$C$5,$C$6,$C$8,AE$37,$C$9)</f>
         <v>7.2729560591388971</v>
       </c>
@@ -15357,7 +15375,7 @@
         <f>_xll.acq_options_bachelier_greeks($AK$36,$AB40,$C$5,$C$6,$C$8,AC$37,$C$9)</f>
         <v>0.52951559224362699</v>
       </c>
-      <c r="AL40" s="19">
+      <c r="AL40" s="18">
         <f>_xll.acq_options_bachelier_greeks($AK$36,$AB40,$C$5,$C$6,$C$8,AD$37,$C$9)</f>
         <v>0.52951585699817971</v>
       </c>
@@ -15492,11 +15510,11 @@
       <c r="AB43" t="s">
         <v>111</v>
       </c>
-      <c r="AD43" s="36">
+      <c r="AD43" s="35">
         <f>AP39-AD42</f>
         <v>9.7506204499442362E-14</v>
       </c>
-      <c r="AE43" s="36">
+      <c r="AE43" s="35">
         <f>AP39-AE42</f>
         <v>8.4073980416432548E-13</v>
       </c>
@@ -15555,7 +15573,7 @@
   <dimension ref="A1:AS56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="AP35" sqref="AP35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15570,39 +15588,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="L2" s="48" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="S2" s="48" t="s">
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="S2" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
       <c r="AD2" s="3" t="s">
         <v>112</v>
       </c>
@@ -15676,7 +15694,7 @@
         <v>127</v>
       </c>
       <c r="AD3" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="AE3" t="s">
         <v>99</v>
@@ -15873,15 +15891,15 @@
         <v>89.999899999999997</v>
       </c>
       <c r="AE5" s="13">
-        <f>_xll.acq_options_blackscholes_price($AD5,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AE$3,$AD5,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>4.1927240301498756</v>
       </c>
       <c r="AF5" s="13">
-        <f>_xll.acq_options_blackscholes_delta($AD5,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AF$3,$AD5,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>0.26820378510747978</v>
       </c>
       <c r="AG5" s="13">
-        <f>_xll.acq_options_blackscholes_gamma($AD5,$C$5,$C$6,$C$8,$C$9,$C$7)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AG$3,$AD5,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>1.0693269851087026E-2</v>
       </c>
       <c r="AH5" s="11"/>
@@ -15985,15 +16003,15 @@
         <v>90</v>
       </c>
       <c r="AE6" s="13">
-        <f>_xll.acq_options_blackscholes_price($AD6,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AE$3,$AD6,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>4.1927508505818558</v>
       </c>
       <c r="AF6" s="13">
-        <f>_xll.acq_options_blackscholes_delta($AD6,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AF$3,$AD6,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>0.2682048544347938</v>
       </c>
       <c r="AG6" s="13">
-        <f>_xll.acq_options_blackscholes_gamma($AD6,$C$5,$C$6,$C$8,$C$9,$C$7)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AG$3,$AD6,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>1.0693276428769077E-2</v>
       </c>
       <c r="AH6" s="11"/>
@@ -16091,15 +16109,15 @@
         <v>90.000100000000003</v>
       </c>
       <c r="AE7" s="13">
-        <f>_xll.acq_options_blackscholes_price($AD7,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AE$3,$AD7,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>4.1927776711207656</v>
       </c>
       <c r="AF7" s="13">
-        <f>_xll.acq_options_blackscholes_delta($AD7,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AF$3,$AD7,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>0.26820592376276564</v>
       </c>
       <c r="AG7" s="13">
-        <f>_xll.acq_options_blackscholes_gamma($AD7,$C$5,$C$6,$C$8,$C$9,$C$7)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AG$3,$AD7,$C$5,$C$6,$C$8,$C$9,$C$7,$C$10)</f>
         <v>1.0693283006315852E-2</v>
       </c>
       <c r="AJ7" s="11"/>
@@ -16199,7 +16217,7 @@
       <c r="B9" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="36">
         <v>0.06</v>
       </c>
       <c r="F9">
@@ -16389,15 +16407,15 @@
       <c r="AD10" t="s">
         <v>111</v>
       </c>
-      <c r="AF10" s="36">
+      <c r="AF10" s="35">
         <f>AF6-AF9</f>
         <v>-6.3076210921053644E-12</v>
       </c>
-      <c r="AG10" s="36">
+      <c r="AG10" s="35">
         <f>AG6-AG9</f>
         <v>3.1879922541069861E-7</v>
       </c>
-      <c r="AH10" s="36">
+      <c r="AH10" s="35">
         <f>AG6-AH9</f>
         <v>-2.0587698212892747E-13</v>
       </c>
@@ -16828,17 +16846,17 @@
         <f>AD17-AE20</f>
         <v>0.19990000000000002</v>
       </c>
-      <c r="AE16">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,$C$6,$C$9,$C$8,AD16,$C$10)</f>
-        <v>10.550537451075833</v>
+      <c r="AE16" s="13">
+        <f>_xll.acq_options_blackscholes_greeks(AE$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD16,$C$10)</f>
+        <v>4.1884205033693505</v>
       </c>
       <c r="AF16" s="13">
-        <f>_xll.acq_options_blackscholes_vega($C$4,$C$5,$C$6,$C$9,$C$8,AD16)</f>
-        <v>53.467042623037301</v>
+        <f>_xll.acq_options_blackscholes_greeks(AF$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD16,$C$10)</f>
+        <v>43.299172667915535</v>
       </c>
       <c r="AG16" s="13">
-        <f>_xll.acq_options_blackscholes_vomma($C$4,$C$5,$C$6,$C$9,$C$8,AD16)</f>
-        <v>-6.6031041777243216</v>
+        <f>_xll.acq_options_blackscholes_greeks(AG$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD16,$C$10)</f>
+        <v>86.030074254044706</v>
       </c>
       <c r="AH16" s="11"/>
     </row>
@@ -16877,33 +16895,33 @@
         <f>_xll.acq_options_blackscholes_vol($C$4,$C$5,$C$6,$C$8,$C$9,$N17,FALSE)</f>
         <v>0.65</v>
       </c>
-      <c r="S17" s="48" t="s">
+      <c r="S17" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="48"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
-      <c r="X17" s="48"/>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="48"/>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="38"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="37"/>
+      <c r="AB17" s="37"/>
       <c r="AD17" s="16">
         <f>C7</f>
         <v>0.2</v>
       </c>
-      <c r="AE17">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,$C$6,$C$9,$C$8,AD17,$C$10)</f>
-        <v>10.555884122316996</v>
+      <c r="AE17" s="13">
+        <f>_xll.acq_options_blackscholes_greeks(AE$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD17,$C$10)</f>
+        <v>4.1927508505818558</v>
       </c>
       <c r="AF17" s="13">
-        <f>_xll.acq_options_blackscholes_vega($C$4,$C$5,$C$6,$C$9,$C$8,AD17)</f>
-        <v>53.466382143845387</v>
+        <f>_xll.acq_options_blackscholes_greeks(AF$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD17,$C$10)</f>
+        <v>43.307769536514776</v>
       </c>
       <c r="AG17" s="13">
-        <f t="shared" ref="AG17:AG18" si="1">_xll.acq_options_blackscholes_vomma($C$4,$C$5,$C$6,$C$9,$C$8,AD17)</f>
-        <v>-6.6064796009357405</v>
+        <f>_xll.acq_options_blackscholes_greeks(AG$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD17,$C$10)</f>
+        <v>85.907330130391927</v>
       </c>
       <c r="AH17" s="11"/>
     </row>
@@ -16979,17 +16997,17 @@
         <f>AD17+AE20</f>
         <v>0.2001</v>
       </c>
-      <c r="AE18">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,$C$6,$C$9,$C$8,AD18,$C$10)</f>
-        <v>10.561230727493346</v>
+      <c r="AE18" s="13">
+        <f>_xll.acq_options_blackscholes_greeks(AE$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD18,$C$10)</f>
+        <v>4.1970820568678278</v>
       </c>
       <c r="AF18" s="13">
-        <f>_xll.acq_options_blackscholes_vega($C$4,$C$5,$C$6,$C$9,$C$8,AD18)</f>
-        <v>53.465721327129046</v>
+        <f>_xll.acq_options_blackscholes_greeks(AF$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD18,$C$10)</f>
+        <v>43.316354140415449</v>
       </c>
       <c r="AG18" s="13">
-        <f t="shared" si="1"/>
-        <v>-6.6098546665583333</v>
+        <f>_xll.acq_options_blackscholes_greeks(AG$14,$C$4,$C$5,$C$6,$C$8,$C$9,$AD18,$C$10)</f>
+        <v>85.784780222062437</v>
       </c>
       <c r="AJ18" s="11"/>
       <c r="AK18" s="11"/>
@@ -17168,15 +17186,15 @@
       </c>
       <c r="AF20" s="17">
         <f>_xll.acq_diff1_c3pt(AD16:AD18,AE16:AE18)</f>
-        <v>53.466382087569492</v>
+        <v>43.307767492391285</v>
       </c>
       <c r="AG20" s="17">
         <f>_xll.acq_diff2_c3pt(AD16:AD18,AE16:AE18)</f>
-        <v>-6.6064814063800439</v>
+        <v>85.907346658596367</v>
       </c>
       <c r="AH20" s="17">
         <f>_xll.acq_diff1_c3pt(AD16:AD18,AF16:AF18)</f>
-        <v>-6.6064795412764168</v>
+        <v>85.907362499578227</v>
       </c>
     </row>
     <row r="21" spans="6:45" x14ac:dyDescent="0.25">
@@ -17245,17 +17263,17 @@
       <c r="AD21" t="s">
         <v>111</v>
       </c>
-      <c r="AF21" s="36">
+      <c r="AF21" s="35">
         <f>AF17-AF20</f>
-        <v>5.6275894166901708E-8</v>
-      </c>
-      <c r="AG21" s="36">
+        <v>2.0441234909185368E-6</v>
+      </c>
+      <c r="AG21" s="35">
         <f>AG17-AG20</f>
-        <v>1.8054443033932444E-6</v>
-      </c>
-      <c r="AH21" s="36">
+        <v>-1.6528204440646732E-5</v>
+      </c>
+      <c r="AH21" s="35">
         <f>AG17-AH20</f>
-        <v>-5.9659323703442624E-8</v>
+        <v>-3.2369186300229558E-5</v>
       </c>
     </row>
     <row r="22" spans="6:45" x14ac:dyDescent="0.25">
@@ -17670,11 +17688,11 @@
         <v>1.9900000000000001E-2</v>
       </c>
       <c r="AE27">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,$C$6,AD27,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AE$25,$C$4,$C$5,$C$6,$AD27,$C$9,$C$7,$C$10)</f>
         <v>4.1877665123257053</v>
       </c>
-      <c r="AF27" s="13">
-        <f>_xll.acq_options_blackscholes_rho($C$4,$C$5,$C$6,AD27,$C$9,$C$7,$C$10)</f>
+      <c r="AF27">
+        <f>_xll.acq_options_blackscholes_greeks(AF$25,$C$4,$C$5,$C$6,$AD27,$C$9,$C$7,$C$10)</f>
         <v>49.822551772366097</v>
       </c>
       <c r="AG27" s="13"/>
@@ -17683,11 +17701,11 @@
         <v>2.4998999999999998</v>
       </c>
       <c r="AI27">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,AH27,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AI$25,$C$4,$C$5,$AH27,$C$8,$C$9,$C$7,$C$10)</f>
         <v>4.1926825566795181</v>
       </c>
-      <c r="AJ27" s="13">
-        <f>_xll.acq_options_blackscholes_theta($C$4,$C$5,AH27,$C$8,$C$9,$C$7,$C$10)</f>
+      <c r="AJ27">
+        <f>_xll.acq_options_blackscholes_greeks(AJ$25,$C$4,$C$5,$AH27,$C$8,$C$9,$C$7,$C$10)</f>
         <v>-0.68295975865340086</v>
       </c>
     </row>
@@ -17740,11 +17758,11 @@
         <v>0.02</v>
       </c>
       <c r="AE28">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,$C$6,AD28,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AE$25,$C$4,$C$5,$C$6,$AD28,$C$9,$C$7,$C$10)</f>
         <v>4.1927508505818558</v>
       </c>
-      <c r="AF28" s="13">
-        <f>_xll.acq_options_blackscholes_rho($C$4,$C$5,$C$6,AD28,$C$9,$C$7,$C$10)</f>
+      <c r="AF28">
+        <f>_xll.acq_options_blackscholes_greeks(AF$25,$C$4,$C$5,$C$6,$AD28,$C$9,$C$7,$C$10)</f>
         <v>49.864215121373967</v>
       </c>
       <c r="AG28" s="13"/>
@@ -17753,11 +17771,11 @@
         <v>2.5</v>
       </c>
       <c r="AI28">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,AH28,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AI$25,$C$4,$C$5,$AH28,$C$8,$C$9,$C$7,$C$10)</f>
         <v>4.1927508505818558</v>
       </c>
-      <c r="AJ28" s="13">
-        <f>_xll.acq_options_blackscholes_theta($C$4,$C$5,AH28,$C$8,$C$9,$C$7,$C$10)</f>
+      <c r="AJ28">
+        <f>_xll.acq_options_blackscholes_greeks(AJ$25,$C$4,$C$5,$AH28,$C$8,$C$9,$C$7,$C$10)</f>
         <v>-0.68291828848369618</v>
       </c>
     </row>
@@ -17810,11 +17828,11 @@
         <v>2.01E-2</v>
       </c>
       <c r="AE29">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,$C$6,AD29,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AE$25,$C$4,$C$5,$C$6,$AD29,$C$9,$C$7,$C$10)</f>
         <v>4.1977393557035931</v>
       </c>
-      <c r="AF29" s="13">
-        <f>_xll.acq_options_blackscholes_rho($C$4,$C$5,$C$6,AD29,$C$9,$C$7,$C$10)</f>
+      <c r="AF29">
+        <f>_xll.acq_options_blackscholes_greeks(AF$25,$C$4,$C$5,$C$6,$AD29,$C$9,$C$7,$C$10)</f>
         <v>49.905889079206759</v>
       </c>
       <c r="AG29" s="13"/>
@@ -17823,11 +17841,11 @@
         <v>2.5001000000000002</v>
       </c>
       <c r="AI29">
-        <f>_xll.acq_options_blackscholes_price($C$4,$C$5,AH29,$C$8,$C$9,$C$7,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks(AI$25,$C$4,$C$5,$AH29,$C$8,$C$9,$C$7,$C$10)</f>
         <v>4.1928191403372992</v>
       </c>
-      <c r="AJ29" s="13">
-        <f>_xll.acq_options_blackscholes_theta($C$4,$C$5,AH29,$C$8,$C$9,$C$7,$C$10)</f>
+      <c r="AJ29">
+        <f>_xll.acq_options_blackscholes_greeks(AJ$25,$C$4,$C$5,$AH29,$C$8,$C$9,$C$7,$C$10)</f>
         <v>-0.68287682086973445</v>
       </c>
     </row>
@@ -17890,7 +17908,7 @@
       <c r="AD32" t="s">
         <v>111</v>
       </c>
-      <c r="AF32" s="36">
+      <c r="AF32" s="35">
         <f>AF28-AF31</f>
         <v>-1.7680655375329479E-6</v>
       </c>
@@ -17898,7 +17916,7 @@
       <c r="AH32" t="s">
         <v>111</v>
       </c>
-      <c r="AJ32" s="36">
+      <c r="AJ32" s="35">
         <f>AJ28-AJ31</f>
         <v>4.205166215243139E-10</v>
       </c>
@@ -18002,18 +18020,18 @@
       <c r="W37" s="11"/>
       <c r="X37" s="11"/>
       <c r="Y37" s="11"/>
-      <c r="AD37" s="29" t="s">
+      <c r="AD37" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="AE37" s="42">
+      <c r="AE37" s="41">
         <f>AF37-AE42</f>
         <v>0.19990000000000002</v>
       </c>
-      <c r="AF37" s="21">
+      <c r="AF37" s="20">
         <f>C7</f>
         <v>0.2</v>
       </c>
-      <c r="AG37" s="43">
+      <c r="AG37" s="42">
         <f>AF37+AE42</f>
         <v>0.2001</v>
       </c>
@@ -18033,56 +18051,56 @@
       <c r="W38" s="11"/>
       <c r="X38" s="11"/>
       <c r="Y38" s="11"/>
-      <c r="AD38" s="39">
+      <c r="AD38" s="38">
         <f>AD39-AE42</f>
         <v>89.999899999999997</v>
       </c>
-      <c r="AE38" s="20">
+      <c r="AE38" s="19">
         <f>_xll.acq_options_blackscholes_price($AD38,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>4.1883936952289851</v>
       </c>
-      <c r="AF38" s="21">
+      <c r="AF38" s="20">
         <f>_xll.acq_options_blackscholes_price($AD38,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>4.1927240301498756</v>
       </c>
-      <c r="AG38" s="33">
+      <c r="AG38" s="32">
         <f>_xll.acq_options_blackscholes_price($AD38,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>4.1970552241516685</v>
       </c>
       <c r="AI38">
-        <f>_xll.acq_options_blackscholes_delta($AD38,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD38,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>0.26808086872425324</v>
       </c>
       <c r="AJ38">
-        <f>_xll.acq_options_blackscholes_delta($AD38,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD38,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>0.26820378510747978</v>
       </c>
       <c r="AK38">
-        <f>_xll.acq_options_blackscholes_delta($AD38,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD38,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>0.26832662704654892</v>
       </c>
       <c r="AM38">
-        <f>_xll.acq_options_blackscholes_vega($AD38,$C$5,$C$6,$C$8,$C$9,AE$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD38,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>43.299049714446767</v>
       </c>
-      <c r="AN38" s="19">
-        <f>_xll.acq_options_blackscholes_vega($AD38,$C$5,$C$6,$C$8,$C$9,AF$37)</f>
+      <c r="AN38">
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD38,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>43.307646657527272</v>
       </c>
       <c r="AO38">
-        <f>_xll.acq_options_blackscholes_vega($AD38,$C$5,$C$6,$C$8,$C$9,AG$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD38,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>43.316231335834985</v>
       </c>
       <c r="AQ38">
-        <f>_xll.acq_options_blackscholes_vanna($AD38,$C$5,$C$6,$C$8,$C$9,AE$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD38,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>1.2295363005253457</v>
       </c>
       <c r="AR38">
-        <f>_xll.acq_options_blackscholes_vanna($AD38,$C$5,$C$6,$C$8,$C$9,AF$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD38,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>1.2287914877713453</v>
       </c>
       <c r="AS38">
-        <f>_xll.acq_options_blackscholes_vanna($AD38,$C$5,$C$6,$C$8,$C$9,AG$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD38,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>1.2280474172622813</v>
       </c>
     </row>
@@ -18101,56 +18119,56 @@
       <c r="W39" s="11"/>
       <c r="X39" s="11"/>
       <c r="Y39" s="11"/>
-      <c r="AD39" s="40">
+      <c r="AD39" s="39">
         <f>C4</f>
         <v>90</v>
       </c>
-      <c r="AE39" s="34">
+      <c r="AE39" s="33">
         <f>_xll.acq_options_blackscholes_price($AD39,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>4.1884205033693505</v>
       </c>
-      <c r="AF39" s="22">
+      <c r="AF39" s="21">
         <f>_xll.acq_options_blackscholes_price($AD39,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>4.1927508505818558</v>
       </c>
-      <c r="AG39" s="23">
+      <c r="AG39" s="22">
         <f>_xll.acq_options_blackscholes_price($AD39,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>4.1970820568678278</v>
       </c>
       <c r="AI39">
-        <f>_xll.acq_options_blackscholes_delta($AD39,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD39,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>0.2680819383741227</v>
       </c>
       <c r="AJ39">
-        <f>_xll.acq_options_blackscholes_delta($AD39,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD39,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>0.2682048544347938</v>
       </c>
       <c r="AK39">
-        <f>_xll.acq_options_blackscholes_delta($AD39,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD39,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>0.26832769605132722</v>
       </c>
       <c r="AM39">
-        <f>_xll.acq_options_blackscholes_vega($AD39,$C$5,$C$6,$C$8,$C$9,AE$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD39,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>43.299172667915535</v>
       </c>
-      <c r="AN39" s="19">
-        <f>_xll.acq_options_blackscholes_vega($AD39,$C$5,$C$6,$C$8,$C$9,AF$37)</f>
+      <c r="AN39">
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD39,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>43.307769536514776</v>
       </c>
       <c r="AO39">
-        <f>_xll.acq_options_blackscholes_vega($AD39,$C$5,$C$6,$C$8,$C$9,AG$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD39,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>43.316354140415449</v>
       </c>
       <c r="AQ39">
-        <f>_xll.acq_options_blackscholes_vanna($AD39,$C$5,$C$6,$C$8,$C$9,AE$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD39,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>1.2295330748740971</v>
       </c>
-      <c r="AR39" s="19">
-        <f>_xll.acq_options_blackscholes_vanna($AD39,$C$5,$C$6,$C$8,$C$9,AF$37)</f>
+      <c r="AR39">
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD39,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>1.2287882623149675</v>
       </c>
       <c r="AS39">
-        <f>_xll.acq_options_blackscholes_vanna($AD39,$C$5,$C$6,$C$8,$C$9,AG$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD39,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>1.2280441920052747</v>
       </c>
     </row>
@@ -18169,56 +18187,56 @@
       <c r="W40" s="11"/>
       <c r="X40" s="11"/>
       <c r="Y40" s="11"/>
-      <c r="AD40" s="41">
+      <c r="AD40" s="40">
         <f>AD39+AE42</f>
         <v>90.000100000000003</v>
       </c>
-      <c r="AE40" s="35">
+      <c r="AE40" s="34">
         <f>_xll.acq_options_blackscholes_price($AD40,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>4.1884473116166703</v>
       </c>
-      <c r="AF40" s="24">
+      <c r="AF40" s="23">
         <f>_xll.acq_options_blackscholes_price($AD40,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>4.1927776711207656</v>
       </c>
-      <c r="AG40" s="25">
+      <c r="AG40" s="24">
         <f>_xll.acq_options_blackscholes_price($AD40,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>4.197108889690881</v>
       </c>
       <c r="AI40">
-        <f>_xll.acq_options_blackscholes_delta($AD40,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD40,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>0.26808300802465251</v>
       </c>
       <c r="AJ40">
-        <f>_xll.acq_options_blackscholes_delta($AD40,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD40,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>0.26820592376276564</v>
       </c>
       <c r="AK40">
-        <f>_xll.acq_options_blackscholes_delta($AD40,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AI$36,$AD40,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>0.26832876505676068</v>
       </c>
       <c r="AM40">
-        <f>_xll.acq_options_blackscholes_vega($AD40,$C$5,$C$6,$C$8,$C$9,AE$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD40,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>43.299295621061738</v>
       </c>
-      <c r="AN40" s="19">
-        <f>_xll.acq_options_blackscholes_vega($AD40,$C$5,$C$6,$C$8,$C$9,AF$37)</f>
+      <c r="AN40">
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD40,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>43.307892415179737</v>
       </c>
       <c r="AO40">
-        <f>_xll.acq_options_blackscholes_vega($AD40,$C$5,$C$6,$C$8,$C$9,AG$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AM$36,$AD40,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>43.31647694467339</v>
       </c>
       <c r="AQ40">
-        <f>_xll.acq_options_blackscholes_vanna($AD40,$C$5,$C$6,$C$8,$C$9,AE$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD40,$C$5,$C$6,$C$8,$C$9,AE$37,$C$10)</f>
         <v>1.2295298491964135</v>
       </c>
       <c r="AR40">
-        <f>_xll.acq_options_blackscholes_vanna($AD40,$C$5,$C$6,$C$8,$C$9,AF$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD40,$C$5,$C$6,$C$8,$C$9,AF$37,$C$10)</f>
         <v>1.2287850368322066</v>
       </c>
       <c r="AS40">
-        <f>_xll.acq_options_blackscholes_vanna($AD40,$C$5,$C$6,$C$8,$C$9,AG$37)</f>
+        <f>_xll.acq_options_blackscholes_greeks($AQ$36,$AD40,$C$5,$C$6,$C$8,$C$9,AG$37,$C$10)</f>
         <v>1.2280409667219361</v>
       </c>
     </row>
@@ -18286,11 +18304,11 @@
       <c r="AD43" t="s">
         <v>111</v>
       </c>
-      <c r="AF43" s="36">
+      <c r="AF43" s="35">
         <f>AR39-AF42</f>
         <v>-1.2370780688719663E-7</v>
       </c>
-      <c r="AG43" s="36">
+      <c r="AG43" s="35">
         <f>AR39-AG42</f>
         <v>3.1671554268086766E-11</v>
       </c>
@@ -18495,8 +18513,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18509,15 +18527,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -18532,15 +18550,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48" t="s">
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="48"/>
+      <c r="J3" s="47"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -18573,49 +18591,49 @@
       <c r="L4" t="s">
         <v>136</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="43">
         <v>120</v>
       </c>
-      <c r="N4" s="44">
+      <c r="N4" s="43">
         <v>130</v>
       </c>
-      <c r="O4" s="44">
+      <c r="O4" s="43">
         <v>140</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="43">
         <v>150</v>
       </c>
-      <c r="Q4" s="44">
+      <c r="Q4" s="43">
         <v>160</v>
       </c>
-      <c r="R4" s="44">
+      <c r="R4" s="43">
         <v>170</v>
       </c>
-      <c r="S4" s="44">
+      <c r="S4" s="43">
         <v>180</v>
       </c>
       <c r="U4" t="s">
         <v>136</v>
       </c>
-      <c r="V4" s="44">
+      <c r="V4" s="43">
         <v>120</v>
       </c>
-      <c r="W4" s="44">
+      <c r="W4" s="43">
         <v>130</v>
       </c>
-      <c r="X4" s="44">
+      <c r="X4" s="43">
         <v>140</v>
       </c>
-      <c r="Y4" s="44">
+      <c r="Y4" s="43">
         <v>150</v>
       </c>
-      <c r="Z4" s="44">
+      <c r="Z4" s="43">
         <v>160</v>
       </c>
-      <c r="AA4" s="44">
+      <c r="AA4" s="43">
         <v>170</v>
       </c>
-      <c r="AB4" s="44">
+      <c r="AB4" s="43">
         <v>180</v>
       </c>
     </row>
@@ -18645,7 +18663,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G5,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.2409702289365026</v>
       </c>
-      <c r="L5" s="46">
+      <c r="L5" s="45">
         <v>0.05</v>
       </c>
       <c r="M5">
@@ -18676,7 +18694,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L5,$C$8,$C$9,$C$7,TRUE)</f>
         <v>29.911482759239618</v>
       </c>
-      <c r="U5" s="46">
+      <c r="U5" s="45">
         <v>0.05</v>
       </c>
       <c r="V5">
@@ -18734,7 +18752,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G6,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.4604738210067554</v>
       </c>
-      <c r="L6" s="46">
+      <c r="L6" s="45">
         <v>0.1</v>
       </c>
       <c r="M6">
@@ -18765,7 +18783,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>29.866937861547115</v>
       </c>
-      <c r="U6" s="46">
+      <c r="U6" s="45">
         <v>0.1</v>
       </c>
       <c r="V6">
@@ -18823,7 +18841,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G7,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.49501536694438641</v>
       </c>
-      <c r="L7" s="46">
+      <c r="L7" s="45">
         <v>0.15</v>
       </c>
       <c r="M7">
@@ -18854,7 +18872,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L7,$C$8,$C$9,$C$7,TRUE)</f>
         <v>29.91318851001617</v>
       </c>
-      <c r="U7" s="46">
+      <c r="U7" s="45">
         <v>0.15</v>
       </c>
       <c r="V7">
@@ -18912,7 +18930,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G8,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.11085764156847244</v>
       </c>
-      <c r="L8" s="46">
+      <c r="L8" s="45">
         <v>0.2</v>
       </c>
       <c r="M8">
@@ -18943,7 +18961,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L8,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.033950291703007</v>
       </c>
-      <c r="U8" s="46">
+      <c r="U8" s="45">
         <v>0.2</v>
       </c>
       <c r="V8">
@@ -18979,7 +18997,7 @@
       <c r="B9" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="36">
         <v>0.06</v>
       </c>
       <c r="F9">
@@ -19001,7 +19019,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G9,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.426895703799709E-2</v>
       </c>
-      <c r="L9" s="46">
+      <c r="L9" s="45">
         <v>0.25</v>
       </c>
       <c r="M9">
@@ -19032,7 +19050,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L9,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.203730848908037</v>
       </c>
-      <c r="U9" s="46">
+      <c r="U9" s="45">
         <v>0.25</v>
       </c>
       <c r="V9">
@@ -19090,7 +19108,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G10,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>9.3215811534007841E-4</v>
       </c>
-      <c r="L10" s="46">
+      <c r="L10" s="45">
         <v>0.3</v>
       </c>
       <c r="M10">
@@ -19121,7 +19139,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L10,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.403895162587332</v>
       </c>
-      <c r="U10" s="46">
+      <c r="U10" s="45">
         <v>0.3</v>
       </c>
       <c r="V10">
@@ -19173,7 +19191,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G11,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>2.8027241433398957E-5</v>
       </c>
-      <c r="L11" s="46">
+      <c r="L11" s="45">
         <v>0.35</v>
       </c>
       <c r="M11">
@@ -19204,7 +19222,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L11,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.622208044236658</v>
       </c>
-      <c r="U11" s="46">
+      <c r="U11" s="45">
         <v>0.35</v>
       </c>
       <c r="V11">
@@ -19256,7 +19274,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G12,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.6218005932214387E-7</v>
       </c>
-      <c r="L12" s="46">
+      <c r="L12" s="45">
         <v>0.4</v>
       </c>
       <c r="M12">
@@ -19287,7 +19305,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L12,$C$8,$C$9,$C$7,TRUE)</f>
         <v>30.850737745484096</v>
       </c>
-      <c r="U12" s="46">
+      <c r="U12" s="45">
         <v>0.4</v>
       </c>
       <c r="V12">
@@ -19339,7 +19357,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G13,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.9304414708222245E-9</v>
       </c>
-      <c r="L13" s="46">
+      <c r="L13" s="45">
         <v>0.45</v>
       </c>
       <c r="M13">
@@ -19370,7 +19388,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L13,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.084295825844606</v>
       </c>
-      <c r="U13" s="46">
+      <c r="U13" s="45">
         <v>0.45</v>
       </c>
       <c r="V13">
@@ -19425,7 +19443,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G14,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>4.167517628471426E-12</v>
       </c>
-      <c r="L14" s="46">
+      <c r="L14" s="45">
         <v>0.5</v>
       </c>
       <c r="M14">
@@ -19456,7 +19474,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L14,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.319444688823182</v>
       </c>
-      <c r="U14" s="46">
+      <c r="U14" s="45">
         <v>0.5</v>
       </c>
       <c r="V14">
@@ -19489,7 +19507,7 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>142</v>
       </c>
       <c r="F15">
@@ -19511,7 +19529,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G15,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.6428793012235105E-15</v>
       </c>
-      <c r="L15" s="46">
+      <c r="L15" s="45">
         <v>0.55000000000000004</v>
       </c>
       <c r="M15">
@@ -19542,7 +19560,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L15,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.553881861379864</v>
       </c>
-      <c r="U15" s="46">
+      <c r="U15" s="45">
         <v>0.55000000000000004</v>
       </c>
       <c r="V15">
@@ -19594,7 +19612,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G16,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.3059135679790043E-18</v>
       </c>
-      <c r="L16" s="46">
+      <c r="L16" s="45">
         <v>0.6</v>
       </c>
       <c r="M16">
@@ -19625,7 +19643,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L16,$C$8,$C$9,$C$7,TRUE)</f>
         <v>31.786054869626298</v>
       </c>
-      <c r="U16" s="46">
+      <c r="U16" s="45">
         <v>0.6</v>
       </c>
       <c r="V16">
@@ -19677,7 +19695,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G17,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.9625621136394617E-22</v>
       </c>
-      <c r="L17" s="46">
+      <c r="L17" s="45">
         <v>0.65</v>
       </c>
       <c r="M17">
@@ -19708,7 +19726,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L17,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.014915973629982</v>
       </c>
-      <c r="U17" s="46">
+      <c r="U17" s="45">
         <v>0.65</v>
       </c>
       <c r="V17">
@@ -19760,7 +19778,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G18,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.2715942320358724E-26</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="45">
         <v>0.7</v>
       </c>
       <c r="M18">
@@ -19791,7 +19809,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L18,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.239762763653374</v>
       </c>
-      <c r="U18" s="46">
+      <c r="U18" s="45">
         <v>0.7</v>
       </c>
       <c r="V18">
@@ -19843,7 +19861,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G19,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.6669095805321848E-31</v>
       </c>
-      <c r="L19" s="46">
+      <c r="L19" s="45">
         <v>0.75</v>
       </c>
       <c r="M19">
@@ -19874,7 +19892,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L19,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.460132474437401</v>
       </c>
-      <c r="U19" s="46">
+      <c r="U19" s="45">
         <v>0.75</v>
       </c>
       <c r="V19">
@@ -19926,7 +19944,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G20,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>4.868419745828726E-36</v>
       </c>
-      <c r="L20" s="46">
+      <c r="L20" s="45">
         <v>0.8</v>
       </c>
       <c r="M20">
@@ -19957,7 +19975,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L20,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.675730604857705</v>
       </c>
-      <c r="U20" s="46">
+      <c r="U20" s="45">
         <v>0.8</v>
       </c>
       <c r="V20">
@@ -20016,7 +20034,7 @@
         <f>_xll.acq_options_blackscholes_price($C$4,G21,$C$6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.0810353477718544E-41</v>
       </c>
-      <c r="L21" s="46">
+      <c r="L21" s="45">
         <v>0.85</v>
       </c>
       <c r="M21">
@@ -20047,7 +20065,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L21,$C$8,$C$9,$C$7,TRUE)</f>
         <v>32.886381891485414</v>
       </c>
-      <c r="U21" s="46">
+      <c r="U21" s="45">
         <v>0.85</v>
       </c>
       <c r="V21">
@@ -20080,7 +20098,7 @@
       </c>
     </row>
     <row r="22" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="L22" s="46">
+      <c r="L22" s="45">
         <v>0.9</v>
       </c>
       <c r="M22">
@@ -20111,7 +20129,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L22,$C$8,$C$9,$C$7,TRUE)</f>
         <v>33.091996127090255</v>
       </c>
-      <c r="U22" s="46">
+      <c r="U22" s="45">
         <v>0.9</v>
       </c>
       <c r="V22">
@@ -20144,7 +20162,7 @@
       </c>
     </row>
     <row r="23" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="L23" s="46">
+      <c r="L23" s="45">
         <v>0.95</v>
       </c>
       <c r="M23">
@@ -20175,7 +20193,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L23,$C$8,$C$9,$C$7,TRUE)</f>
         <v>33.292544011466831</v>
       </c>
-      <c r="U23" s="46">
+      <c r="U23" s="45">
         <v>0.95</v>
       </c>
       <c r="V23">
@@ -20215,7 +20233,7 @@
       </c>
     </row>
     <row r="24" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="L24" s="46">
+      <c r="L24" s="45">
         <v>1</v>
       </c>
       <c r="M24">
@@ -20246,7 +20264,7 @@
         <f>_xll.acq_options_bjerksund_price_approx(S$4,$C$5,$L24,$C$8,$C$9,$C$7,TRUE)</f>
         <v>33.488039891384361</v>
       </c>
-      <c r="U24" s="46">
+      <c r="U24" s="45">
         <v>1</v>
       </c>
       <c r="V24">
@@ -20279,53 +20297,53 @@
       </c>
     </row>
     <row r="26" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="V26" s="47"/>
-      <c r="W26" s="47"/>
-      <c r="X26" s="47"/>
-      <c r="Y26" s="47"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="46"/>
+      <c r="X26" s="46"/>
+      <c r="Y26" s="46"/>
     </row>
     <row r="27" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="V27" s="47"/>
-      <c r="W27" s="47"/>
-      <c r="X27" s="47"/>
-      <c r="Y27" s="47"/>
-      <c r="Z27" s="47"/>
+      <c r="V27" s="46"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="46"/>
+      <c r="Y27" s="46"/>
+      <c r="Z27" s="46"/>
     </row>
     <row r="28" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="V28" s="47"/>
-      <c r="W28" s="47"/>
-      <c r="X28" s="47"/>
-      <c r="Y28" s="47"/>
-      <c r="Z28" s="47"/>
+      <c r="V28" s="46"/>
+      <c r="W28" s="46"/>
+      <c r="X28" s="46"/>
+      <c r="Y28" s="46"/>
+      <c r="Z28" s="46"/>
     </row>
     <row r="29" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="V29" s="47"/>
-      <c r="W29" s="47"/>
-      <c r="X29" s="47"/>
-      <c r="Y29" s="47"/>
-      <c r="Z29" s="47"/>
+      <c r="V29" s="46"/>
+      <c r="W29" s="46"/>
+      <c r="X29" s="46"/>
+      <c r="Y29" s="46"/>
+      <c r="Z29" s="46"/>
     </row>
     <row r="30" spans="6:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="48" t="s">
+      <c r="G30" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="S30" s="48" t="s">
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="S30" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="T30" s="48"/>
-      <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="48"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="V30" s="47"/>
+      <c r="W30" s="47"/>
+      <c r="X30" s="47"/>
+      <c r="Y30" s="47"/>
+      <c r="Z30" s="47"/>
       <c r="AC30" t="s">
         <v>147</v>
       </c>
@@ -21531,46 +21549,46 @@
       </c>
     </row>
     <row r="43" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="V43" s="47"/>
-      <c r="W43" s="47"/>
-      <c r="X43" s="47"/>
-      <c r="Y43" s="47"/>
-      <c r="Z43" s="47"/>
-      <c r="AA43" s="47"/>
-      <c r="AB43" s="47"/>
+      <c r="V43" s="46"/>
+      <c r="W43" s="46"/>
+      <c r="X43" s="46"/>
+      <c r="Y43" s="46"/>
+      <c r="Z43" s="46"/>
+      <c r="AA43" s="46"/>
+      <c r="AB43" s="46"/>
     </row>
     <row r="44" spans="6:35" x14ac:dyDescent="0.25">
-      <c r="V44" s="47"/>
-      <c r="W44" s="47"/>
-      <c r="X44" s="47"/>
-      <c r="Y44" s="47"/>
-      <c r="Z44" s="47"/>
-      <c r="AA44" s="47"/>
-      <c r="AB44" s="47"/>
+      <c r="V44" s="46"/>
+      <c r="W44" s="46"/>
+      <c r="X44" s="46"/>
+      <c r="Y44" s="46"/>
+      <c r="Z44" s="46"/>
+      <c r="AA44" s="46"/>
+      <c r="AB44" s="46"/>
     </row>
     <row r="45" spans="6:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="48" t="s">
+      <c r="G45" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="48"/>
-      <c r="N45" s="48"/>
-      <c r="S45" s="48" t="s">
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="47"/>
+      <c r="S45" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="T45" s="48"/>
-      <c r="U45" s="48"/>
-      <c r="V45" s="48"/>
-      <c r="W45" s="48"/>
-      <c r="X45" s="48"/>
-      <c r="Y45" s="48"/>
-      <c r="Z45" s="48"/>
-      <c r="AA45" s="47"/>
-      <c r="AB45" s="47"/>
+      <c r="T45" s="47"/>
+      <c r="U45" s="47"/>
+      <c r="V45" s="47"/>
+      <c r="W45" s="47"/>
+      <c r="X45" s="47"/>
+      <c r="Y45" s="47"/>
+      <c r="Z45" s="47"/>
+      <c r="AA45" s="46"/>
+      <c r="AB45" s="46"/>
     </row>
     <row r="46" spans="6:35" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
@@ -22443,7 +22461,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added utils to count number of unique elements (acq_count_unique) and concatenates the elements to string (acq_join)
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BFFC55-3F41-4F14-8DAC-A269988898E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B3ADC8-FCFA-434A-A21A-478811F2D30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="1605" windowWidth="21405" windowHeight="11370" tabRatio="900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="BlackScholes" sheetId="14" r:id="rId4"/>
     <sheet name="BjerksundStensland2002" sheetId="16" r:id="rId5"/>
     <sheet name="Description" sheetId="7" r:id="rId6"/>
-    <sheet name="Special" sheetId="9" r:id="rId7"/>
+    <sheet name="Types" sheetId="17" r:id="rId7"/>
+    <sheet name="Special" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="162">
   <si>
     <t>x</t>
   </si>
@@ -646,15 +647,46 @@
   <si>
     <t>Adjust to Business Day</t>
   </si>
+  <si>
+    <t>acq_join</t>
+  </si>
+  <si>
+    <t>Concatenates the elements of a specified array using the specified separator (optional) between each element</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>acq_tostring</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>acq_count_unique</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1015,7 +1047,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1065,13 +1097,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
@@ -10281,10 +10315,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10294,13 +10328,13 @@
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -10309,16 +10343,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8024.36739</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1.3.8025.38970</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -10327,7 +10361,7 @@
         <v>D:\Github\ACQ\Distribution\ACQ64.xll</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -10336,7 +10370,7 @@
         <v>1.1.0.3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -10345,13 +10379,17 @@
         <v>4.0.30319.42000</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="H9" t="str">
+        <f>_xll.acq_join(C3:C11)</f>
+        <v>16,1.3.8025.38970,D:\Github\ACQ\Distribution\ACQ64.xll,1.1.0.3,4.0.30319.42000,,,Ctrl+Shift+H,Ctrl+Shift+A</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -10359,7 +10397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -10435,37 +10473,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="L2" s="47" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="L2" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="S2" s="47" t="s">
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="S2" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -11276,18 +11314,18 @@
       <c r="AI11" s="11"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="F12" s="49">
+      <c r="F12" s="47">
         <v>90</v>
       </c>
-      <c r="G12" s="49">
+      <c r="G12" s="47">
         <f>_xll.acq_options_black_price($C$4,F12,$C$6,$C$8,$C$7,TRUE)</f>
         <v>9.9783611447713145</v>
       </c>
-      <c r="H12" s="49">
+      <c r="H12" s="47">
         <f>_xll.acq_options_black_price($C$4,F12,$C$6,$C$8,$C$7,FALSE)</f>
         <v>9.9783611447713145</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I12" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -11640,16 +11678,16 @@
         <f>_xll.acq_options_black_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>0.65000000000000013</v>
       </c>
-      <c r="S17" s="47" t="s">
+      <c r="S17" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="47"/>
-      <c r="U17" s="47"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="47"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>0.2</v>
@@ -12830,37 +12868,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="L2" s="47" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="L2" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="S2" s="47" t="s">
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="S2" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -14035,16 +14073,16 @@
         <f>_xll.acq_options_bachelier_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>25.999999999962554</v>
       </c>
-      <c r="S17" s="47" t="s">
+      <c r="S17" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="47"/>
-      <c r="U17" s="47"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="47"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>20</v>
@@ -14921,14 +14959,14 @@
       </c>
     </row>
     <row r="32" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="47" t="s">
+      <c r="L32" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="47"/>
-      <c r="Q32" s="47"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
       <c r="AB32" t="s">
         <v>111</v>
       </c>
@@ -15588,37 +15626,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="L2" s="47" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="L2" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="S2" s="47" t="s">
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="S2" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
       <c r="AA2" s="37"/>
       <c r="AB2" s="37"/>
       <c r="AD2" s="3" t="s">
@@ -16895,16 +16933,16 @@
         <f>_xll.acq_options_blackscholes_vol($C$4,$C$5,$C$6,$C$8,$C$9,$N17,FALSE)</f>
         <v>0.65</v>
       </c>
-      <c r="S17" s="47" t="s">
+      <c r="S17" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="47"/>
-      <c r="U17" s="47"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="47"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
       <c r="AA17" s="37"/>
       <c r="AB17" s="37"/>
       <c r="AD17" s="16">
@@ -18527,15 +18565,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -18550,15 +18588,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="47"/>
+      <c r="J3" s="50"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -20324,26 +20362,26 @@
       <c r="Z29" s="46"/>
     </row>
     <row r="30" spans="6:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="47" t="s">
+      <c r="G30" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="S30" s="47" t="s">
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="S30" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="T30" s="47"/>
-      <c r="U30" s="47"/>
-      <c r="V30" s="47"/>
-      <c r="W30" s="47"/>
-      <c r="X30" s="47"/>
-      <c r="Y30" s="47"/>
-      <c r="Z30" s="47"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="50"/>
       <c r="AC30" t="s">
         <v>147</v>
       </c>
@@ -21567,26 +21605,26 @@
       <c r="AB44" s="46"/>
     </row>
     <row r="45" spans="6:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="47" t="s">
+      <c r="G45" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
-      <c r="M45" s="47"/>
-      <c r="N45" s="47"/>
-      <c r="S45" s="47" t="s">
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="S45" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="T45" s="47"/>
-      <c r="U45" s="47"/>
-      <c r="V45" s="47"/>
-      <c r="W45" s="47"/>
-      <c r="X45" s="47"/>
-      <c r="Y45" s="47"/>
-      <c r="Z45" s="47"/>
+      <c r="T45" s="50"/>
+      <c r="U45" s="50"/>
+      <c r="V45" s="50"/>
+      <c r="W45" s="50"/>
+      <c r="X45" s="50"/>
+      <c r="Y45" s="50"/>
+      <c r="Z45" s="50"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
     </row>
@@ -22459,10 +22497,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="B1:E26"/>
+  <dimension ref="B1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22820,6 +22858,33 @@
         <v>28</v>
       </c>
     </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -22829,6 +22894,170 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39FFD-CFD5-4286-8CBC-756067E23C33}">
+  <dimension ref="B2:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="5">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f>_xll.acq_tostring(C3)</f>
+        <v>3.14159265358979</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="48">
+        <f ca="1">TODAY()</f>
+        <v>44551</v>
+      </c>
+      <c r="E4" s="49" t="str">
+        <f ca="1">_xll.acq_tostring(C4)</f>
+        <v>44551</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f>_xll.acq_tostring(C5)</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="5" t="e">
+        <f>SQRT(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f>_xll.acq_tostring(C6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="E7" s="6" t="str">
+        <f>_xll.acq_tostring(C7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="5" t="e">
+        <f ca="1">DS()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f ca="1">_xll.acq_tostring(C8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f>_xll.acq_tostring(C9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="5" t="e">
+        <f>LOOKUP(C3,)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f>_xll.acq_tostring(C10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" t="str">
+        <f ca="1">_xll.acq_join(C3:C10)</f>
+        <v>3.14159265358979,44551,True,,,,,</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="str">
+        <f ca="1">_xll.acq_join(E3:E10, "|")</f>
+        <v>3.14159265358979|44551|TRUE|||||</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15">
+        <f ca="1">_xll.acq_count_unique(C3:C10)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16">
+        <f ca="1">_xll.acq_count_unique(C3:C10,FALSE)</f>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet7">
     <tabColor theme="2"/>

</xml_diff>

<commit_message>
added check for integer
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2272CC-374A-4857-880E-D4AF44F5CBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB75BDC4-C240-4203-93FD-416B0EE47185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -22,8 +22,7 @@
     <sheet name="TrinomialAmerican" sheetId="20" r:id="rId7"/>
     <sheet name="Comparison-American" sheetId="19" r:id="rId8"/>
     <sheet name="Description" sheetId="7" r:id="rId9"/>
-    <sheet name="Types" sheetId="17" r:id="rId10"/>
-    <sheet name="Special" sheetId="9" r:id="rId11"/>
+    <sheet name="Special" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -193,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="176">
   <si>
     <t>x</t>
   </si>
@@ -716,6 +715,12 @@
   <si>
     <t>Put Greeks: Trinomial Numerical Greeks</t>
   </si>
+  <si>
+    <t>acq_isprime</t>
+  </si>
+  <si>
+    <t>acq_isinteger</t>
+  </si>
 </sst>
 </file>
 
@@ -864,7 +869,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1074,6 +1079,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1088,7 +1136,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1144,6 +1192,9 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="3" fillId="3" borderId="2" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="3" fillId="3" borderId="17" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -13441,10 +13492,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13452,15 +13503,24 @@
     <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -13468,8 +13528,19 @@
         <f>_xll.acq_excel_version()</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>153</v>
+      </c>
+      <c r="L3" s="5">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="N3" s="6" t="str">
+        <f>_xll.acq_tostring(L3)</f>
+        <v>3.14159265358979</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -13477,8 +13548,19 @@
         <f>_xll.acq_version()</f>
         <v>1.3.8029.2058</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="48">
+        <f ca="1">TODAY()</f>
+        <v>44555</v>
+      </c>
+      <c r="N4" s="49" t="str">
+        <f ca="1">_xll.acq_tostring(L4)</f>
+        <v>44555</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -13486,8 +13568,18 @@
         <f>_xll.acq_xllpath()</f>
         <v>D:\Github\ACQ\Distribution\ACQ64.xll</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6" t="str">
+        <f>_xll.acq_tostring(L5)</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -13495,8 +13587,19 @@
         <f>_xll.acq_exceldna_version()</f>
         <v>1.1.0.3</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L6" s="5" t="e">
+        <f>SQRT(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N6" s="6" t="str">
+        <f>_xll.acq_tostring(L6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -13504,22 +13607,65 @@
         <f>_xll.acq_dotnet_version()</f>
         <v>4.0.30319.42000</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>155</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="N7" s="6" t="str">
+        <f>_xll.acq_tostring(L7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" s="5" t="e">
+        <f ca="1">DS()</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N8" s="6" t="str">
+        <f ca="1">_xll.acq_tostring(L8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>156</v>
+      </c>
+      <c r="L9" s="5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N9" s="6" t="str">
+        <f>_xll.acq_tostring(L9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>159</v>
+      </c>
+      <c r="L10" s="5" t="e">
+        <f>LOOKUP(L3,)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N10" s="6" t="str">
+        <f>_xll.acq_tostring(L10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -13527,13 +13673,49 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="L13" t="str">
+        <f ca="1">_xll.acq_join(L3:L10)</f>
+        <v>3.14159265358979,44555,True,,,,,</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="L14" t="str">
+        <f ca="1">_xll.acq_join(N3:N10, "|")</f>
+        <v>3.14159265358979|44555|TRUE|||||</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L15">
+        <f ca="1">_xll.acq_count_unique(L3:L10)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L16">
+        <f ca="1">_xll.acq_count_unique(L3:L10,FALSE)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
@@ -13541,7 +13723,7 @@
         <v>20150630</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
@@ -13549,8 +13731,16 @@
         <f>_xll.acq_convert_todate(C18)</f>
         <v>42185</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K19" s="19"/>
+      <c r="L19" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="N19" s="19"/>
+      <c r="O19" s="53" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>149</v>
       </c>
@@ -13558,14 +13748,152 @@
         <f>_xll.acq_nextbusinessday(C19)</f>
         <v>42186</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="K20" s="54">
+        <v>0</v>
+      </c>
+      <c r="L20" s="22" t="b">
+        <f>_xll.acq_isprime(K20)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="54">
+        <v>1</v>
+      </c>
+      <c r="O20" s="22" t="b">
+        <f>_xll.acq_isinteger(N20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C21" s="4">
         <f>_xll.acq_adjustbusinessday(C19,-1)</f>
         <v>42185</v>
+      </c>
+      <c r="K21" s="54">
+        <v>1</v>
+      </c>
+      <c r="L21" s="22" t="b">
+        <f>_xll.acq_isprime(K21)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="54">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="O21" s="22" t="b">
+        <f>_xll.acq_isinteger(N21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="54">
+        <v>2</v>
+      </c>
+      <c r="L22" s="22" t="b">
+        <f>_xll.acq_isprime(K22)</f>
+        <v>1</v>
+      </c>
+      <c r="N22" s="54" t="str">
+        <f>"text"</f>
+        <v>text</v>
+      </c>
+      <c r="O22" s="22" t="b">
+        <f>_xll.acq_isinteger(N22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="54">
+        <v>3</v>
+      </c>
+      <c r="L23" s="22" t="b">
+        <f>_xll.acq_isprime(K23)</f>
+        <v>1</v>
+      </c>
+      <c r="N23" s="54" t="str">
+        <f>"3.14"</f>
+        <v>3.14</v>
+      </c>
+      <c r="O23" s="22" t="b">
+        <f>_xll.acq_isinteger(N23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K24" s="54">
+        <v>4</v>
+      </c>
+      <c r="L24" s="22" t="b">
+        <f>_xll.acq_isprime(K24)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="54" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="O24" s="22" t="b">
+        <f>_xll.acq_isinteger(N24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K25" s="54">
+        <v>5</v>
+      </c>
+      <c r="L25" s="22" t="b">
+        <f>_xll.acq_isprime(K25)</f>
+        <v>1</v>
+      </c>
+      <c r="N25" s="54" t="str">
+        <f>"3.00"</f>
+        <v>3.00</v>
+      </c>
+      <c r="O25" s="22" t="b">
+        <f>_xll.acq_isinteger(N25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K26" s="54">
+        <v>6</v>
+      </c>
+      <c r="L26" s="22" t="b">
+        <f>_xll.acq_isprime(K26)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="54">
+        <v>2</v>
+      </c>
+      <c r="O26" s="22" t="b">
+        <f>_xll.acq_isinteger(N26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K27" s="55">
+        <v>7</v>
+      </c>
+      <c r="L27" s="24" t="b">
+        <f>_xll.acq_isprime(K27)</f>
+        <v>1</v>
+      </c>
+      <c r="N27" s="55">
+        <v>8</v>
+      </c>
+      <c r="O27" s="24" t="b">
+        <f>_xll.acq_isinteger(N27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K28" s="55">
+        <v>7.2</v>
+      </c>
+      <c r="L28" s="24" t="b">
+        <f>_xll.acq_isprime(K28)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -13575,171 +13903,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C39FFD-CFD5-4286-8CBC-756067E23C33}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="B2:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="5">
-        <f>PI()</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <f>_xll.acq_tostring(C3)</f>
-        <v>3.14159265358979</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="48">
-        <f ca="1">TODAY()</f>
-        <v>44555</v>
-      </c>
-      <c r="E4" s="49" t="str">
-        <f ca="1">_xll.acq_tostring(C4)</f>
-        <v>44555</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="str">
-        <f>_xll.acq_tostring(C5)</f>
-        <v>TRUE</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="5" t="e">
-        <f>SQRT(-1)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E6" s="6" t="str">
-        <f>_xll.acq_tostring(C6)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="E7" s="6" t="str">
-        <f>_xll.acq_tostring(C7)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="5" t="e">
-        <f ca="1">DS()</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E8" s="6" t="str">
-        <f ca="1">_xll.acq_tostring(C8)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E9" s="6" t="str">
-        <f>_xll.acq_tostring(C9)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" s="5" t="e">
-        <f>LOOKUP(C3,)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E10" s="6" t="str">
-        <f>_xll.acq_tostring(C10)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" t="str">
-        <f ca="1">_xll.acq_join(C3:C10)</f>
-        <v>3.14159265358979,44555,True,,,,,</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C14" t="str">
-        <f ca="1">_xll.acq_join(E3:E10, "|")</f>
-        <v>3.14159265358979|44555|TRUE|||||</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15">
-        <f ca="1">_xll.acq_count_unique(C3:C10)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16">
-        <f ca="1">_xll.acq_count_unique(C3:C10,FALSE)</f>
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet7">
     <tabColor theme="2"/>
@@ -22063,37 +22226,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="L2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="L2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="S2" s="53" t="s">
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="S2" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -23268,16 +23431,16 @@
         <f>_xll.acq_options_black_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>0.65000000000000013</v>
       </c>
-      <c r="S17" s="53" t="s">
+      <c r="S17" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
-      <c r="Y17" s="53"/>
-      <c r="Z17" s="53"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>0.2</v>
@@ -24458,37 +24621,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="L2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="L2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="S2" s="53" t="s">
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="S2" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -25663,16 +25826,16 @@
         <f>_xll.acq_options_bachelier_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>25.999999999962554</v>
       </c>
-      <c r="S17" s="53" t="s">
+      <c r="S17" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
-      <c r="Y17" s="53"/>
-      <c r="Z17" s="53"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>20</v>
@@ -26549,14 +26712,14 @@
       </c>
     </row>
     <row r="32" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="53" t="s">
+      <c r="L32" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="M32" s="53"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="53"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="53"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
       <c r="AB32" t="s">
         <v>111</v>
       </c>
@@ -27216,37 +27379,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="L2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="L2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="S2" s="53" t="s">
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="S2" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
       <c r="AA2" s="37"/>
       <c r="AB2" s="37"/>
       <c r="AD2" s="3" t="s">
@@ -28523,16 +28686,16 @@
         <f>_xll.acq_options_blackscholes_vol($C$4,$C$5,$C$6,$C$8,$C$9,$N17,FALSE)</f>
         <v>0.65</v>
       </c>
-      <c r="S17" s="53" t="s">
+      <c r="S17" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
-      <c r="Y17" s="53"/>
-      <c r="Z17" s="53"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
       <c r="AA17" s="37"/>
       <c r="AB17" s="37"/>
       <c r="AD17" s="16">
@@ -30156,15 +30319,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -30179,15 +30342,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53" t="s">
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="53"/>
+      <c r="J3" s="56"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -31946,26 +32109,26 @@
       <c r="Z29" s="46"/>
     </row>
     <row r="30" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="53"/>
-      <c r="S30" s="53" t="s">
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="S30" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
-      <c r="V30" s="53"/>
-      <c r="W30" s="53"/>
-      <c r="X30" s="53"/>
-      <c r="Y30" s="53"/>
-      <c r="Z30" s="53"/>
+      <c r="T30" s="56"/>
+      <c r="U30" s="56"/>
+      <c r="V30" s="56"/>
+      <c r="W30" s="56"/>
+      <c r="X30" s="56"/>
+      <c r="Y30" s="56"/>
+      <c r="Z30" s="56"/>
     </row>
     <row r="31" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
@@ -32834,26 +32997,26 @@
       <c r="AB44" s="46"/>
     </row>
     <row r="45" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="53" t="s">
+      <c r="G45" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="53"/>
-      <c r="S45" s="53" t="s">
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="S45" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="T45" s="53"/>
-      <c r="U45" s="53"/>
-      <c r="V45" s="53"/>
-      <c r="W45" s="53"/>
-      <c r="X45" s="53"/>
-      <c r="Y45" s="53"/>
-      <c r="Z45" s="53"/>
+      <c r="T45" s="56"/>
+      <c r="U45" s="56"/>
+      <c r="V45" s="56"/>
+      <c r="W45" s="56"/>
+      <c r="X45" s="56"/>
+      <c r="Y45" s="56"/>
+      <c r="Z45" s="56"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
     </row>
@@ -33742,15 +33905,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -33765,15 +33928,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53" t="s">
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="53"/>
+      <c r="J3" s="56"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -35530,26 +35693,26 @@
       <c r="Z29" s="46"/>
     </row>
     <row r="30" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="53"/>
-      <c r="S30" s="53" t="s">
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="S30" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
-      <c r="V30" s="53"/>
-      <c r="W30" s="53"/>
-      <c r="X30" s="53"/>
-      <c r="Y30" s="53"/>
-      <c r="Z30" s="53"/>
+      <c r="T30" s="56"/>
+      <c r="U30" s="56"/>
+      <c r="V30" s="56"/>
+      <c r="W30" s="56"/>
+      <c r="X30" s="56"/>
+      <c r="Y30" s="56"/>
+      <c r="Z30" s="56"/>
     </row>
     <row r="31" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
@@ -36418,26 +36581,26 @@
       <c r="AB44" s="46"/>
     </row>
     <row r="45" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="53" t="s">
+      <c r="G45" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="53"/>
-      <c r="S45" s="53" t="s">
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="S45" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="T45" s="53"/>
-      <c r="U45" s="53"/>
-      <c r="V45" s="53"/>
-      <c r="W45" s="53"/>
-      <c r="X45" s="53"/>
-      <c r="Y45" s="53"/>
-      <c r="Z45" s="53"/>
+      <c r="T45" s="56"/>
+      <c r="U45" s="56"/>
+      <c r="V45" s="56"/>
+      <c r="W45" s="56"/>
+      <c r="X45" s="56"/>
+      <c r="Y45" s="56"/>
+      <c r="Z45" s="56"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
     </row>
@@ -37321,15 +37484,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -37344,15 +37507,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53" t="s">
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="53"/>
+      <c r="J3" s="56"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -39125,26 +39288,26 @@
       <c r="Z29" s="46"/>
     </row>
     <row r="30" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="53"/>
-      <c r="S30" s="53" t="s">
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="S30" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
-      <c r="V30" s="53"/>
-      <c r="W30" s="53"/>
-      <c r="X30" s="53"/>
-      <c r="Y30" s="53"/>
-      <c r="Z30" s="53"/>
+      <c r="T30" s="56"/>
+      <c r="U30" s="56"/>
+      <c r="V30" s="56"/>
+      <c r="W30" s="56"/>
+      <c r="X30" s="56"/>
+      <c r="Y30" s="56"/>
+      <c r="Z30" s="56"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
@@ -40013,26 +40176,26 @@
       <c r="AB44" s="46"/>
     </row>
     <row r="45" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="53" t="s">
+      <c r="G45" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="53"/>
-      <c r="S45" s="53" t="s">
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="S45" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="T45" s="53"/>
-      <c r="U45" s="53"/>
-      <c r="V45" s="53"/>
-      <c r="W45" s="53"/>
-      <c r="X45" s="53"/>
-      <c r="Y45" s="53"/>
-      <c r="Z45" s="53"/>
+      <c r="T45" s="56"/>
+      <c r="U45" s="56"/>
+      <c r="V45" s="56"/>
+      <c r="W45" s="56"/>
+      <c r="X45" s="56"/>
+      <c r="Y45" s="56"/>
+      <c r="Z45" s="56"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
     </row>
@@ -40902,7 +41065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF3CA9D-20A9-4DB7-AD8A-F59DC22CC79A}">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -40920,15 +41083,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
       <c r="I1">
         <f>_xll.acq_options_binomial_american_price($C$5,F14,$C$7,$C$9,$C$10,$C$8,FALSE,6)</f>
         <v>20.986795441796307</v>
@@ -40940,40 +41103,40 @@
         <v>170</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53" t="s">
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53" t="s">
+      <c r="J3" s="56"/>
+      <c r="K3" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53" t="s">
+      <c r="L3" s="56"/>
+      <c r="M3" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="N3" s="53"/>
-      <c r="P3" s="53" t="s">
+      <c r="N3" s="56"/>
+      <c r="P3" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53" t="s">
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53" t="s">
+      <c r="T3" s="56"/>
+      <c r="U3" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53" t="s">
+      <c r="V3" s="56"/>
+      <c r="W3" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="X3" s="53"/>
+      <c r="X3" s="56"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">

</xml_diff>

<commit_message>
refactored binomial option pricer to take general payoff function
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB75BDC4-C240-4203-93FD-416B0EE47185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966F6409-9B89-4490-9BCC-F8A0CED33039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="825" windowWidth="24465" windowHeight="12840" tabRatio="900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="176">
   <si>
     <t>x</t>
   </si>
@@ -13494,7 +13494,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -13546,7 +13546,7 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8029.2058</v>
+        <v>1.3.8029.25470</v>
       </c>
       <c r="K4" t="s">
         <v>1</v>
@@ -33889,10 +33889,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A153B6B9-5563-4A5A-994F-A4DB117E644D}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:AB57"/>
+  <dimension ref="A1:AT57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33904,7 +33904,7 @@
     <col min="31" max="31" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
         <v>162</v>
       </c>
@@ -33915,15 +33915,21 @@
       <c r="F1" s="57"/>
       <c r="G1" s="57"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
         <v>140</v>
       </c>
       <c r="U2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>92</v>
       </c>
@@ -33943,8 +33949,14 @@
       <c r="V3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AE3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>124</v>
       </c>
@@ -34014,8 +34026,56 @@
       <c r="AB4" s="43">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE4">
+        <v>120</v>
+      </c>
+      <c r="AF4">
+        <v>130</v>
+      </c>
+      <c r="AG4">
+        <v>140</v>
+      </c>
+      <c r="AH4">
+        <v>150</v>
+      </c>
+      <c r="AI4">
+        <v>160</v>
+      </c>
+      <c r="AJ4">
+        <v>170</v>
+      </c>
+      <c r="AK4">
+        <v>180</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN4">
+        <v>120</v>
+      </c>
+      <c r="AO4">
+        <v>130</v>
+      </c>
+      <c r="AP4">
+        <v>140</v>
+      </c>
+      <c r="AQ4">
+        <v>150</v>
+      </c>
+      <c r="AR4">
+        <v>160</v>
+      </c>
+      <c r="AS4">
+        <v>170</v>
+      </c>
+      <c r="AT4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>87</v>
       </c>
@@ -34103,8 +34163,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U5,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.1233079681879743E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD5">
+        <v>0.05</v>
+      </c>
+      <c r="AE5">
+        <v>6.47885622121005E-5</v>
+      </c>
+      <c r="AF5">
+        <v>1.4806633008807357E-2</v>
+      </c>
+      <c r="AG5">
+        <v>0.46327538134639434</v>
+      </c>
+      <c r="AH5">
+        <v>3.5277905365628364</v>
+      </c>
+      <c r="AI5">
+        <v>10.854397955373866</v>
+      </c>
+      <c r="AJ5">
+        <v>20.398245605225771</v>
+      </c>
+      <c r="AK5">
+        <v>30.360468484994357</v>
+      </c>
+      <c r="AM5">
+        <v>0.05</v>
+      </c>
+      <c r="AN5">
+        <v>30.000000000007944</v>
+      </c>
+      <c r="AO5">
+        <v>20.000000000008811</v>
+      </c>
+      <c r="AP5">
+        <v>10.226132459460437</v>
+      </c>
+      <c r="AQ5">
+        <v>3.1790029284836754</v>
+      </c>
+      <c r="AR5">
+        <v>0.48754530179488176</v>
+      </c>
+      <c r="AS5">
+        <v>3.4019614928197786E-2</v>
+      </c>
+      <c r="AT5">
+        <v>1.1233079681879743E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>88</v>
       </c>
@@ -34192,8 +34300,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U6,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.8583844005032689E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD6">
+        <v>0.1</v>
+      </c>
+      <c r="AE6">
+        <v>9.1248830034959434E-3</v>
+      </c>
+      <c r="AF6">
+        <v>0.17885106898621184</v>
+      </c>
+      <c r="AG6">
+        <v>1.3493143126169751</v>
+      </c>
+      <c r="AH6">
+        <v>5.093879400981173</v>
+      </c>
+      <c r="AI6">
+        <v>12.008481773814808</v>
+      </c>
+      <c r="AJ6">
+        <v>20.989035434736152</v>
+      </c>
+      <c r="AK6">
+        <v>30.755768827066532</v>
+      </c>
+      <c r="AM6">
+        <v>0.1</v>
+      </c>
+      <c r="AN6">
+        <v>29.999999999996874</v>
+      </c>
+      <c r="AO6">
+        <v>19.999999999996476</v>
+      </c>
+      <c r="AP6">
+        <v>10.797609727004986</v>
+      </c>
+      <c r="AQ6">
+        <v>4.4028779916287712</v>
+      </c>
+      <c r="AR6">
+        <v>1.2825833785772736</v>
+      </c>
+      <c r="AS6">
+        <v>0.26342580573432217</v>
+      </c>
+      <c r="AT6">
+        <v>3.8583844005032689E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>89</v>
       </c>
@@ -34281,8 +34437,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U7,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.14956122530436966</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD7">
+        <v>0.15</v>
+      </c>
+      <c r="AE7">
+        <v>5.8077899595978963E-2</v>
+      </c>
+      <c r="AF7">
+        <v>0.49244708697616602</v>
+      </c>
+      <c r="AG7">
+        <v>2.2192034827575045</v>
+      </c>
+      <c r="AH7">
+        <v>6.3354932334738869</v>
+      </c>
+      <c r="AI7">
+        <v>13.082256699580331</v>
+      </c>
+      <c r="AJ7">
+        <v>21.691322996615757</v>
+      </c>
+      <c r="AK7">
+        <v>31.222516029227904</v>
+      </c>
+      <c r="AM7">
+        <v>0.15</v>
+      </c>
+      <c r="AN7">
+        <v>30.000000000002515</v>
+      </c>
+      <c r="AO7">
+        <v>20.027854351695026</v>
+      </c>
+      <c r="AP7">
+        <v>11.353356804736338</v>
+      </c>
+      <c r="AQ7">
+        <v>5.3062813983176547</v>
+      </c>
+      <c r="AR7">
+        <v>2.0030892793519759</v>
+      </c>
+      <c r="AS7">
+        <v>0.60807550371991215</v>
+      </c>
+      <c r="AT7">
+        <v>0.14956122530436966</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>90</v>
       </c>
@@ -34370,8 +34574,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U8,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.3201665321074566</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD8">
+        <v>0.2</v>
+      </c>
+      <c r="AE8">
+        <v>0.16136804829456403</v>
+      </c>
+      <c r="AF8">
+        <v>0.8860473909070643</v>
+      </c>
+      <c r="AG8">
+        <v>3.0435348720524895</v>
+      </c>
+      <c r="AH8">
+        <v>7.4083750302895854</v>
+      </c>
+      <c r="AI8">
+        <v>14.068853304358285</v>
+      </c>
+      <c r="AJ8">
+        <v>22.426190917393427</v>
+      </c>
+      <c r="AK8">
+        <v>31.746454818833193</v>
+      </c>
+      <c r="AM8">
+        <v>0.2</v>
+      </c>
+      <c r="AN8">
+        <v>29.999999999993349</v>
+      </c>
+      <c r="AO8">
+        <v>20.13073400794984</v>
+      </c>
+      <c r="AP8">
+        <v>11.863106149450129</v>
+      </c>
+      <c r="AQ8">
+        <v>6.0442186276654537</v>
+      </c>
+      <c r="AR8">
+        <v>2.6409942086201346</v>
+      </c>
+      <c r="AS8">
+        <v>0.98906799961525138</v>
+      </c>
+      <c r="AT8">
+        <v>0.3201665321074566</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>123</v>
       </c>
@@ -34459,8 +34711,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U9,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.52750606510265219</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD9">
+        <v>0.25</v>
+      </c>
+      <c r="AE9">
+        <v>0.31325094901697909</v>
+      </c>
+      <c r="AF9">
+        <v>1.3206650122883798</v>
+      </c>
+      <c r="AG9">
+        <v>3.8215367979400421</v>
+      </c>
+      <c r="AH9">
+        <v>8.3729100913056413</v>
+      </c>
+      <c r="AI9">
+        <v>14.984356354747003</v>
+      </c>
+      <c r="AJ9">
+        <v>23.161178919125021</v>
+      </c>
+      <c r="AK9">
+        <v>32.304511439276084</v>
+      </c>
+      <c r="AM9">
+        <v>0.25</v>
+      </c>
+      <c r="AN9">
+        <v>30.0000000000028</v>
+      </c>
+      <c r="AO9">
+        <v>20.274504805299543</v>
+      </c>
+      <c r="AP9">
+        <v>12.327876459814949</v>
+      </c>
+      <c r="AQ9">
+        <v>6.6766919114698968</v>
+      </c>
+      <c r="AR9">
+        <v>3.2120003339687822</v>
+      </c>
+      <c r="AS9">
+        <v>1.3736497278310844</v>
+      </c>
+      <c r="AT9">
+        <v>0.52750606510265219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>91</v>
       </c>
@@ -34548,8 +34848,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U10,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.75487996900595666</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD10">
+        <v>0.3</v>
+      </c>
+      <c r="AE10">
+        <v>0.50723351768046687</v>
+      </c>
+      <c r="AF10">
+        <v>1.7778898294447549</v>
+      </c>
+      <c r="AG10">
+        <v>4.5610278170178651</v>
+      </c>
+      <c r="AH10">
+        <v>9.2600973651020233</v>
+      </c>
+      <c r="AI10">
+        <v>15.845950364108626</v>
+      </c>
+      <c r="AJ10">
+        <v>23.88749944641949</v>
+      </c>
+      <c r="AK10">
+        <v>32.87973756386954</v>
+      </c>
+      <c r="AM10">
+        <v>0.3</v>
+      </c>
+      <c r="AN10">
+        <v>30.000000000002743</v>
+      </c>
+      <c r="AO10">
+        <v>20.440193582355914</v>
+      </c>
+      <c r="AP10">
+        <v>12.754290425942102</v>
+      </c>
+      <c r="AQ10">
+        <v>7.2344336704707839</v>
+      </c>
+      <c r="AR10">
+        <v>3.7317306145519544</v>
+      </c>
+      <c r="AS10">
+        <v>1.7527580521189718</v>
+      </c>
+      <c r="AT10">
+        <v>0.75487996900595666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>161</v>
       </c>
@@ -34638,8 +34986,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U11,$C$8,$C$9,$C$7,FALSE)</f>
         <v>0.99553681262010585</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD11">
+        <v>0.35</v>
+      </c>
+      <c r="AE11">
+        <v>0.73125251323826879</v>
+      </c>
+      <c r="AF11">
+        <v>2.2425629675526668</v>
+      </c>
+      <c r="AG11">
+        <v>5.2618578149379438</v>
+      </c>
+      <c r="AH11">
+        <v>10.08836927608</v>
+      </c>
+      <c r="AI11">
+        <v>16.658382519599211</v>
+      </c>
+      <c r="AJ11">
+        <v>24.600440523935646</v>
+      </c>
+      <c r="AK11">
+        <v>33.465938073747651</v>
+      </c>
+      <c r="AM11">
+        <v>0.35</v>
+      </c>
+      <c r="AN11">
+        <v>29.999999999996248</v>
+      </c>
+      <c r="AO11">
+        <v>20.614981977575212</v>
+      </c>
+      <c r="AP11">
+        <v>13.14532203793252</v>
+      </c>
+      <c r="AQ11">
+        <v>7.735689758679209</v>
+      </c>
+      <c r="AR11">
+        <v>4.2065120657730173</v>
+      </c>
+      <c r="AS11">
+        <v>2.1214486509235293</v>
+      </c>
+      <c r="AT11">
+        <v>0.99553681262010585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>80</v>
       </c>
@@ -34721,8 +35117,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U12,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.2394163077110454</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD12">
+        <v>0.4</v>
+      </c>
+      <c r="AE12">
+        <v>0.98074725352978653</v>
+      </c>
+      <c r="AF12">
+        <v>2.7108623936882199</v>
+      </c>
+      <c r="AG12">
+        <v>5.9331503559943091</v>
+      </c>
+      <c r="AH12">
+        <v>10.869747155346124</v>
+      </c>
+      <c r="AI12">
+        <v>17.439320147336176</v>
+      </c>
+      <c r="AJ12">
+        <v>25.292119275335775</v>
+      </c>
+      <c r="AK12">
+        <v>34.052619910449579</v>
+      </c>
+      <c r="AM12">
+        <v>0.4</v>
+      </c>
+      <c r="AN12">
+        <v>29.999999999999787</v>
+      </c>
+      <c r="AO12">
+        <v>20.79423171930236</v>
+      </c>
+      <c r="AP12">
+        <v>13.507534862877332</v>
+      </c>
+      <c r="AQ12">
+        <v>8.1923374611286697</v>
+      </c>
+      <c r="AR12">
+        <v>4.6510025026004902</v>
+      </c>
+      <c r="AS12">
+        <v>2.4723128103769398</v>
+      </c>
+      <c r="AT12">
+        <v>1.2394163077110454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>90</v>
       </c>
@@ -34804,8 +35248,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U13,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.4858297365660946</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD13">
+        <v>0.45</v>
+      </c>
+      <c r="AE13">
+        <v>1.2470004782783017</v>
+      </c>
+      <c r="AF13">
+        <v>3.1843266342166752</v>
+      </c>
+      <c r="AG13">
+        <v>6.5857879830962656</v>
+      </c>
+      <c r="AH13">
+        <v>11.612589204012622</v>
+      </c>
+      <c r="AI13">
+        <v>18.18171358281873</v>
+      </c>
+      <c r="AJ13">
+        <v>25.972533818763516</v>
+      </c>
+      <c r="AK13">
+        <v>34.63989179675373</v>
+      </c>
+      <c r="AM13">
+        <v>0.45</v>
+      </c>
+      <c r="AN13">
+        <v>29.999999999992809</v>
+      </c>
+      <c r="AO13">
+        <v>20.976031447468223</v>
+      </c>
+      <c r="AP13">
+        <v>13.850939518869161</v>
+      </c>
+      <c r="AQ13">
+        <v>8.6126322014121452</v>
+      </c>
+      <c r="AR13">
+        <v>5.0602658139661454</v>
+      </c>
+      <c r="AS13">
+        <v>2.8133889019011615</v>
+      </c>
+      <c r="AT13">
+        <v>1.4858297365660946</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>100</v>
       </c>
@@ -34887,8 +35379,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U14,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.7335499493219952</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD14">
+        <v>0.5</v>
+      </c>
+      <c r="AE14">
+        <v>1.5281847509030895</v>
+      </c>
+      <c r="AF14">
+        <v>3.6455355589481657</v>
+      </c>
+      <c r="AG14">
+        <v>7.2111511027985165</v>
+      </c>
+      <c r="AH14">
+        <v>12.322987010315092</v>
+      </c>
+      <c r="AI14">
+        <v>18.891665822159915</v>
+      </c>
+      <c r="AJ14">
+        <v>26.629771214566016</v>
+      </c>
+      <c r="AK14">
+        <v>35.225855437579256</v>
+      </c>
+      <c r="AM14">
+        <v>0.5</v>
+      </c>
+      <c r="AN14">
+        <v>30.01357994271202</v>
+      </c>
+      <c r="AO14">
+        <v>21.15200671396223</v>
+      </c>
+      <c r="AP14">
+        <v>14.170235970354575</v>
+      </c>
+      <c r="AQ14">
+        <v>9.0025754232218205</v>
+      </c>
+      <c r="AR14">
+        <v>5.440504492483285</v>
+      </c>
+      <c r="AS14">
+        <v>3.1354763991069881</v>
+      </c>
+      <c r="AT14">
+        <v>1.7335499493219952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>110</v>
       </c>
@@ -34970,8 +35510,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U15,$C$8,$C$9,$C$7,FALSE)</f>
         <v>1.9708398941787317</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AE15">
+        <v>1.8239007301477845</v>
+      </c>
+      <c r="AF15">
+        <v>4.1151087291769262</v>
+      </c>
+      <c r="AG15">
+        <v>7.813111808473657</v>
+      </c>
+      <c r="AH15">
+        <v>13.005543865476119</v>
+      </c>
+      <c r="AI15">
+        <v>19.5823066688422</v>
+      </c>
+      <c r="AJ15">
+        <v>27.281215949496463</v>
+      </c>
+      <c r="AK15">
+        <v>35.798090255173449</v>
+      </c>
+      <c r="AM15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AN15">
+        <v>30.038544836649557</v>
+      </c>
+      <c r="AO15">
+        <v>21.330445738968635</v>
+      </c>
+      <c r="AP15">
+        <v>14.468681374332336</v>
+      </c>
+      <c r="AQ15">
+        <v>9.3666840898581079</v>
+      </c>
+      <c r="AR15">
+        <v>5.8034874671570558</v>
+      </c>
+      <c r="AS15">
+        <v>3.4522522165303364</v>
+      </c>
+      <c r="AT15">
+        <v>1.9708398941787317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>120</v>
       </c>
@@ -35053,8 +35641,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U16,$C$8,$C$9,$C$7,FALSE)</f>
         <v>2.2146665611764895</v>
       </c>
-    </row>
-    <row r="17" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD16">
+        <v>0.6</v>
+      </c>
+      <c r="AE16">
+        <v>2.1215661214389336</v>
+      </c>
+      <c r="AF16">
+        <v>4.5729995607255551</v>
+      </c>
+      <c r="AG16">
+        <v>8.3961077286980821</v>
+      </c>
+      <c r="AH16">
+        <v>13.663839736257879</v>
+      </c>
+      <c r="AI16">
+        <v>20.254066648520276</v>
+      </c>
+      <c r="AJ16">
+        <v>27.910096953130402</v>
+      </c>
+      <c r="AK16">
+        <v>36.376463582641435</v>
+      </c>
+      <c r="AM16">
+        <v>0.6</v>
+      </c>
+      <c r="AN16">
+        <v>30.070414645125808</v>
+      </c>
+      <c r="AO16">
+        <v>21.502433988306827</v>
+      </c>
+      <c r="AP16">
+        <v>14.749679016584579</v>
+      </c>
+      <c r="AQ16">
+        <v>9.7084828669159471</v>
+      </c>
+      <c r="AR16">
+        <v>6.1485117480984979</v>
+      </c>
+      <c r="AS16">
+        <v>3.7497888277682891</v>
+      </c>
+      <c r="AT16">
+        <v>2.2146665611764895</v>
+      </c>
+    </row>
+    <row r="17" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>130</v>
       </c>
@@ -35136,8 +35772,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U17,$C$8,$C$9,$C$7,FALSE)</f>
         <v>2.4447713399422337</v>
       </c>
-    </row>
-    <row r="18" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD17">
+        <v>0.65</v>
+      </c>
+      <c r="AE17">
+        <v>2.4322564265597215</v>
+      </c>
+      <c r="AF17">
+        <v>5.0224921872256481</v>
+      </c>
+      <c r="AG17">
+        <v>8.9736290576865478</v>
+      </c>
+      <c r="AH17">
+        <v>14.300724555368561</v>
+      </c>
+      <c r="AI17">
+        <v>20.903720858487453</v>
+      </c>
+      <c r="AJ17">
+        <v>28.523264212015864</v>
+      </c>
+      <c r="AK17">
+        <v>36.937673160665199</v>
+      </c>
+      <c r="AM17">
+        <v>0.65</v>
+      </c>
+      <c r="AN17">
+        <v>30.111791078120248</v>
+      </c>
+      <c r="AO17">
+        <v>21.668180784889717</v>
+      </c>
+      <c r="AP17">
+        <v>15.022913971768219</v>
+      </c>
+      <c r="AQ17">
+        <v>10.030755857159793</v>
+      </c>
+      <c r="AR17">
+        <v>6.4738643533267375</v>
+      </c>
+      <c r="AS17">
+        <v>4.0351902216613516</v>
+      </c>
+      <c r="AT17">
+        <v>2.4447713399422337</v>
+      </c>
+    </row>
+    <row r="18" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>140</v>
       </c>
@@ -35219,8 +35903,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U18,$C$8,$C$9,$C$7,FALSE)</f>
         <v>2.6769358533655034</v>
       </c>
-    </row>
-    <row r="19" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD18">
+        <v>0.7</v>
+      </c>
+      <c r="AE18">
+        <v>2.7398970024350779</v>
+      </c>
+      <c r="AF18">
+        <v>5.4783444827316536</v>
+      </c>
+      <c r="AG18">
+        <v>9.5345453500097577</v>
+      </c>
+      <c r="AH18">
+        <v>14.918511496002189</v>
+      </c>
+      <c r="AI18">
+        <v>21.533662877514285</v>
+      </c>
+      <c r="AJ18">
+        <v>29.133690903382561</v>
+      </c>
+      <c r="AK18">
+        <v>37.498997043070389</v>
+      </c>
+      <c r="AM18">
+        <v>0.7</v>
+      </c>
+      <c r="AN18">
+        <v>30.155643983820472</v>
+      </c>
+      <c r="AO18">
+        <v>21.835712678340293</v>
+      </c>
+      <c r="AP18">
+        <v>15.282133973957995</v>
+      </c>
+      <c r="AQ18">
+        <v>10.33578045914636</v>
+      </c>
+      <c r="AR18">
+        <v>6.7818740437543577</v>
+      </c>
+      <c r="AS18">
+        <v>4.3176119877586281</v>
+      </c>
+      <c r="AT18">
+        <v>2.6769358533655034</v>
+      </c>
+    </row>
+    <row r="19" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>150</v>
       </c>
@@ -35302,8 +36034,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U19,$C$8,$C$9,$C$7,FALSE)</f>
         <v>2.9022681246916715</v>
       </c>
-    </row>
-    <row r="20" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD19">
+        <v>0.75</v>
+      </c>
+      <c r="AE19">
+        <v>3.0612500938520979</v>
+      </c>
+      <c r="AF19">
+        <v>5.9229778472484842</v>
+      </c>
+      <c r="AG19">
+        <v>10.080514227124009</v>
+      </c>
+      <c r="AH19">
+        <v>15.519109012187322</v>
+      </c>
+      <c r="AI19">
+        <v>22.14586732772327</v>
+      </c>
+      <c r="AJ19">
+        <v>29.727218566263986</v>
+      </c>
+      <c r="AK19">
+        <v>38.052083397046495</v>
+      </c>
+      <c r="AM19">
+        <v>0.75</v>
+      </c>
+      <c r="AN19">
+        <v>30.207232228449922</v>
+      </c>
+      <c r="AO19">
+        <v>21.996417380647536</v>
+      </c>
+      <c r="AP19">
+        <v>15.528497549570506</v>
+      </c>
+      <c r="AQ19">
+        <v>10.625411692111369</v>
+      </c>
+      <c r="AR19">
+        <v>7.0745178030450688</v>
+      </c>
+      <c r="AS19">
+        <v>4.5857815788687404</v>
+      </c>
+      <c r="AT19">
+        <v>2.9022681246916715</v>
+      </c>
+    </row>
+    <row r="20" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>160</v>
       </c>
@@ -35385,8 +36165,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U20,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.1172324099143998</v>
       </c>
-    </row>
-    <row r="21" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD20">
+        <v>0.8</v>
+      </c>
+      <c r="AE20">
+        <v>3.3760679090846142</v>
+      </c>
+      <c r="AF20">
+        <v>6.3574367666391716</v>
+      </c>
+      <c r="AG20">
+        <v>10.612922302756481</v>
+      </c>
+      <c r="AH20">
+        <v>16.104113814319668</v>
+      </c>
+      <c r="AI20">
+        <v>22.741986135096859</v>
+      </c>
+      <c r="AJ20">
+        <v>30.305423594084502</v>
+      </c>
+      <c r="AK20">
+        <v>38.591643807770645</v>
+      </c>
+      <c r="AM20">
+        <v>0.8</v>
+      </c>
+      <c r="AN20">
+        <v>30.259373769473957</v>
+      </c>
+      <c r="AO20">
+        <v>22.150453437182545</v>
+      </c>
+      <c r="AP20">
+        <v>15.763230324066519</v>
+      </c>
+      <c r="AQ20">
+        <v>10.90120779543015</v>
+      </c>
+      <c r="AR20">
+        <v>7.3533355204141024</v>
+      </c>
+      <c r="AS20">
+        <v>4.8413869253896635</v>
+      </c>
+      <c r="AT20">
+        <v>3.1172324099143998</v>
+      </c>
+    </row>
+    <row r="21" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>170</v>
       </c>
@@ -35468,8 +36296,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U21,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.3329533106290485</v>
       </c>
-    </row>
-    <row r="22" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD21">
+        <v>0.85</v>
+      </c>
+      <c r="AE21">
+        <v>3.6970934807160312</v>
+      </c>
+      <c r="AF21">
+        <v>6.7878683966650888</v>
+      </c>
+      <c r="AG21">
+        <v>11.13294360230978</v>
+      </c>
+      <c r="AH21">
+        <v>16.674878044259088</v>
+      </c>
+      <c r="AI21">
+        <v>23.323418075877768</v>
+      </c>
+      <c r="AJ21">
+        <v>30.869640468009369</v>
+      </c>
+      <c r="AK21">
+        <v>39.130007454034043</v>
+      </c>
+      <c r="AM21">
+        <v>0.85</v>
+      </c>
+      <c r="AN21">
+        <v>30.314573182467761</v>
+      </c>
+      <c r="AO21">
+        <v>22.300254774455361</v>
+      </c>
+      <c r="AP21">
+        <v>15.987414079511197</v>
+      </c>
+      <c r="AQ21">
+        <v>11.164487628573138</v>
+      </c>
+      <c r="AR21">
+        <v>7.6197810921715865</v>
+      </c>
+      <c r="AS21">
+        <v>5.085975020532258</v>
+      </c>
+      <c r="AT21">
+        <v>3.3329533106290485</v>
+      </c>
+    </row>
+    <row r="22" spans="6:46" x14ac:dyDescent="0.25">
       <c r="L22" s="45">
         <v>0.9</v>
       </c>
@@ -35532,8 +36408,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U22,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.5451577697247849</v>
       </c>
-    </row>
-    <row r="23" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD22">
+        <v>0.9</v>
+      </c>
+      <c r="AE22">
+        <v>4.0226096355607233</v>
+      </c>
+      <c r="AF22">
+        <v>7.2227377546292395</v>
+      </c>
+      <c r="AG22">
+        <v>11.641582714736746</v>
+      </c>
+      <c r="AH22">
+        <v>17.232558898229541</v>
+      </c>
+      <c r="AI22">
+        <v>23.891360149612545</v>
+      </c>
+      <c r="AJ22">
+        <v>31.42992022819066</v>
+      </c>
+      <c r="AK22">
+        <v>39.664294213456529</v>
+      </c>
+      <c r="AM22">
+        <v>0.9</v>
+      </c>
+      <c r="AN22">
+        <v>30.373679070968116</v>
+      </c>
+      <c r="AO22">
+        <v>22.450948798364585</v>
+      </c>
+      <c r="AP22">
+        <v>16.201952543951933</v>
+      </c>
+      <c r="AQ22">
+        <v>11.416371229360646</v>
+      </c>
+      <c r="AR22">
+        <v>7.8750764808474587</v>
+      </c>
+      <c r="AS22">
+        <v>5.3280983055611504</v>
+      </c>
+      <c r="AT22">
+        <v>3.5451577697247849</v>
+      </c>
+    </row>
+    <row r="23" spans="6:46" x14ac:dyDescent="0.25">
       <c r="L23" s="45">
         <v>0.95</v>
       </c>
@@ -35596,8 +36520,56 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U23,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.7486766576694794</v>
       </c>
-    </row>
-    <row r="24" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD23">
+        <v>0.95</v>
+      </c>
+      <c r="AE23">
+        <v>4.3425600360567156</v>
+      </c>
+      <c r="AF23">
+        <v>7.6492287010063276</v>
+      </c>
+      <c r="AG23">
+        <v>12.13970728885575</v>
+      </c>
+      <c r="AH23">
+        <v>17.778155998949195</v>
+      </c>
+      <c r="AI23">
+        <v>24.450872926370785</v>
+      </c>
+      <c r="AJ23">
+        <v>31.983975075847844</v>
+      </c>
+      <c r="AK23">
+        <v>40.187331898399165</v>
+      </c>
+      <c r="AM23">
+        <v>0.95</v>
+      </c>
+      <c r="AN23">
+        <v>30.432535843598799</v>
+      </c>
+      <c r="AO23">
+        <v>22.596386076654408</v>
+      </c>
+      <c r="AP23">
+        <v>16.407639013932588</v>
+      </c>
+      <c r="AQ23">
+        <v>11.657828910294933</v>
+      </c>
+      <c r="AR23">
+        <v>8.1234766093562545</v>
+      </c>
+      <c r="AS23">
+        <v>5.5642994016355161</v>
+      </c>
+      <c r="AT23">
+        <v>3.7486766576694794</v>
+      </c>
+    </row>
+    <row r="24" spans="6:46" x14ac:dyDescent="0.25">
       <c r="L24" s="45">
         <v>1</v>
       </c>
@@ -35660,14 +36632,118 @@
         <f>_xll.acq_options_binomial_american_price(AB$4,$C$5,$U24,$C$8,$C$9,$C$7,FALSE)</f>
         <v>3.9444600804233492</v>
       </c>
-    </row>
-    <row r="26" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AD24">
+        <v>1</v>
+      </c>
+      <c r="AE24">
+        <v>4.6590187874285469</v>
+      </c>
+      <c r="AF24">
+        <v>8.0679435144803957</v>
+      </c>
+      <c r="AG24">
+        <v>12.628072924725879</v>
+      </c>
+      <c r="AH24">
+        <v>18.312540023842111</v>
+      </c>
+      <c r="AI24">
+        <v>25.002843572928668</v>
+      </c>
+      <c r="AJ24">
+        <v>32.526481100177023</v>
+      </c>
+      <c r="AK24">
+        <v>40.699934502208627</v>
+      </c>
+      <c r="AM24">
+        <v>1</v>
+      </c>
+      <c r="AN24">
+        <v>30.49070965005788</v>
+      </c>
+      <c r="AO24">
+        <v>22.73665926882417</v>
+      </c>
+      <c r="AP24">
+        <v>16.605190083791207</v>
+      </c>
+      <c r="AQ24">
+        <v>11.889697305262722</v>
+      </c>
+      <c r="AR24">
+        <v>8.3645040630454659</v>
+      </c>
+      <c r="AS24">
+        <v>5.7911212518975752</v>
+      </c>
+      <c r="AT24">
+        <v>3.9444600804233492</v>
+      </c>
+    </row>
+    <row r="26" spans="6:46" x14ac:dyDescent="0.25">
       <c r="V26" s="46"/>
       <c r="W26" s="46"/>
       <c r="X26" s="46"/>
       <c r="Y26" s="46"/>
-    </row>
-    <row r="27" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE26">
+        <f>AE5-M5</f>
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <f t="shared" ref="AF26:AJ26" si="0">AF5-N5</f>
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <f t="shared" ref="AK26:AK45" si="1">AK5-S5</f>
+        <v>0</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" ref="AN26:AT26" si="2">AN5-V5</f>
+        <v>0</v>
+      </c>
+      <c r="AO26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AQ26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AR26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AS26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AT26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="6:46" x14ac:dyDescent="0.25">
       <c r="S27">
         <f>_xll.acq_options_bjerksund_price($F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>6.1672981556468613</v>
@@ -35677,22 +36753,190 @@
       <c r="X27" s="46"/>
       <c r="Y27" s="46"/>
       <c r="Z27" s="46"/>
-    </row>
-    <row r="28" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE27">
+        <f t="shared" ref="AE27:AE43" si="3">AE6-M6</f>
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <f t="shared" ref="AF27:AF43" si="4">AF6-N6</f>
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <f t="shared" ref="AG27:AG43" si="5">AG6-O6</f>
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <f t="shared" ref="AH27:AH43" si="6">AH6-P6</f>
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <f t="shared" ref="AI27:AI43" si="7">AI6-Q6</f>
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <f t="shared" ref="AJ27:AJ43" si="8">AJ6-R6</f>
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <f t="shared" ref="AN27:AT27" si="9">AN6-V6</f>
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AQ27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AR27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AS27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AT27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="6:46" x14ac:dyDescent="0.25">
       <c r="V28" s="46"/>
       <c r="W28" s="46"/>
       <c r="X28" s="46"/>
       <c r="Y28" s="46"/>
       <c r="Z28" s="46"/>
-    </row>
-    <row r="29" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN28">
+        <f t="shared" ref="AN28:AT28" si="10">AN7-V7</f>
+        <v>0</v>
+      </c>
+      <c r="AO28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AP28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AQ28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AR28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AS28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AT28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="6:46" x14ac:dyDescent="0.25">
       <c r="V29" s="46"/>
       <c r="W29" s="46"/>
       <c r="X29" s="46"/>
       <c r="Y29" s="46"/>
       <c r="Z29" s="46"/>
-    </row>
-    <row r="30" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN29">
+        <f t="shared" ref="AN29:AT29" si="11">AN8-V8</f>
+        <v>0</v>
+      </c>
+      <c r="AO29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AP29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AQ29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AS29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="56" t="s">
         <v>164</v>
       </c>
@@ -35713,8 +36957,64 @@
       <c r="X30" s="56"/>
       <c r="Y30" s="56"/>
       <c r="Z30" s="56"/>
-    </row>
-    <row r="31" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" ref="AN30:AT30" si="12">AN9-V9</f>
+        <v>0</v>
+      </c>
+      <c r="AO30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AR30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AS30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AT30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>125</v>
       </c>
@@ -35769,8 +37069,64 @@
       <c r="Z31" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="32" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" ref="AN31:AT31" si="13">AN10-V10</f>
+        <v>0</v>
+      </c>
+      <c r="AO31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AQ31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AR31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AS31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AT31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F32" s="13">
         <v>100</v>
       </c>
@@ -35841,8 +37197,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F32,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-3.8124741214318192</v>
       </c>
-    </row>
-    <row r="33" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" ref="AN32:AT32" si="14">AN11-V11</f>
+        <v>0</v>
+      </c>
+      <c r="AO32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AQ32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AR32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AS32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AT32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F33" s="13">
         <v>110</v>
       </c>
@@ -35913,8 +37325,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F33,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-4.7974659680676268</v>
       </c>
-    </row>
-    <row r="34" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN33">
+        <f t="shared" ref="AN33:AT33" si="15">AN12-V12</f>
+        <v>0</v>
+      </c>
+      <c r="AO33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AQ33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AR33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AS33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AT33">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F34" s="13">
         <v>120</v>
       </c>
@@ -35985,8 +37453,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F34,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-5.6647244150695997</v>
       </c>
-    </row>
-    <row r="35" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE34">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN34">
+        <f t="shared" ref="AN34:AT34" si="16">AN13-V13</f>
+        <v>0</v>
+      </c>
+      <c r="AO34">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AQ34">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AR34">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AS34">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AT34">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F35" s="13">
         <v>130</v>
       </c>
@@ -36057,8 +37581,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F35,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-6.3712633617853953</v>
       </c>
-    </row>
-    <row r="36" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN35">
+        <f t="shared" ref="AN35:AT35" si="17">AN14-V14</f>
+        <v>0</v>
+      </c>
+      <c r="AO35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AQ35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AR35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AS35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AT35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F36" s="13">
         <v>140</v>
       </c>
@@ -36129,8 +37709,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F36,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-6.9023897426347958</v>
       </c>
-    </row>
-    <row r="37" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN36">
+        <f t="shared" ref="AN36:AT36" si="18">AN15-V15</f>
+        <v>0</v>
+      </c>
+      <c r="AO36">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AP36">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AQ36">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AR36">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AS36">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AT36">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F37" s="13">
         <v>150</v>
       </c>
@@ -36201,8 +37837,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F37,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-7.2641111709899064</v>
       </c>
-    </row>
-    <row r="38" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN37">
+        <f t="shared" ref="AN37:AT37" si="19">AN16-V16</f>
+        <v>0</v>
+      </c>
+      <c r="AO37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AP37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AQ37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AR37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AS37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AT37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F38" s="13">
         <v>160</v>
       </c>
@@ -36273,8 +37965,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F38,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-7.4751432483637359</v>
       </c>
-    </row>
-    <row r="39" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" ref="AN38:AT38" si="20">AN17-V17</f>
+        <v>0</v>
+      </c>
+      <c r="AO38">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AP38">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AQ38">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AR38">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AS38">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AT38">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F39" s="13">
         <v>170</v>
       </c>
@@ -36345,8 +38093,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F39,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-7.5602846421602976</v>
       </c>
-    </row>
-    <row r="40" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN39">
+        <f t="shared" ref="AN39:AT39" si="21">AN18-V18</f>
+        <v>0</v>
+      </c>
+      <c r="AO39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AP39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AQ39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AR39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AS39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AT39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F40" s="13">
         <v>180</v>
       </c>
@@ -36417,8 +38221,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F40,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-7.5456940949294449</v>
       </c>
-    </row>
-    <row r="41" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH40">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI40">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN40">
+        <f t="shared" ref="AN40:AT40" si="22">AN19-V19</f>
+        <v>0</v>
+      </c>
+      <c r="AO40">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AP40">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AQ40">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AR40">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AS40">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AT40">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F41" s="13">
         <v>190</v>
       </c>
@@ -36489,8 +38349,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F41,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-7.4559444641266737</v>
       </c>
-    </row>
-    <row r="42" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE41">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN41">
+        <f t="shared" ref="AN41:AT41" si="23">AN20-V20</f>
+        <v>0</v>
+      </c>
+      <c r="AO41">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AP41">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AQ41">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AR41">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AS41">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AT41">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F42" s="13">
         <v>200</v>
       </c>
@@ -36561,8 +38477,64 @@
         <f>_xll.acq_options_bjerksund_greeks(Z$31,$F42,$C$5,$C$6,$C$8,$C$9,$C$7,TRUE)</f>
         <v>-7.3124679884983834</v>
       </c>
-    </row>
-    <row r="43" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE42">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH42">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI42">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ42">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN42">
+        <f t="shared" ref="AN42:AT42" si="24">AN21-V21</f>
+        <v>0</v>
+      </c>
+      <c r="AO42">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AP42">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AQ42">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AR42">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AS42">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AT42">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:46" x14ac:dyDescent="0.25">
       <c r="V43" s="46"/>
       <c r="W43" s="46"/>
       <c r="X43" s="46"/>
@@ -36570,8 +38542,64 @@
       <c r="Z43" s="46"/>
       <c r="AA43" s="46"/>
       <c r="AB43" s="46"/>
-    </row>
-    <row r="44" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH43">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN43">
+        <f t="shared" ref="AN43:AT43" si="25">AN22-V22</f>
+        <v>0</v>
+      </c>
+      <c r="AO43">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AP43">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AQ43">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AR43">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AS43">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AT43">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:46" x14ac:dyDescent="0.25">
       <c r="V44" s="46"/>
       <c r="W44" s="46"/>
       <c r="X44" s="46"/>
@@ -36579,8 +38607,64 @@
       <c r="Z44" s="46"/>
       <c r="AA44" s="46"/>
       <c r="AB44" s="46"/>
-    </row>
-    <row r="45" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE44">
+        <f t="shared" ref="AE44:AE45" si="26">AE23-M23</f>
+        <v>0</v>
+      </c>
+      <c r="AF44">
+        <f t="shared" ref="AF44:AF45" si="27">AF23-N23</f>
+        <v>0</v>
+      </c>
+      <c r="AG44">
+        <f t="shared" ref="AG44:AG45" si="28">AG23-O23</f>
+        <v>0</v>
+      </c>
+      <c r="AH44">
+        <f t="shared" ref="AH44:AH45" si="29">AH23-P23</f>
+        <v>0</v>
+      </c>
+      <c r="AI44">
+        <f t="shared" ref="AI44:AI45" si="30">AI23-Q23</f>
+        <v>0</v>
+      </c>
+      <c r="AJ44">
+        <f t="shared" ref="AJ44:AJ45" si="31">AJ23-R23</f>
+        <v>0</v>
+      </c>
+      <c r="AK44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN44">
+        <f t="shared" ref="AN44:AT44" si="32">AN23-V23</f>
+        <v>0</v>
+      </c>
+      <c r="AO44">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AP44">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AQ44">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AR44">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AS44">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AT44">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G45" s="56" t="s">
         <v>165</v>
       </c>
@@ -36603,8 +38687,64 @@
       <c r="Z45" s="56"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
-    </row>
-    <row r="46" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="AE45">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="AF45">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="AG45">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AH45">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AI45">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="AJ45">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="AK45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN45">
+        <f t="shared" ref="AN45:AT45" si="33">AN24-V24</f>
+        <v>0</v>
+      </c>
+      <c r="AO45">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AP45">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AQ45">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AR45">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AS45">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="AT45">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>125</v>
       </c>
@@ -36660,7 +38800,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F47" s="13">
         <v>100</v>
       </c>
@@ -36732,7 +38872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:46" x14ac:dyDescent="0.25">
       <c r="F48" s="13">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
added function to check for a leap year
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966F6409-9B89-4490-9BCC-F8A0CED33039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96848E57-EA90-4D0E-A156-70287A4EC269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="825" windowWidth="24465" windowHeight="12840" tabRatio="900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="705" windowWidth="24465" windowHeight="12840" tabRatio="900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="178">
   <si>
     <t>x</t>
   </si>
@@ -720,6 +720,12 @@
   </si>
   <si>
     <t>acq_isinteger</t>
+  </si>
+  <si>
+    <t>acq_isleap_year</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -13492,35 +13498,36 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:O28"/>
+  <dimension ref="B2:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="L2" t="s">
+      <c r="H2" t="s">
         <v>157</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -13528,39 +13535,39 @@
         <f>_xll.acq_excel_version()</f>
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="G3" t="s">
         <v>153</v>
       </c>
-      <c r="L3" s="5">
+      <c r="H3" s="5">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="N3" s="6" t="str">
-        <f>_xll.acq_tostring(L3)</f>
+      <c r="J3" s="6" t="str">
+        <f>_xll.acq_tostring(H3)</f>
         <v>3.14159265358979</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8029.25470</v>
-      </c>
-      <c r="K4" t="s">
+        <v>1.3.8029.27023</v>
+      </c>
+      <c r="G4" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="48">
+      <c r="H4" s="48">
         <f ca="1">TODAY()</f>
         <v>44555</v>
       </c>
-      <c r="N4" s="49" t="str">
-        <f ca="1">_xll.acq_tostring(L4)</f>
+      <c r="J4" s="49" t="str">
+        <f ca="1">_xll.acq_tostring(H4)</f>
         <v>44555</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -13568,18 +13575,18 @@
         <f>_xll.acq_xllpath()</f>
         <v>D:\Github\ACQ\Distribution\ACQ64.xll</v>
       </c>
-      <c r="K5" t="s">
+      <c r="G5" t="s">
         <v>154</v>
       </c>
-      <c r="L5" s="5" t="b">
+      <c r="H5" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="N5" s="6" t="str">
-        <f>_xll.acq_tostring(L5)</f>
+      <c r="J5" s="6" t="str">
+        <f>_xll.acq_tostring(H5)</f>
         <v>TRUE</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -13587,19 +13594,19 @@
         <f>_xll.acq_exceldna_version()</f>
         <v>1.1.0.3</v>
       </c>
-      <c r="K6" t="s">
+      <c r="G6" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="5" t="e">
+      <c r="H6" s="5" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N6" s="6" t="str">
-        <f>_xll.acq_tostring(L6)</f>
+      <c r="J6" s="6" t="str">
+        <f>_xll.acq_tostring(H6)</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -13607,65 +13614,65 @@
         <f>_xll.acq_dotnet_version()</f>
         <v>4.0.30319.42000</v>
       </c>
-      <c r="K7" t="s">
+      <c r="G7" t="s">
         <v>155</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="N7" s="6" t="str">
-        <f>_xll.acq_tostring(L7)</f>
+      <c r="H7" s="5"/>
+      <c r="J7" s="6" t="str">
+        <f>_xll.acq_tostring(H7)</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K8" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
         <v>111</v>
       </c>
-      <c r="L8" s="5" t="e">
+      <c r="H8" s="5" t="e">
         <f ca="1">DS()</f>
         <v>#NAME?</v>
       </c>
-      <c r="N8" s="6" t="str">
-        <f ca="1">_xll.acq_tostring(L8)</f>
+      <c r="J8" s="6" t="str">
+        <f ca="1">_xll.acq_tostring(H8)</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="K9" t="s">
+      <c r="G9" t="s">
         <v>156</v>
       </c>
-      <c r="L9" s="5" t="e">
+      <c r="H9" s="5" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="N9" s="6" t="str">
-        <f>_xll.acq_tostring(L9)</f>
+      <c r="J9" s="6" t="str">
+        <f>_xll.acq_tostring(H9)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K10" t="s">
+      <c r="G10" t="s">
         <v>159</v>
       </c>
-      <c r="L10" s="5" t="e">
-        <f>LOOKUP(L3,)</f>
+      <c r="H10" s="5" t="e">
+        <f>LOOKUP(H3,)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N10" s="6" t="str">
-        <f>_xll.acq_tostring(L10)</f>
+      <c r="J10" s="6" t="str">
+        <f>_xll.acq_tostring(H10)</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -13673,49 +13680,49 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K13" s="3" t="s">
+    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="L13" t="str">
-        <f ca="1">_xll.acq_join(L3:L10)</f>
+      <c r="H13" t="str">
+        <f ca="1">_xll.acq_join(H3:H10)</f>
         <v>3.14159265358979,44555,True,,,,,</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K14" s="3" t="s">
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="L14" t="str">
-        <f ca="1">_xll.acq_join(N3:N10, "|")</f>
+      <c r="H14" t="str">
+        <f ca="1">_xll.acq_join(J3:J10, "|")</f>
         <v>3.14159265358979|44555|TRUE|||||</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K15" s="3" t="s">
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="L15">
-        <f ca="1">_xll.acq_count_unique(L3:L10)</f>
+      <c r="H15">
+        <f ca="1">_xll.acq_count_unique(H3:H10)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K16" s="3" t="s">
+    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="L16">
-        <f ca="1">_xll.acq_count_unique(L3:L10,FALSE)</f>
+      <c r="H16">
+        <f ca="1">_xll.acq_count_unique(H3:H10,FALSE)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
@@ -13723,7 +13730,7 @@
         <v>20150630</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
@@ -13731,16 +13738,22 @@
         <f>_xll.acq_convert_todate(C18)</f>
         <v>42185</v>
       </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="53" t="s">
+      <c r="G19" s="19"/>
+      <c r="H19" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="53" t="s">
+      <c r="J19" s="19"/>
+      <c r="K19" s="53" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M19" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="N19" s="53" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>149</v>
       </c>
@@ -13748,22 +13761,29 @@
         <f>_xll.acq_nextbusinessday(C19)</f>
         <v>42186</v>
       </c>
-      <c r="K20" s="54">
-        <v>0</v>
-      </c>
-      <c r="L20" s="22" t="b">
-        <f>_xll.acq_isprime(K20)</f>
-        <v>0</v>
-      </c>
-      <c r="N20" s="54">
+      <c r="G20" s="54">
+        <v>0</v>
+      </c>
+      <c r="H20" s="22" t="b">
+        <f>_xll.acq_isprime(G20)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="54">
         <v>1</v>
       </c>
-      <c r="O20" s="22" t="b">
-        <f>_xll.acq_isinteger(N20)</f>
+      <c r="K20" s="22" t="b">
+        <f>_xll.acq_isinteger(J20)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M20" s="33">
+        <v>1992</v>
+      </c>
+      <c r="N20" s="22" t="b">
+        <f>_xll.acq_isleap_year(M20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>150</v>
       </c>
@@ -13771,128 +13791,436 @@
         <f>_xll.acq_adjustbusinessday(C19,-1)</f>
         <v>42185</v>
       </c>
-      <c r="K21" s="54">
+      <c r="G21" s="54">
         <v>1</v>
       </c>
-      <c r="L21" s="22" t="b">
-        <f>_xll.acq_isprime(K21)</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="54">
+      <c r="H21" s="22" t="b">
+        <f>_xll.acq_isprime(G21)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="54">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="O21" s="22" t="b">
-        <f>_xll.acq_isinteger(N21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K22" s="54">
+      <c r="K21" s="22" t="b">
+        <f>_xll.acq_isinteger(J21)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="33">
+        <v>2000</v>
+      </c>
+      <c r="N21" s="22" t="b">
+        <f>_xll.acq_isleap_year(M21)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G22" s="54">
         <v>2</v>
       </c>
-      <c r="L22" s="22" t="b">
-        <f>_xll.acq_isprime(K22)</f>
+      <c r="H22" s="22" t="b">
+        <f>_xll.acq_isprime(G22)</f>
         <v>1</v>
       </c>
-      <c r="N22" s="54" t="str">
+      <c r="J22" s="54" t="str">
         <f>"text"</f>
         <v>text</v>
       </c>
-      <c r="O22" s="22" t="b">
-        <f>_xll.acq_isinteger(N22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K23" s="54">
+      <c r="K22" s="22" t="b">
+        <f>_xll.acq_isinteger(J22)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="33">
+        <v>1900</v>
+      </c>
+      <c r="N22" s="22" t="b">
+        <f>_xll.acq_isleap_year(M22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G23" s="54">
         <v>3</v>
       </c>
-      <c r="L23" s="22" t="b">
-        <f>_xll.acq_isprime(K23)</f>
+      <c r="H23" s="22" t="b">
+        <f>_xll.acq_isprime(G23)</f>
         <v>1</v>
       </c>
-      <c r="N23" s="54" t="str">
+      <c r="J23" s="54" t="str">
         <f>"3.14"</f>
         <v>3.14</v>
       </c>
-      <c r="O23" s="22" t="b">
-        <f>_xll.acq_isinteger(N23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K24" s="54">
+      <c r="K23" s="22" t="b">
+        <f>_xll.acq_isinteger(J23)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="33">
+        <v>1700</v>
+      </c>
+      <c r="N23" s="22" t="b">
+        <f>_xll.acq_isleap_year(M23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G24" s="54">
         <v>4</v>
       </c>
-      <c r="L24" s="22" t="b">
-        <f>_xll.acq_isprime(K24)</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="54" t="str">
+      <c r="H24" s="22" t="b">
+        <f>_xll.acq_isprime(G24)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="54" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="O24" s="22" t="b">
-        <f>_xll.acq_isinteger(N24)</f>
+      <c r="K24" s="22" t="b">
+        <f>_xll.acq_isinteger(J24)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K25" s="54">
+      <c r="M24" s="33">
+        <v>1800</v>
+      </c>
+      <c r="N24" s="22" t="b">
+        <f>_xll.acq_isleap_year(M24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G25" s="54">
         <v>5</v>
       </c>
-      <c r="L25" s="22" t="b">
-        <f>_xll.acq_isprime(K25)</f>
+      <c r="H25" s="22" t="b">
+        <f>_xll.acq_isprime(G25)</f>
         <v>1</v>
       </c>
-      <c r="N25" s="54" t="str">
+      <c r="J25" s="54" t="str">
         <f>"3.00"</f>
         <v>3.00</v>
       </c>
-      <c r="O25" s="22" t="b">
-        <f>_xll.acq_isinteger(N25)</f>
+      <c r="K25" s="22" t="b">
+        <f>_xll.acq_isinteger(J25)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K26" s="54">
+      <c r="M25" s="33">
+        <v>1900</v>
+      </c>
+      <c r="N25" s="22" t="b">
+        <f>_xll.acq_isleap_year(M25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G26" s="54">
         <v>6</v>
       </c>
-      <c r="L26" s="22" t="b">
-        <f>_xll.acq_isprime(K26)</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="54">
+      <c r="H26" s="22" t="b">
+        <f>_xll.acq_isprime(G26)</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="54">
         <v>2</v>
       </c>
-      <c r="O26" s="22" t="b">
-        <f>_xll.acq_isinteger(N26)</f>
+      <c r="K26" s="22" t="b">
+        <f>_xll.acq_isinteger(J26)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K27" s="55">
+      <c r="M26" s="33">
+        <v>2100</v>
+      </c>
+      <c r="N26" s="22" t="b">
+        <f>_xll.acq_isleap_year(M26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G27" s="55">
         <v>7</v>
       </c>
-      <c r="L27" s="24" t="b">
-        <f>_xll.acq_isprime(K27)</f>
+      <c r="H27" s="24" t="b">
+        <f>_xll.acq_isprime(G27)</f>
         <v>1</v>
       </c>
-      <c r="N27" s="55">
+      <c r="J27" s="55">
         <v>8</v>
       </c>
-      <c r="O27" s="24" t="b">
-        <f>_xll.acq_isinteger(N27)</f>
+      <c r="K27" s="24" t="b">
+        <f>_xll.acq_isinteger(J27)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K28" s="55">
+      <c r="M27" s="33">
+        <v>2200</v>
+      </c>
+      <c r="N27" s="22" t="b">
+        <f>_xll.acq_isleap_year(M27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G28" s="55">
         <v>7.2</v>
       </c>
-      <c r="L28" s="24" t="b">
-        <f>_xll.acq_isprime(K28)</f>
+      <c r="H28" s="24" t="b">
+        <f>_xll.acq_isprime(G28)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="33">
+        <v>2300</v>
+      </c>
+      <c r="N28" s="22" t="b">
+        <f>_xll.acq_isleap_year(M28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M29" s="33">
+        <v>2500</v>
+      </c>
+      <c r="N29" s="22" t="b">
+        <f>_xll.acq_isleap_year(M29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M30" s="33">
+        <v>2600</v>
+      </c>
+      <c r="N30" s="22" t="b">
+        <f>_xll.acq_isleap_year(M30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M31" s="33">
+        <v>1600</v>
+      </c>
+      <c r="N31" s="22" t="b">
+        <f>_xll.acq_isleap_year(M31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M32" s="33">
+        <v>2000</v>
+      </c>
+      <c r="N32" s="22" t="b">
+        <f>_xll.acq_isleap_year(M32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M33" s="33">
+        <v>2400</v>
+      </c>
+      <c r="N33" s="22" t="b">
+        <f>_xll.acq_isleap_year(M33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M34" s="33">
+        <v>23.4</v>
+      </c>
+      <c r="N34" s="22" t="e">
+        <f>_xll.acq_isleap_year(M34)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M35" s="33">
+        <v>2000</v>
+      </c>
+      <c r="N35" s="22" t="b">
+        <f>_xll.acq_isleap_year(M35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M36" s="33">
+        <v>2001</v>
+      </c>
+      <c r="N36" s="22" t="b">
+        <f>_xll.acq_isleap_year(M36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M37" s="33">
+        <v>2002</v>
+      </c>
+      <c r="N37" s="22" t="b">
+        <f>_xll.acq_isleap_year(M37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M38" s="33">
+        <v>2003</v>
+      </c>
+      <c r="N38" s="22" t="b">
+        <f>_xll.acq_isleap_year(M38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M39" s="33">
+        <v>2004</v>
+      </c>
+      <c r="N39" s="22" t="b">
+        <f>_xll.acq_isleap_year(M39)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M40" s="33">
+        <v>2005</v>
+      </c>
+      <c r="N40" s="22" t="b">
+        <f>_xll.acq_isleap_year(M40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M41" s="33">
+        <v>2006</v>
+      </c>
+      <c r="N41" s="22" t="b">
+        <f>_xll.acq_isleap_year(M41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M42" s="33">
+        <v>2007</v>
+      </c>
+      <c r="N42" s="22" t="b">
+        <f>_xll.acq_isleap_year(M42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M43" s="33">
+        <v>2008</v>
+      </c>
+      <c r="N43" s="22" t="b">
+        <f>_xll.acq_isleap_year(M43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M44" s="33">
+        <v>2009</v>
+      </c>
+      <c r="N44" s="22" t="b">
+        <f>_xll.acq_isleap_year(M44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="33">
+        <v>2010</v>
+      </c>
+      <c r="N45" s="22" t="b">
+        <f>_xll.acq_isleap_year(M45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M46" s="33">
+        <v>2011</v>
+      </c>
+      <c r="N46" s="22" t="b">
+        <f>_xll.acq_isleap_year(M46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M47" s="33">
+        <v>2012</v>
+      </c>
+      <c r="N47" s="22" t="b">
+        <f>_xll.acq_isleap_year(M47)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M48" s="33">
+        <v>2013</v>
+      </c>
+      <c r="N48" s="22" t="b">
+        <f>_xll.acq_isleap_year(M48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49" s="33">
+        <v>2014</v>
+      </c>
+      <c r="N49" s="22" t="b">
+        <f>_xll.acq_isleap_year(M49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M50" s="33">
+        <v>2015</v>
+      </c>
+      <c r="N50" s="22" t="b">
+        <f>_xll.acq_isleap_year(M50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M51" s="33">
+        <v>2016</v>
+      </c>
+      <c r="N51" s="22" t="b">
+        <f>_xll.acq_isleap_year(M51)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M52" s="33">
+        <v>2017</v>
+      </c>
+      <c r="N52" s="22" t="b">
+        <f>_xll.acq_isleap_year(M52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M53" s="33">
+        <v>2018</v>
+      </c>
+      <c r="N53" s="22" t="b">
+        <f>_xll.acq_isleap_year(M53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M54" s="33">
+        <v>2019</v>
+      </c>
+      <c r="N54" s="22" t="b">
+        <f>_xll.acq_isleap_year(M54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M55" s="33">
+        <v>2020</v>
+      </c>
+      <c r="N55" s="22" t="b">
+        <f>_xll.acq_isleap_year(M55)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M56" s="34">
+        <v>2021</v>
+      </c>
+      <c r="N56" s="24" t="b">
+        <f>_xll.acq_isleap_year(M56)</f>
         <v>0</v>
       </c>
     </row>
@@ -33891,7 +34219,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AT57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added stat utils (like weighted mean )
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96848E57-EA90-4D0E-A156-70287A4EC269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BC0DB-928E-4FF6-A8BA-1D02D9AE1EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="705" windowWidth="24465" windowHeight="12840" tabRatio="900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="705" windowWidth="26475" windowHeight="12885" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -13500,8 +13500,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13509,7 +13509,7 @@
     <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -14008,7 +14008,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G33" s="12"/>
       <c r="M33" s="33">
         <v>2400</v>
       </c>
@@ -14017,7 +14018,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G34" s="12"/>
       <c r="M34" s="33">
         <v>23.4</v>
       </c>
@@ -14026,7 +14028,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G35" s="12"/>
       <c r="M35" s="33">
         <v>2000</v>
       </c>
@@ -14035,7 +14038,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G36" s="12"/>
       <c r="M36" s="33">
         <v>2001</v>
       </c>
@@ -14044,7 +14048,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G37" s="12"/>
       <c r="M37" s="33">
         <v>2002</v>
       </c>
@@ -14053,7 +14058,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G38" s="12"/>
       <c r="M38" s="33">
         <v>2003</v>
       </c>
@@ -14062,7 +14068,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G39" s="12"/>
       <c r="M39" s="33">
         <v>2004</v>
       </c>
@@ -14071,7 +14078,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G40" s="12"/>
       <c r="M40" s="33">
         <v>2005</v>
       </c>
@@ -14080,7 +14088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M41" s="33">
         <v>2006</v>
       </c>
@@ -14089,7 +14097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M42" s="33">
         <v>2007</v>
       </c>
@@ -14098,7 +14106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M43" s="33">
         <v>2008</v>
       </c>
@@ -14107,7 +14115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M44" s="33">
         <v>2009</v>
       </c>
@@ -14116,7 +14124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M45" s="33">
         <v>2010</v>
       </c>
@@ -14125,7 +14133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M46" s="33">
         <v>2011</v>
       </c>
@@ -14134,7 +14142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M47" s="33">
         <v>2012</v>
       </c>
@@ -14143,7 +14151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:14" x14ac:dyDescent="0.25">
       <c r="M48" s="33">
         <v>2013</v>
       </c>
@@ -22538,7 +22546,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AQ43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AH43" sqref="AH43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added function to compute max, min while ignoring non numeric values acq_min/acq_max
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Options.xlsx
+++ b/ACQ.Excel/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BC0DB-928E-4FF6-A8BA-1D02D9AE1EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C52927-8748-480A-8AFF-3BB3B1A12830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="705" windowWidth="26475" windowHeight="12885" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-885" yWindow="1485" windowWidth="24450" windowHeight="12690" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -13553,18 +13553,18 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8029.27023</v>
+        <v>1.3.8032.39391</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="48">
         <f ca="1">TODAY()</f>
-        <v>44555</v>
+        <v>44558</v>
       </c>
       <c r="J4" s="49" t="str">
         <f ca="1">_xll.acq_tostring(H4)</f>
-        <v>44555</v>
+        <v>44558</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -13686,7 +13686,7 @@
       </c>
       <c r="H13" t="str">
         <f ca="1">_xll.acq_join(H3:H10)</f>
-        <v>3.14159265358979,44555,True,,,,,</v>
+        <v>3.14159265358979,44558,True,,,,,</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13695,7 +13695,7 @@
       </c>
       <c r="H14" t="str">
         <f ca="1">_xll.acq_join(J3:J10, "|")</f>
-        <v>3.14159265358979|44555|TRUE|||||</v>
+        <v>3.14159265358979|44558|TRUE|||||</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>